<commit_message>
Finished annotating Amm pos with rescue feats
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48903B1E-FD15-4F89-B8CC-361EEF76DE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32925962-E7AD-4DB6-ADB0-D9B5554B4469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4463" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4553" uniqueCount="357">
   <si>
     <t>Amm</t>
   </si>
@@ -801,9 +801,6 @@
     <t>FT0053</t>
   </si>
   <si>
-    <t>Unpicked peak at 13 minutes</t>
-  </si>
-  <si>
     <t>FT0150</t>
   </si>
   <si>
@@ -966,15 +963,9 @@
     <t>FT1668</t>
   </si>
   <si>
-    <t>Unpicked but could be rescued @9.2 or 10.1</t>
-  </si>
-  <si>
     <t>FT1705</t>
   </si>
   <si>
-    <t>Unpicked but could be rescued @9.0</t>
-  </si>
-  <si>
     <t>FT1750</t>
   </si>
   <si>
@@ -1026,31 +1017,85 @@
     <t>FT2100</t>
   </si>
   <si>
-    <t>Unpicked but could be rescued @9.2</t>
-  </si>
-  <si>
     <t>FT2227</t>
   </si>
   <si>
-    <t>Unpicked but could be rescued @12.1</t>
-  </si>
-  <si>
     <t>FT2276</t>
   </si>
   <si>
     <t>Stans a bit off from samps but prob ok</t>
   </si>
   <si>
-    <t>Unpicked but could be rescued @15.8</t>
-  </si>
-  <si>
     <t>FT2396</t>
   </si>
   <si>
-    <t>Unpicked but could maybe be rescued @2.2</t>
-  </si>
-  <si>
     <t>FT2627</t>
+  </si>
+  <si>
+    <t>FT2807</t>
+  </si>
+  <si>
+    <t>Unpicked</t>
+  </si>
+  <si>
+    <t>FT2849</t>
+  </si>
+  <si>
+    <t>FT2866</t>
+  </si>
+  <si>
+    <t>FT2942</t>
+  </si>
+  <si>
+    <t>FT2943</t>
+  </si>
+  <si>
+    <t>FT3051</t>
+  </si>
+  <si>
+    <t>FT3133</t>
+  </si>
+  <si>
+    <t>Low quality but maybe useable</t>
+  </si>
+  <si>
+    <t>FT3230</t>
+  </si>
+  <si>
+    <t>FT3297</t>
+  </si>
+  <si>
+    <t>Actually seems to be a different peak? One at 8 and one at 10.5</t>
+  </si>
+  <si>
+    <t>FT1688</t>
+  </si>
+  <si>
+    <t>FT1707</t>
+  </si>
+  <si>
+    <t>FT2200</t>
+  </si>
+  <si>
+    <t>FT2228</t>
+  </si>
+  <si>
+    <t>FT2278</t>
+  </si>
+  <si>
+    <t>FT2426</t>
+  </si>
+  <si>
+    <t>FT2792</t>
+  </si>
+  <si>
+    <t>FT2814</t>
+  </si>
+  <si>
+    <t>FT2960</t>
+  </si>
+  <si>
+    <t>FT3015</t>
   </si>
 </sst>
 </file>
@@ -1370,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="G106" sqref="G106"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1434,6 +1479,9 @@
       <c r="G2" t="s">
         <v>3</v>
       </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
       <c r="I2" t="s">
         <v>256</v>
       </c>
@@ -1460,6 +1508,9 @@
       <c r="G3" t="s">
         <v>5</v>
       </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
       <c r="I3" t="s">
         <v>256</v>
       </c>
@@ -1512,8 +1563,8 @@
       <c r="G5" t="s">
         <v>3</v>
       </c>
-      <c r="I5" t="s">
-        <v>258</v>
+      <c r="H5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1539,7 +1590,7 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1565,7 +1616,7 @@
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1591,7 +1642,7 @@
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1617,7 +1668,7 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1643,7 +1694,7 @@
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1668,6 +1719,9 @@
       <c r="G11" t="s">
         <v>3</v>
       </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
       <c r="I11" t="s">
         <v>256</v>
       </c>
@@ -1695,10 +1749,10 @@
         <v>3</v>
       </c>
       <c r="H12" t="s">
+        <v>263</v>
+      </c>
+      <c r="I12" t="s">
         <v>264</v>
-      </c>
-      <c r="I12" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1724,10 +1778,10 @@
         <v>3</v>
       </c>
       <c r="H13" t="s">
+        <v>265</v>
+      </c>
+      <c r="I13" t="s">
         <v>266</v>
-      </c>
-      <c r="I13" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1753,7 +1807,7 @@
         <v>3</v>
       </c>
       <c r="H14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1778,6 +1832,9 @@
       <c r="G15" t="s">
         <v>11</v>
       </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
       <c r="I15" t="s">
         <v>256</v>
       </c>
@@ -1805,10 +1862,10 @@
         <v>11</v>
       </c>
       <c r="H16" t="s">
+        <v>268</v>
+      </c>
+      <c r="I16" t="s">
         <v>269</v>
-      </c>
-      <c r="I16" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1834,7 +1891,7 @@
         <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1859,6 +1916,9 @@
       <c r="G18" t="s">
         <v>3</v>
       </c>
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
       <c r="I18" t="s">
         <v>256</v>
       </c>
@@ -1886,7 +1946,7 @@
         <v>3</v>
       </c>
       <c r="H19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1911,6 +1971,9 @@
       <c r="G20" t="s">
         <v>3</v>
       </c>
+      <c r="H20" t="s">
+        <v>5</v>
+      </c>
       <c r="I20" t="s">
         <v>256</v>
       </c>
@@ -1938,7 +2001,7 @@
         <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1963,6 +2026,9 @@
       <c r="G22" t="s">
         <v>3</v>
       </c>
+      <c r="H22" t="s">
+        <v>5</v>
+      </c>
       <c r="I22" t="s">
         <v>256</v>
       </c>
@@ -1990,10 +2056,10 @@
         <v>3</v>
       </c>
       <c r="H23" t="s">
+        <v>273</v>
+      </c>
+      <c r="I23" t="s">
         <v>274</v>
-      </c>
-      <c r="I23" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -2018,6 +2084,9 @@
       <c r="G24" t="s">
         <v>3</v>
       </c>
+      <c r="H24" t="s">
+        <v>5</v>
+      </c>
       <c r="I24" t="s">
         <v>256</v>
       </c>
@@ -2045,7 +2114,7 @@
         <v>11</v>
       </c>
       <c r="H25" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -2070,6 +2139,9 @@
       <c r="G26" t="s">
         <v>5</v>
       </c>
+      <c r="H26" t="s">
+        <v>5</v>
+      </c>
       <c r="I26" t="s">
         <v>256</v>
       </c>
@@ -2096,6 +2168,9 @@
       <c r="G27" t="s">
         <v>5</v>
       </c>
+      <c r="H27" t="s">
+        <v>5</v>
+      </c>
       <c r="I27" t="s">
         <v>256</v>
       </c>
@@ -2123,10 +2198,10 @@
         <v>11</v>
       </c>
       <c r="H28" t="s">
+        <v>276</v>
+      </c>
+      <c r="I28" t="s">
         <v>277</v>
-      </c>
-      <c r="I28" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -2151,6 +2226,9 @@
       <c r="G29" t="s">
         <v>5</v>
       </c>
+      <c r="H29" t="s">
+        <v>5</v>
+      </c>
       <c r="I29" t="s">
         <v>256</v>
       </c>
@@ -2178,10 +2256,10 @@
         <v>11</v>
       </c>
       <c r="H30" t="s">
+        <v>278</v>
+      </c>
+      <c r="I30" t="s">
         <v>279</v>
-      </c>
-      <c r="I30" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -2206,6 +2284,9 @@
       <c r="G31" t="s">
         <v>11</v>
       </c>
+      <c r="H31" t="s">
+        <v>5</v>
+      </c>
       <c r="I31" t="s">
         <v>256</v>
       </c>
@@ -2232,6 +2313,9 @@
       <c r="G32" t="s">
         <v>11</v>
       </c>
+      <c r="H32" t="s">
+        <v>5</v>
+      </c>
       <c r="I32" t="s">
         <v>256</v>
       </c>
@@ -2258,6 +2342,9 @@
       <c r="G33" t="s">
         <v>11</v>
       </c>
+      <c r="H33" t="s">
+        <v>5</v>
+      </c>
       <c r="I33" t="s">
         <v>256</v>
       </c>
@@ -2285,10 +2372,10 @@
         <v>3</v>
       </c>
       <c r="H34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -2313,8 +2400,11 @@
       <c r="G35" t="s">
         <v>3</v>
       </c>
+      <c r="H35" t="s">
+        <v>5</v>
+      </c>
       <c r="I35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -2339,8 +2429,11 @@
       <c r="G36" t="s">
         <v>3</v>
       </c>
+      <c r="H36" t="s">
+        <v>5</v>
+      </c>
       <c r="I36" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -2366,7 +2459,7 @@
         <v>3</v>
       </c>
       <c r="H37" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -2392,7 +2485,7 @@
         <v>3</v>
       </c>
       <c r="H38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -2418,10 +2511,10 @@
         <v>3</v>
       </c>
       <c r="H39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I39" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -2447,7 +2540,7 @@
         <v>11</v>
       </c>
       <c r="H40" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -2473,10 +2566,10 @@
         <v>3</v>
       </c>
       <c r="H41" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I41" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -2502,7 +2595,7 @@
         <v>3</v>
       </c>
       <c r="H42" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -2528,7 +2621,7 @@
         <v>3</v>
       </c>
       <c r="H43" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -2554,7 +2647,7 @@
         <v>11</v>
       </c>
       <c r="H44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -2579,6 +2672,9 @@
       <c r="G45" t="s">
         <v>11</v>
       </c>
+      <c r="H45" t="s">
+        <v>5</v>
+      </c>
       <c r="I45" t="s">
         <v>256</v>
       </c>
@@ -2606,7 +2702,7 @@
         <v>11</v>
       </c>
       <c r="H46" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -2632,7 +2728,7 @@
         <v>3</v>
       </c>
       <c r="H47" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
@@ -2658,10 +2754,10 @@
         <v>11</v>
       </c>
       <c r="H48" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I48" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -2687,10 +2783,10 @@
         <v>11</v>
       </c>
       <c r="H49" t="s">
+        <v>295</v>
+      </c>
+      <c r="I49" t="s">
         <v>296</v>
-      </c>
-      <c r="I49" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -2716,7 +2812,7 @@
         <v>11</v>
       </c>
       <c r="H50" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -2742,7 +2838,7 @@
         <v>3</v>
       </c>
       <c r="H51" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -2768,10 +2864,10 @@
         <v>11</v>
       </c>
       <c r="H52" t="s">
+        <v>299</v>
+      </c>
+      <c r="I52" t="s">
         <v>300</v>
-      </c>
-      <c r="I52" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -2796,6 +2892,9 @@
       <c r="G53" t="s">
         <v>11</v>
       </c>
+      <c r="H53" t="s">
+        <v>5</v>
+      </c>
       <c r="I53" t="s">
         <v>256</v>
       </c>
@@ -2822,6 +2921,9 @@
       <c r="G54" t="s">
         <v>5</v>
       </c>
+      <c r="H54" t="s">
+        <v>5</v>
+      </c>
       <c r="I54" t="s">
         <v>256</v>
       </c>
@@ -2849,7 +2951,7 @@
         <v>11</v>
       </c>
       <c r="H55" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -2875,7 +2977,7 @@
         <v>3</v>
       </c>
       <c r="H56" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -2901,7 +3003,7 @@
         <v>3</v>
       </c>
       <c r="H57" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -2927,10 +3029,10 @@
         <v>11</v>
       </c>
       <c r="H58" t="s">
+        <v>304</v>
+      </c>
+      <c r="I58" t="s">
         <v>305</v>
-      </c>
-      <c r="I58" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -2956,7 +3058,7 @@
         <v>3</v>
       </c>
       <c r="H59" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
@@ -2981,6 +3083,9 @@
       <c r="G60" t="s">
         <v>3</v>
       </c>
+      <c r="H60" t="s">
+        <v>5</v>
+      </c>
       <c r="I60" t="s">
         <v>256</v>
       </c>
@@ -3007,6 +3112,9 @@
       <c r="G61" t="s">
         <v>3</v>
       </c>
+      <c r="H61" t="s">
+        <v>5</v>
+      </c>
       <c r="I61" t="s">
         <v>256</v>
       </c>
@@ -3034,10 +3142,10 @@
         <v>11</v>
       </c>
       <c r="H62" t="s">
+        <v>307</v>
+      </c>
+      <c r="I62" t="s">
         <v>308</v>
-      </c>
-      <c r="I62" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
@@ -3063,10 +3171,10 @@
         <v>3</v>
       </c>
       <c r="H63" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I63" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -3092,7 +3200,7 @@
         <v>11</v>
       </c>
       <c r="H64" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -3118,7 +3226,7 @@
         <v>3</v>
       </c>
       <c r="H65" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -3143,6 +3251,9 @@
       <c r="G66" t="s">
         <v>11</v>
       </c>
+      <c r="H66" t="s">
+        <v>5</v>
+      </c>
       <c r="I66" t="s">
         <v>256</v>
       </c>
@@ -3169,8 +3280,8 @@
       <c r="G67" t="s">
         <v>5</v>
       </c>
-      <c r="I67" t="s">
-        <v>313</v>
+      <c r="H67" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -3195,6 +3306,9 @@
       <c r="G68" t="s">
         <v>5</v>
       </c>
+      <c r="H68" t="s">
+        <v>5</v>
+      </c>
       <c r="I68" t="s">
         <v>256</v>
       </c>
@@ -3221,6 +3335,9 @@
       <c r="G69" t="s">
         <v>5</v>
       </c>
+      <c r="H69" t="s">
+        <v>5</v>
+      </c>
       <c r="I69" t="s">
         <v>256</v>
       </c>
@@ -3248,7 +3365,7 @@
         <v>11</v>
       </c>
       <c r="H70" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
@@ -3273,8 +3390,8 @@
       <c r="G71" t="s">
         <v>11</v>
       </c>
-      <c r="I71" t="s">
-        <v>315</v>
+      <c r="H71" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
@@ -3299,6 +3416,9 @@
       <c r="G72" t="s">
         <v>11</v>
       </c>
+      <c r="H72" t="s">
+        <v>5</v>
+      </c>
       <c r="I72" t="s">
         <v>256</v>
       </c>
@@ -3326,7 +3446,7 @@
         <v>3</v>
       </c>
       <c r="H73" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -3352,7 +3472,7 @@
         <v>11</v>
       </c>
       <c r="H74" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -3378,7 +3498,7 @@
         <v>11</v>
       </c>
       <c r="H75" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -3404,10 +3524,10 @@
         <v>5</v>
       </c>
       <c r="H76" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I76" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
@@ -3433,10 +3553,10 @@
         <v>5</v>
       </c>
       <c r="H77" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I77" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
@@ -3462,10 +3582,10 @@
         <v>5</v>
       </c>
       <c r="H78" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I78" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -3491,7 +3611,7 @@
         <v>5</v>
       </c>
       <c r="H79" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
@@ -3517,7 +3637,7 @@
         <v>5</v>
       </c>
       <c r="H80" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -3543,7 +3663,7 @@
         <v>3</v>
       </c>
       <c r="H81" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -3568,6 +3688,9 @@
       <c r="G82" t="s">
         <v>3</v>
       </c>
+      <c r="H82" t="s">
+        <v>5</v>
+      </c>
       <c r="I82" t="s">
         <v>256</v>
       </c>
@@ -3595,10 +3718,10 @@
         <v>3</v>
       </c>
       <c r="H83" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I83" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
@@ -3623,8 +3746,11 @@
       <c r="G84" t="s">
         <v>5</v>
       </c>
+      <c r="H84" t="s">
+        <v>5</v>
+      </c>
       <c r="I84" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
@@ -3649,6 +3775,9 @@
       <c r="G85" t="s">
         <v>11</v>
       </c>
+      <c r="H85" t="s">
+        <v>5</v>
+      </c>
       <c r="I85" t="s">
         <v>256</v>
       </c>
@@ -3675,8 +3804,11 @@
       <c r="G86" t="s">
         <v>3</v>
       </c>
+      <c r="H86" t="s">
+        <v>5</v>
+      </c>
       <c r="I86" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
@@ -3701,6 +3833,9 @@
       <c r="G87" t="s">
         <v>3</v>
       </c>
+      <c r="H87" t="s">
+        <v>5</v>
+      </c>
       <c r="I87" t="s">
         <v>256</v>
       </c>
@@ -3728,7 +3863,7 @@
         <v>5</v>
       </c>
       <c r="H88" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
@@ -3754,7 +3889,7 @@
         <v>3</v>
       </c>
       <c r="H89" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
@@ -3779,6 +3914,9 @@
       <c r="G90" t="s">
         <v>3</v>
       </c>
+      <c r="H90" t="s">
+        <v>5</v>
+      </c>
       <c r="I90" t="s">
         <v>256</v>
       </c>
@@ -3806,7 +3944,7 @@
         <v>3</v>
       </c>
       <c r="H91" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
@@ -3832,7 +3970,7 @@
         <v>11</v>
       </c>
       <c r="H92" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
@@ -3857,6 +3995,9 @@
       <c r="G93" t="s">
         <v>3</v>
       </c>
+      <c r="H93" t="s">
+        <v>5</v>
+      </c>
       <c r="I93" t="s">
         <v>256</v>
       </c>
@@ -3884,7 +4025,7 @@
         <v>11</v>
       </c>
       <c r="H94" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
@@ -3909,6 +4050,9 @@
       <c r="G95" t="s">
         <v>3</v>
       </c>
+      <c r="H95" t="s">
+        <v>5</v>
+      </c>
       <c r="I95" t="s">
         <v>256</v>
       </c>
@@ -3935,8 +4079,8 @@
       <c r="G96" t="s">
         <v>3</v>
       </c>
-      <c r="I96" t="s">
-        <v>333</v>
+      <c r="H96" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -3962,7 +4106,7 @@
         <v>3</v>
       </c>
       <c r="H97" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
@@ -3987,8 +4131,8 @@
       <c r="G98" t="s">
         <v>3</v>
       </c>
-      <c r="I98" t="s">
-        <v>335</v>
+      <c r="H98" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
@@ -4014,10 +4158,10 @@
         <v>3</v>
       </c>
       <c r="H99" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="I99" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
@@ -4042,8 +4186,8 @@
       <c r="G100" t="s">
         <v>11</v>
       </c>
-      <c r="I100" t="s">
-        <v>338</v>
+      <c r="H100" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
@@ -4068,6 +4212,9 @@
       <c r="G101" t="s">
         <v>3</v>
       </c>
+      <c r="H101" t="s">
+        <v>5</v>
+      </c>
       <c r="I101" t="s">
         <v>256</v>
       </c>
@@ -4095,7 +4242,7 @@
         <v>3</v>
       </c>
       <c r="H102" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
@@ -4120,8 +4267,8 @@
       <c r="G103" t="s">
         <v>11</v>
       </c>
-      <c r="I103" t="s">
-        <v>340</v>
+      <c r="H103" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
@@ -4146,6 +4293,9 @@
       <c r="G104" t="s">
         <v>5</v>
       </c>
+      <c r="H104" t="s">
+        <v>5</v>
+      </c>
       <c r="I104" t="s">
         <v>256</v>
       </c>
@@ -4172,6 +4322,9 @@
       <c r="G105" t="s">
         <v>3</v>
       </c>
+      <c r="H105" t="s">
+        <v>5</v>
+      </c>
       <c r="I105" t="s">
         <v>256</v>
       </c>
@@ -4198,6 +4351,9 @@
       <c r="G106" t="s">
         <v>3</v>
       </c>
+      <c r="H106" t="s">
+        <v>5</v>
+      </c>
       <c r="I106" t="s">
         <v>256</v>
       </c>
@@ -4224,6 +4380,9 @@
       <c r="G107" t="s">
         <v>11</v>
       </c>
+      <c r="H107" t="s">
+        <v>5</v>
+      </c>
       <c r="I107" t="s">
         <v>256</v>
       </c>
@@ -4250,6 +4409,9 @@
       <c r="G108" t="s">
         <v>11</v>
       </c>
+      <c r="H108" t="s">
+        <v>5</v>
+      </c>
       <c r="I108" t="s">
         <v>256</v>
       </c>
@@ -4276,6 +4438,9 @@
       <c r="G109" t="s">
         <v>11</v>
       </c>
+      <c r="H109" t="s">
+        <v>5</v>
+      </c>
       <c r="I109" t="s">
         <v>256</v>
       </c>
@@ -4303,7 +4468,7 @@
         <v>5</v>
       </c>
       <c r="H110" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
@@ -4328,6 +4493,9 @@
       <c r="G111" t="s">
         <v>3</v>
       </c>
+      <c r="H111" t="s">
+        <v>5</v>
+      </c>
       <c r="I111" t="s">
         <v>256</v>
       </c>
@@ -4354,6 +4522,9 @@
       <c r="G112" t="s">
         <v>3</v>
       </c>
+      <c r="H112" t="s">
+        <v>5</v>
+      </c>
       <c r="I112" t="s">
         <v>256</v>
       </c>
@@ -4380,6 +4551,9 @@
       <c r="G113" t="s">
         <v>3</v>
       </c>
+      <c r="H113" t="s">
+        <v>5</v>
+      </c>
       <c r="I113" t="s">
         <v>256</v>
       </c>
@@ -4406,6 +4580,9 @@
       <c r="G114" t="s">
         <v>11</v>
       </c>
+      <c r="H114" t="s">
+        <v>5</v>
+      </c>
       <c r="I114" t="s">
         <v>256</v>
       </c>
@@ -4432,8 +4609,8 @@
       <c r="G115" t="s">
         <v>11</v>
       </c>
-      <c r="I115" t="s">
-        <v>256</v>
+      <c r="H115" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
@@ -4458,6 +4635,9 @@
       <c r="G116" t="s">
         <v>5</v>
       </c>
+      <c r="H116" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
@@ -4481,6 +4661,12 @@
       <c r="G117" t="s">
         <v>5</v>
       </c>
+      <c r="H117" t="s">
+        <v>5</v>
+      </c>
+      <c r="I117" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
@@ -4504,6 +4690,9 @@
       <c r="G118" t="s">
         <v>5</v>
       </c>
+      <c r="H118" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
@@ -4527,6 +4716,12 @@
       <c r="G119" t="s">
         <v>3</v>
       </c>
+      <c r="H119" t="s">
+        <v>5</v>
+      </c>
+      <c r="I119" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
@@ -4550,6 +4745,9 @@
       <c r="G120" t="s">
         <v>11</v>
       </c>
+      <c r="H120" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
@@ -4573,6 +4771,12 @@
       <c r="G121" t="s">
         <v>11</v>
       </c>
+      <c r="H121" t="s">
+        <v>5</v>
+      </c>
+      <c r="I121" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
@@ -4596,6 +4800,9 @@
       <c r="G122" t="s">
         <v>3</v>
       </c>
+      <c r="H122" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
@@ -4619,6 +4826,12 @@
       <c r="G123" t="s">
         <v>3</v>
       </c>
+      <c r="H123" t="s">
+        <v>5</v>
+      </c>
+      <c r="I123" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
@@ -4642,6 +4855,12 @@
       <c r="G124" t="s">
         <v>11</v>
       </c>
+      <c r="H124" t="s">
+        <v>5</v>
+      </c>
+      <c r="I124" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
@@ -4665,6 +4884,9 @@
       <c r="G125" t="s">
         <v>11</v>
       </c>
+      <c r="H125" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
@@ -4688,6 +4910,9 @@
       <c r="G126" t="s">
         <v>5</v>
       </c>
+      <c r="H126" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
@@ -4711,6 +4936,12 @@
       <c r="G127" t="s">
         <v>3</v>
       </c>
+      <c r="H127" t="s">
+        <v>5</v>
+      </c>
+      <c r="I127" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
@@ -4734,8 +4965,11 @@
       <c r="G128" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H128" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>0</v>
       </c>
@@ -4757,8 +4991,11 @@
       <c r="G129" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H129" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>0</v>
       </c>
@@ -4780,8 +5017,14 @@
       <c r="G130" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H130" t="s">
+        <v>5</v>
+      </c>
+      <c r="I130" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>0</v>
       </c>
@@ -4803,8 +5046,14 @@
       <c r="G131" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H131" t="s">
+        <v>5</v>
+      </c>
+      <c r="I131" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>0</v>
       </c>
@@ -4826,8 +5075,11 @@
       <c r="G132" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H132" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>0</v>
       </c>
@@ -4849,8 +5101,11 @@
       <c r="G133" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H133" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>0</v>
       </c>
@@ -4872,8 +5127,11 @@
       <c r="G134" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H134" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>0</v>
       </c>
@@ -4895,8 +5153,11 @@
       <c r="G135" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>0</v>
       </c>
@@ -4918,8 +5179,11 @@
       <c r="G136" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H136" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>0</v>
       </c>
@@ -4941,8 +5205,14 @@
       <c r="G137" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H137" t="s">
+        <v>342</v>
+      </c>
+      <c r="I137" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>0</v>
       </c>
@@ -4964,8 +5234,11 @@
       <c r="G138" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H138" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>0</v>
       </c>
@@ -4987,8 +5260,11 @@
       <c r="G139" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H139" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>0</v>
       </c>
@@ -5010,8 +5286,11 @@
       <c r="G140" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H140" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>0</v>
       </c>
@@ -5033,8 +5312,11 @@
       <c r="G141" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H141" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>0</v>
       </c>
@@ -5056,8 +5338,11 @@
       <c r="G142" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H142" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>0</v>
       </c>
@@ -5079,8 +5364,14 @@
       <c r="G143" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H143" t="s">
+        <v>345</v>
+      </c>
+      <c r="I143" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>0</v>
       </c>
@@ -5102,8 +5393,11 @@
       <c r="G144" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H144" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>0</v>
       </c>
@@ -5125,8 +5419,11 @@
       <c r="G145" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H145" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>0</v>
       </c>
@@ -5148,8 +5445,11 @@
       <c r="G146" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H146" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>0</v>
       </c>
@@ -5171,8 +5471,11 @@
       <c r="G147" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H147" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>0</v>
       </c>
@@ -5194,8 +5497,11 @@
       <c r="G148" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H148" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>0</v>
       </c>
@@ -5217,8 +5523,11 @@
       <c r="G149" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H149" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>0</v>
       </c>
@@ -5240,8 +5549,11 @@
       <c r="G150" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H150" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>0</v>
       </c>
@@ -5263,8 +5575,11 @@
       <c r="G151" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H151" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>0</v>
       </c>
@@ -5287,7 +5602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>0</v>
       </c>
@@ -5310,7 +5625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>0</v>
       </c>
@@ -5333,7 +5648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>0</v>
       </c>
@@ -5356,7 +5671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>0</v>
       </c>
@@ -5379,7 +5694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>0</v>
       </c>
@@ -5402,7 +5717,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>0</v>
       </c>
@@ -5425,7 +5740,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>0</v>
       </c>
@@ -5448,7 +5763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Finished Amm neg mode annotations (not many good ones, oof)
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32925962-E7AD-4DB6-ADB0-D9B5554B4469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9880DA7C-358B-4B08-B8BE-AA6FF6720434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4553" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4680" uniqueCount="382">
   <si>
     <t>Amm</t>
   </si>
@@ -1096,6 +1096,81 @@
   </si>
   <si>
     <t>FT3015</t>
+  </si>
+  <si>
+    <t>FT0227</t>
+  </si>
+  <si>
+    <t>Peak shifts a lot</t>
+  </si>
+  <si>
+    <t>FT0253</t>
+  </si>
+  <si>
+    <t>FT1201</t>
+  </si>
+  <si>
+    <t>FT1376</t>
+  </si>
+  <si>
+    <t>FT1391</t>
+  </si>
+  <si>
+    <t>FT1397</t>
+  </si>
+  <si>
+    <t>FT1452</t>
+  </si>
+  <si>
+    <t>FT1557</t>
+  </si>
+  <si>
+    <t>FT1616</t>
+  </si>
+  <si>
+    <t>FT1664</t>
+  </si>
+  <si>
+    <t>FT1666</t>
+  </si>
+  <si>
+    <t>FT1732</t>
+  </si>
+  <si>
+    <t>FT1861</t>
+  </si>
+  <si>
+    <t>FT1918</t>
+  </si>
+  <si>
+    <t>FT2039</t>
+  </si>
+  <si>
+    <t>Maybe the gross peak at 9.5, super low quality</t>
+  </si>
+  <si>
+    <t>Peak looks terrible</t>
+  </si>
+  <si>
+    <t>FT2435</t>
+  </si>
+  <si>
+    <t>FT2626</t>
+  </si>
+  <si>
+    <t>Maybe, standards look terrible</t>
+  </si>
+  <si>
+    <t>FT3204</t>
+  </si>
+  <si>
+    <t>Meh peak</t>
+  </si>
+  <si>
+    <t>Looks fine in stans but not present in samps</t>
+  </si>
+  <si>
+    <t>FT3571</t>
   </si>
 </sst>
 </file>
@@ -1415,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="E200" sqref="E200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5397,7 +5472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>0</v>
       </c>
@@ -5423,7 +5498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>0</v>
       </c>
@@ -5449,7 +5524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>0</v>
       </c>
@@ -5475,7 +5550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>0</v>
       </c>
@@ -5501,7 +5576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>0</v>
       </c>
@@ -5527,7 +5602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>0</v>
       </c>
@@ -5553,7 +5628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>0</v>
       </c>
@@ -5579,7 +5654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>0</v>
       </c>
@@ -5601,8 +5676,14 @@
       <c r="G152" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H152" t="s">
+        <v>357</v>
+      </c>
+      <c r="I152" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>0</v>
       </c>
@@ -5624,8 +5705,11 @@
       <c r="G153" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H153" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>0</v>
       </c>
@@ -5647,8 +5731,11 @@
       <c r="G154" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H154" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>0</v>
       </c>
@@ -5670,8 +5757,11 @@
       <c r="G155" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H155" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>0</v>
       </c>
@@ -5693,8 +5783,11 @@
       <c r="G156" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I156" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>0</v>
       </c>
@@ -5716,8 +5809,11 @@
       <c r="G157" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H157" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>0</v>
       </c>
@@ -5739,8 +5835,11 @@
       <c r="G158" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H158" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>0</v>
       </c>
@@ -5762,8 +5861,11 @@
       <c r="G159" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H159" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>0</v>
       </c>
@@ -5785,8 +5887,11 @@
       <c r="G160" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H160" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>0</v>
       </c>
@@ -5808,8 +5913,11 @@
       <c r="G161" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H161" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>0</v>
       </c>
@@ -5831,8 +5939,11 @@
       <c r="G162" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I162" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>0</v>
       </c>
@@ -5854,8 +5965,11 @@
       <c r="G163" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H163" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>0</v>
       </c>
@@ -5877,8 +5991,11 @@
       <c r="G164" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H164" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>0</v>
       </c>
@@ -5900,8 +6017,11 @@
       <c r="G165" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H165" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>0</v>
       </c>
@@ -5923,8 +6043,11 @@
       <c r="G166" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H166" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>0</v>
       </c>
@@ -5946,8 +6069,11 @@
       <c r="G167" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H167" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>0</v>
       </c>
@@ -5969,8 +6095,11 @@
       <c r="G168" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H168" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>0</v>
       </c>
@@ -5992,8 +6121,11 @@
       <c r="G169" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H169" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>0</v>
       </c>
@@ -6015,8 +6147,11 @@
       <c r="G170" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I170" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>0</v>
       </c>
@@ -6038,8 +6173,11 @@
       <c r="G171" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H171" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>0</v>
       </c>
@@ -6061,8 +6199,11 @@
       <c r="G172" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H172" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>0</v>
       </c>
@@ -6084,8 +6225,11 @@
       <c r="G173" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H173" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>0</v>
       </c>
@@ -6107,8 +6251,11 @@
       <c r="G174" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H174" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>0</v>
       </c>
@@ -6130,8 +6277,11 @@
       <c r="G175" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H175" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>0</v>
       </c>
@@ -6153,8 +6303,11 @@
       <c r="G176" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H176" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>0</v>
       </c>
@@ -6176,8 +6329,11 @@
       <c r="G177" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H177" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>0</v>
       </c>
@@ -6199,8 +6355,11 @@
       <c r="G178" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H178" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>0</v>
       </c>
@@ -6222,8 +6381,11 @@
       <c r="G179" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H179" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>0</v>
       </c>
@@ -6245,8 +6407,11 @@
       <c r="G180" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H180" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>0</v>
       </c>
@@ -6268,8 +6433,11 @@
       <c r="G181" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H181" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>0</v>
       </c>
@@ -6291,8 +6459,11 @@
       <c r="G182" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H182" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>0</v>
       </c>
@@ -6314,8 +6485,11 @@
       <c r="G183" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H183" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>0</v>
       </c>
@@ -6337,8 +6511,11 @@
       <c r="G184" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H184" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>0</v>
       </c>
@@ -6360,8 +6537,11 @@
       <c r="G185" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H185" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>0</v>
       </c>
@@ -6383,8 +6563,11 @@
       <c r="G186" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H186" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>0</v>
       </c>
@@ -6406,8 +6589,11 @@
       <c r="G187" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H187" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>0</v>
       </c>
@@ -6429,8 +6615,11 @@
       <c r="G188" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H188" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>0</v>
       </c>
@@ -6452,8 +6641,11 @@
       <c r="G189" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H189" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>0</v>
       </c>
@@ -6475,8 +6667,11 @@
       <c r="G190" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H190" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>0</v>
       </c>
@@ -6498,8 +6693,11 @@
       <c r="G191" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H191" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>0</v>
       </c>
@@ -6521,8 +6719,11 @@
       <c r="G192" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H192" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>0</v>
       </c>
@@ -6544,8 +6745,11 @@
       <c r="G193" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H193" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>0</v>
       </c>
@@ -6567,8 +6771,11 @@
       <c r="G194" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H194" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>0</v>
       </c>
@@ -6590,8 +6797,11 @@
       <c r="G195" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H195" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>0</v>
       </c>
@@ -6613,8 +6823,14 @@
       <c r="G196" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H196" t="s">
+        <v>5</v>
+      </c>
+      <c r="I196" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>0</v>
       </c>
@@ -6636,8 +6852,11 @@
       <c r="G197" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H197" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>0</v>
       </c>
@@ -6659,8 +6878,14 @@
       <c r="G198" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H198" t="s">
+        <v>5</v>
+      </c>
+      <c r="I198" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>0</v>
       </c>
@@ -6682,8 +6907,11 @@
       <c r="G199" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H199" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>0</v>
       </c>
@@ -6705,8 +6933,11 @@
       <c r="G200" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H200" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>0</v>
       </c>
@@ -6728,8 +6959,11 @@
       <c r="G201" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H201" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>0</v>
       </c>
@@ -6751,8 +6985,11 @@
       <c r="G202" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H202" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>0</v>
       </c>
@@ -6774,8 +7011,11 @@
       <c r="G203" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H203" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>0</v>
       </c>
@@ -6797,8 +7037,11 @@
       <c r="G204" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H204" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>0</v>
       </c>
@@ -6820,8 +7063,11 @@
       <c r="G205" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H205" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>0</v>
       </c>
@@ -6843,8 +7089,11 @@
       <c r="G206" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H206" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>0</v>
       </c>
@@ -6866,8 +7115,11 @@
       <c r="G207" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H207" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>0</v>
       </c>
@@ -6889,8 +7141,11 @@
       <c r="G208" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H208" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>0</v>
       </c>
@@ -6912,8 +7167,11 @@
       <c r="G209" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H209" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>0</v>
       </c>
@@ -6935,8 +7193,14 @@
       <c r="G210" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H210" t="s">
+        <v>375</v>
+      </c>
+      <c r="I210" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>0</v>
       </c>
@@ -6958,8 +7222,11 @@
       <c r="G211" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H211" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>0</v>
       </c>
@@ -6981,8 +7248,11 @@
       <c r="G212" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H212" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>0</v>
       </c>
@@ -7004,8 +7274,11 @@
       <c r="G213" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H213" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>0</v>
       </c>
@@ -7027,8 +7300,11 @@
       <c r="G214" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H214" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>0</v>
       </c>
@@ -7050,8 +7326,14 @@
       <c r="G215" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H215" t="s">
+        <v>376</v>
+      </c>
+      <c r="I215" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>0</v>
       </c>
@@ -7073,8 +7355,11 @@
       <c r="G216" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H216" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>0</v>
       </c>
@@ -7096,8 +7381,11 @@
       <c r="G217" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H217" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>0</v>
       </c>
@@ -7119,8 +7407,11 @@
       <c r="G218" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H218" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>0</v>
       </c>
@@ -7142,8 +7433,11 @@
       <c r="G219" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H219" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>0</v>
       </c>
@@ -7165,8 +7459,11 @@
       <c r="G220" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H220" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>0</v>
       </c>
@@ -7188,8 +7485,11 @@
       <c r="G221" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H221" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>0</v>
       </c>
@@ -7211,8 +7511,11 @@
       <c r="G222" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H222" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>0</v>
       </c>
@@ -7234,8 +7537,11 @@
       <c r="G223" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H223" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>0</v>
       </c>
@@ -7257,8 +7563,11 @@
       <c r="G224" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H224" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>0</v>
       </c>
@@ -7280,8 +7589,11 @@
       <c r="G225" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H225" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>0</v>
       </c>
@@ -7303,8 +7615,11 @@
       <c r="G226" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H226" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>0</v>
       </c>
@@ -7326,8 +7641,11 @@
       <c r="G227" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H227" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>0</v>
       </c>
@@ -7349,8 +7667,14 @@
       <c r="G228" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H228" t="s">
+        <v>378</v>
+      </c>
+      <c r="I228" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>0</v>
       </c>
@@ -7372,8 +7696,14 @@
       <c r="G229" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H229" t="s">
+        <v>5</v>
+      </c>
+      <c r="I229" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>0</v>
       </c>
@@ -7395,8 +7725,11 @@
       <c r="G230" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H230" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>0</v>
       </c>
@@ -7418,8 +7751,11 @@
       <c r="G231" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H231" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>0</v>
       </c>
@@ -7441,8 +7777,11 @@
       <c r="G232" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H232" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>0</v>
       </c>
@@ -7464,8 +7803,11 @@
       <c r="G233" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H233" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>0</v>
       </c>
@@ -7487,8 +7829,11 @@
       <c r="G234" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H234" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>0</v>
       </c>
@@ -7510,8 +7855,11 @@
       <c r="G235" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H235" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>0</v>
       </c>
@@ -7533,8 +7881,11 @@
       <c r="G236" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H236" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>0</v>
       </c>
@@ -7556,8 +7907,11 @@
       <c r="G237" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H237" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>0</v>
       </c>
@@ -7579,8 +7933,11 @@
       <c r="G238" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H238" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>0</v>
       </c>
@@ -7602,8 +7959,11 @@
       <c r="G239" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H239" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>0</v>
       </c>
@@ -7625,8 +7985,11 @@
       <c r="G240" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H240" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>0</v>
       </c>
@@ -7648,8 +8011,11 @@
       <c r="G241" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H241" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>0</v>
       </c>
@@ -7671,8 +8037,11 @@
       <c r="G242" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H242" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>0</v>
       </c>
@@ -7694,8 +8063,11 @@
       <c r="G243" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H243" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>0</v>
       </c>
@@ -7717,8 +8089,11 @@
       <c r="G244" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H244" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>0</v>
       </c>
@@ -7740,8 +8115,11 @@
       <c r="G245" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H245" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>0</v>
       </c>
@@ -7763,8 +8141,11 @@
       <c r="G246" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H246" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>0</v>
       </c>
@@ -7786,8 +8167,11 @@
       <c r="G247" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H247" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>0</v>
       </c>
@@ -7809,8 +8193,11 @@
       <c r="G248" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H248" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>0</v>
       </c>
@@ -7832,8 +8219,11 @@
       <c r="G249" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H249" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>0</v>
       </c>
@@ -7855,8 +8245,11 @@
       <c r="G250" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H250" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>0</v>
       </c>
@@ -7878,8 +8271,11 @@
       <c r="G251" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H251" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>0</v>
       </c>
@@ -7901,8 +8297,11 @@
       <c r="G252" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H252" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>0</v>
       </c>
@@ -7924,8 +8323,11 @@
       <c r="G253" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H253" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>0</v>
       </c>
@@ -7947,8 +8349,11 @@
       <c r="G254" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H254" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>0</v>
       </c>
@@ -7970,8 +8375,11 @@
       <c r="G255" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H255" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>0</v>
       </c>
@@ -7993,8 +8401,11 @@
       <c r="G256" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H256" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>0</v>
       </c>
@@ -8016,8 +8427,11 @@
       <c r="G257" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H257" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>0</v>
       </c>
@@ -8039,8 +8453,11 @@
       <c r="G258" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H258" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>0</v>
       </c>
@@ -8062,8 +8479,11 @@
       <c r="G259" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H259" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>0</v>
       </c>
@@ -8085,8 +8505,11 @@
       <c r="G260" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H260" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>0</v>
       </c>
@@ -8108,8 +8531,11 @@
       <c r="G261" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H261" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>0</v>
       </c>
@@ -8131,8 +8557,11 @@
       <c r="G262" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H262" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>0</v>
       </c>
@@ -8154,8 +8583,11 @@
       <c r="G263" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H263" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>0</v>
       </c>
@@ -8177,8 +8609,11 @@
       <c r="G264" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H264" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>0</v>
       </c>
@@ -8200,8 +8635,11 @@
       <c r="G265" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H265" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>0</v>
       </c>
@@ -8223,8 +8661,11 @@
       <c r="G266" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H266" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>0</v>
       </c>
@@ -8246,8 +8687,11 @@
       <c r="G267" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H267" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>0</v>
       </c>
@@ -8269,8 +8713,11 @@
       <c r="G268" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H268" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>0</v>
       </c>
@@ -8292,8 +8739,11 @@
       <c r="G269" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H269" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>0</v>
       </c>
@@ -8315,8 +8765,11 @@
       <c r="G270" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H270" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>0</v>
       </c>
@@ -8338,8 +8791,11 @@
       <c r="G271" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H271" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>244</v>
       </c>

</xml_diff>

<commit_message>
Annotated Nit pos, needs rescuing still
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9880DA7C-358B-4B08-B8BE-AA6FF6720434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0131ED56-A00C-49F8-ABFC-59816B7ECD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4680" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4853" uniqueCount="469">
   <si>
     <t>Amm</t>
   </si>
@@ -1171,6 +1171,267 @@
   </si>
   <si>
     <t>FT3571</t>
+  </si>
+  <si>
+    <t>FT0042</t>
+  </si>
+  <si>
+    <t>Barely present</t>
+  </si>
+  <si>
+    <t>FT0251</t>
+  </si>
+  <si>
+    <t>Multiple peaks in stans?</t>
+  </si>
+  <si>
+    <t>FT0255</t>
+  </si>
+  <si>
+    <t>FT0551</t>
+  </si>
+  <si>
+    <t>FT0549</t>
+  </si>
+  <si>
+    <t>FT0550</t>
+  </si>
+  <si>
+    <t>Spread out across FIVE minutes, ugh</t>
+  </si>
+  <si>
+    <t>FT1106/FT1107</t>
+  </si>
+  <si>
+    <t>Two features need combining</t>
+  </si>
+  <si>
+    <t>FT1242</t>
+  </si>
+  <si>
+    <t>Rescue</t>
+  </si>
+  <si>
+    <t>FT1419</t>
+  </si>
+  <si>
+    <t>Rescue (optional)</t>
+  </si>
+  <si>
+    <t>FT1478</t>
+  </si>
+  <si>
+    <t>FT1558</t>
+  </si>
+  <si>
+    <t>FT1575</t>
+  </si>
+  <si>
+    <t>Too messy to separate</t>
+  </si>
+  <si>
+    <t>Not great</t>
+  </si>
+  <si>
+    <t>FT1788</t>
+  </si>
+  <si>
+    <t>Check on grouping</t>
+  </si>
+  <si>
+    <t>FT1815</t>
+  </si>
+  <si>
+    <t>Maybe FT1904?</t>
+  </si>
+  <si>
+    <t>FT1943</t>
+  </si>
+  <si>
+    <t>FT1947</t>
+  </si>
+  <si>
+    <t>FT1958</t>
+  </si>
+  <si>
+    <t>FT1955</t>
+  </si>
+  <si>
+    <t>FT1972</t>
+  </si>
+  <si>
+    <t>FT1992</t>
+  </si>
+  <si>
+    <t>FT2010</t>
+  </si>
+  <si>
+    <t>FT2024</t>
+  </si>
+  <si>
+    <t>FT2023</t>
+  </si>
+  <si>
+    <t>FT2034</t>
+  </si>
+  <si>
+    <t>FT2036</t>
+  </si>
+  <si>
+    <t>FT2060</t>
+  </si>
+  <si>
+    <t>FT2059</t>
+  </si>
+  <si>
+    <t>FT2092</t>
+  </si>
+  <si>
+    <t>FT2273</t>
+  </si>
+  <si>
+    <t>FT2310</t>
+  </si>
+  <si>
+    <t>FT2363</t>
+  </si>
+  <si>
+    <t>Ugh, could be rescued?</t>
+  </si>
+  <si>
+    <t>FT2400</t>
+  </si>
+  <si>
+    <t>FT2412</t>
+  </si>
+  <si>
+    <t>FT2419</t>
+  </si>
+  <si>
+    <t>FT2482</t>
+  </si>
+  <si>
+    <t>Rescue?</t>
+  </si>
+  <si>
+    <t>FT2521</t>
+  </si>
+  <si>
+    <t>FT2526</t>
+  </si>
+  <si>
+    <t>FT2582</t>
+  </si>
+  <si>
+    <t>FT2676</t>
+  </si>
+  <si>
+    <t>FT2683</t>
+  </si>
+  <si>
+    <t>FT2700</t>
+  </si>
+  <si>
+    <t>Maybe? Not in mix but firs of 3 peaks</t>
+  </si>
+  <si>
+    <t>FT2708</t>
+  </si>
+  <si>
+    <t>FT2707</t>
+  </si>
+  <si>
+    <t>FT2855</t>
+  </si>
+  <si>
+    <t>FT3052</t>
+  </si>
+  <si>
+    <t>FT3053</t>
+  </si>
+  <si>
+    <t>FT3062</t>
+  </si>
+  <si>
+    <t>FT3102</t>
+  </si>
+  <si>
+    <t>FT3106</t>
+  </si>
+  <si>
+    <t>Not aligned with peak in stans</t>
+  </si>
+  <si>
+    <t>FT3175</t>
+  </si>
+  <si>
+    <t>FT3222</t>
+  </si>
+  <si>
+    <t>FT3223</t>
+  </si>
+  <si>
+    <t>FT3309</t>
+  </si>
+  <si>
+    <t>Check on grouping (do this first)</t>
+  </si>
+  <si>
+    <t>Could be worth rescuing</t>
+  </si>
+  <si>
+    <t>FT3542</t>
+  </si>
+  <si>
+    <t>FT3949</t>
+  </si>
+  <si>
+    <t>FT4286</t>
+  </si>
+  <si>
+    <t>FT4301</t>
+  </si>
+  <si>
+    <t>FT4306</t>
+  </si>
+  <si>
+    <t>FT4372</t>
+  </si>
+  <si>
+    <t>FT4492</t>
+  </si>
+  <si>
+    <t>FT4630</t>
+  </si>
+  <si>
+    <t>FT4631</t>
+  </si>
+  <si>
+    <t>FT4660</t>
+  </si>
+  <si>
+    <t>FT4825</t>
+  </si>
+  <si>
+    <t>FT4868</t>
+  </si>
+  <si>
+    <t>FT4904</t>
+  </si>
+  <si>
+    <t>FT5110</t>
+  </si>
+  <si>
+    <t>FT5371</t>
+  </si>
+  <si>
+    <t>FT5478</t>
+  </si>
+  <si>
+    <t>Couldn't check on chrom bc too early eluting</t>
+  </si>
+  <si>
+    <t>FT5606</t>
   </si>
 </sst>
 </file>
@@ -1490,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="E200" sqref="E200"/>
+    <sheetView tabSelected="1" topLeftCell="A395" workbookViewId="0">
+      <selection activeCell="D404" sqref="D404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8817,8 +9078,11 @@
       <c r="G272" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H272" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>244</v>
       </c>
@@ -8840,8 +9104,11 @@
       <c r="G273" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H273" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>244</v>
       </c>
@@ -8863,8 +9130,14 @@
       <c r="G274" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H274" t="s">
+        <v>382</v>
+      </c>
+      <c r="I274" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>244</v>
       </c>
@@ -8886,8 +9159,11 @@
       <c r="G275" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H275" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>244</v>
       </c>
@@ -8909,8 +9185,14 @@
       <c r="G276" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H276" t="s">
+        <v>384</v>
+      </c>
+      <c r="I276" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>244</v>
       </c>
@@ -8932,8 +9214,11 @@
       <c r="G277" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H277" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>244</v>
       </c>
@@ -8955,8 +9240,11 @@
       <c r="G278" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H278" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>244</v>
       </c>
@@ -8978,8 +9266,11 @@
       <c r="G279" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H279" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>244</v>
       </c>
@@ -9001,8 +9292,11 @@
       <c r="G280" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H280" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>244</v>
       </c>
@@ -9024,8 +9318,11 @@
       <c r="G281" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H281" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>244</v>
       </c>
@@ -9047,8 +9344,11 @@
       <c r="G282" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H282" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>244</v>
       </c>
@@ -9070,8 +9370,14 @@
       <c r="G283" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H283" t="s">
+        <v>5</v>
+      </c>
+      <c r="I283" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>244</v>
       </c>
@@ -9093,8 +9399,14 @@
       <c r="G284" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H284" t="s">
+        <v>391</v>
+      </c>
+      <c r="I284" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>244</v>
       </c>
@@ -9116,8 +9428,11 @@
       <c r="G285" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H285" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>244</v>
       </c>
@@ -9139,8 +9454,11 @@
       <c r="G286" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H286" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>244</v>
       </c>
@@ -9162,8 +9480,11 @@
       <c r="G287" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I287" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>244</v>
       </c>
@@ -9185,8 +9506,11 @@
       <c r="G288" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H288" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>244</v>
       </c>
@@ -9208,8 +9532,11 @@
       <c r="G289" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H289" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>244</v>
       </c>
@@ -9231,8 +9558,11 @@
       <c r="G290" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I290" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="291" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>244</v>
       </c>
@@ -9254,8 +9584,11 @@
       <c r="G291" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H291" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>244</v>
       </c>
@@ -9277,8 +9610,11 @@
       <c r="G292" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H292" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>244</v>
       </c>
@@ -9300,8 +9636,14 @@
       <c r="G293" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H293" t="s">
+        <v>398</v>
+      </c>
+      <c r="I293" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>244</v>
       </c>
@@ -9323,8 +9665,14 @@
       <c r="G294" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H294" t="s">
+        <v>398</v>
+      </c>
+      <c r="I294" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>244</v>
       </c>
@@ -9346,8 +9694,11 @@
       <c r="G295" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H295" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>244</v>
       </c>
@@ -9369,8 +9720,11 @@
       <c r="G296" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H296" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>244</v>
       </c>
@@ -9392,8 +9746,11 @@
       <c r="G297" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H297" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="298" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>244</v>
       </c>
@@ -9415,8 +9772,14 @@
       <c r="G298" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H298" t="s">
+        <v>5</v>
+      </c>
+      <c r="I298" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="299" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>244</v>
       </c>
@@ -9438,8 +9801,11 @@
       <c r="G299" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H299" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="300" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>244</v>
       </c>
@@ -9461,8 +9827,14 @@
       <c r="G300" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H300" t="s">
+        <v>402</v>
+      </c>
+      <c r="I300" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>244</v>
       </c>
@@ -9484,8 +9856,11 @@
       <c r="G301" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H301" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>244</v>
       </c>
@@ -9507,8 +9882,11 @@
       <c r="G302" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H302" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="303" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>244</v>
       </c>
@@ -9530,8 +9908,11 @@
       <c r="G303" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H303" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>244</v>
       </c>
@@ -9553,8 +9934,11 @@
       <c r="G304" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H304" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="305" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>244</v>
       </c>
@@ -9576,8 +9960,14 @@
       <c r="G305" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H305" t="s">
+        <v>5</v>
+      </c>
+      <c r="I305" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="306" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>244</v>
       </c>
@@ -9599,8 +9989,11 @@
       <c r="G306" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H306" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="307" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>244</v>
       </c>
@@ -9622,8 +10015,11 @@
       <c r="G307" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H307" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="308" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>244</v>
       </c>
@@ -9645,8 +10041,11 @@
       <c r="G308" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I308" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="309" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>244</v>
       </c>
@@ -9668,8 +10067,14 @@
       <c r="G309" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H309" t="s">
+        <v>408</v>
+      </c>
+      <c r="I309" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="310" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>244</v>
       </c>
@@ -9691,8 +10096,11 @@
       <c r="G310" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H310" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="311" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>244</v>
       </c>
@@ -9714,8 +10122,14 @@
       <c r="G311" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H311" t="s">
+        <v>410</v>
+      </c>
+      <c r="I311" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="312" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>244</v>
       </c>
@@ -9737,8 +10151,11 @@
       <c r="G312" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I312" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="313" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>244</v>
       </c>
@@ -9760,8 +10177,14 @@
       <c r="G313" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H313" t="s">
+        <v>411</v>
+      </c>
+      <c r="I313" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="314" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>244</v>
       </c>
@@ -9783,8 +10206,11 @@
       <c r="G314" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H314" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="315" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>244</v>
       </c>
@@ -9806,8 +10232,11 @@
       <c r="G315" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="316" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H315" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="316" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>244</v>
       </c>
@@ -9829,8 +10258,11 @@
       <c r="G316" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="317" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H316" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="317" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>244</v>
       </c>
@@ -9852,8 +10284,11 @@
       <c r="G317" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="318" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H317" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="318" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>244</v>
       </c>
@@ -9875,8 +10310,11 @@
       <c r="G318" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="319" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H318" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="319" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>244</v>
       </c>
@@ -9898,8 +10336,11 @@
       <c r="G319" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="320" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H319" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="320" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>244</v>
       </c>
@@ -9921,8 +10362,11 @@
       <c r="G320" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="321" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H320" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="321" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>244</v>
       </c>
@@ -9944,8 +10388,11 @@
       <c r="G321" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="322" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H321" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="322" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>244</v>
       </c>
@@ -9967,8 +10414,14 @@
       <c r="G322" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="323" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H322" t="s">
+        <v>419</v>
+      </c>
+      <c r="I322" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="323" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>244</v>
       </c>
@@ -9990,8 +10443,11 @@
       <c r="G323" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="324" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H323" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="324" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>244</v>
       </c>
@@ -10013,8 +10469,11 @@
       <c r="G324" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H324" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="325" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>244</v>
       </c>
@@ -10036,8 +10495,11 @@
       <c r="G325" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="326" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H325" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="326" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>244</v>
       </c>
@@ -10059,8 +10521,11 @@
       <c r="G326" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="327" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H326" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="327" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>244</v>
       </c>
@@ -10082,8 +10547,11 @@
       <c r="G327" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="328" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H327" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="328" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>244</v>
       </c>
@@ -10105,8 +10573,14 @@
       <c r="G328" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="329" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H328" t="s">
+        <v>5</v>
+      </c>
+      <c r="I328" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="329" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>244</v>
       </c>
@@ -10128,8 +10602,11 @@
       <c r="G329" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="330" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H329" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="330" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>244</v>
       </c>
@@ -10151,8 +10628,11 @@
       <c r="G330" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="331" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I330" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="331" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>244</v>
       </c>
@@ -10174,8 +10654,11 @@
       <c r="G331" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="332" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H331" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="332" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>244</v>
       </c>
@@ -10197,8 +10680,14 @@
       <c r="G332" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="333" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H332" t="s">
+        <v>425</v>
+      </c>
+      <c r="I332" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="333" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>244</v>
       </c>
@@ -10220,8 +10709,14 @@
       <c r="G333" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="334" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H333" t="s">
+        <v>425</v>
+      </c>
+      <c r="I333" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="334" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>244</v>
       </c>
@@ -10243,8 +10738,11 @@
       <c r="G334" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="335" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H334" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="335" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>244</v>
       </c>
@@ -10266,8 +10764,14 @@
       <c r="G335" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="336" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H335" t="s">
+        <v>427</v>
+      </c>
+      <c r="I335" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="336" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>244</v>
       </c>
@@ -10289,8 +10793,11 @@
       <c r="G336" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H336" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="337" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>244</v>
       </c>
@@ -10312,8 +10819,11 @@
       <c r="G337" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I337" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="338" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>244</v>
       </c>
@@ -10335,8 +10845,11 @@
       <c r="G338" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H338" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="339" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>244</v>
       </c>
@@ -10358,8 +10871,11 @@
       <c r="G339" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H339" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="340" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>244</v>
       </c>
@@ -10381,8 +10897,11 @@
       <c r="G340" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H340" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="341" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>244</v>
       </c>
@@ -10404,8 +10923,11 @@
       <c r="G341" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H341" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="342" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>244</v>
       </c>
@@ -10427,8 +10949,11 @@
       <c r="G342" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H342" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="343" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>244</v>
       </c>
@@ -10450,8 +10975,11 @@
       <c r="G343" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H343" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="344" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>244</v>
       </c>
@@ -10473,8 +11001,11 @@
       <c r="G344" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H344" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="345" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>244</v>
       </c>
@@ -10496,8 +11027,11 @@
       <c r="G345" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="346" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H345" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="346" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>244</v>
       </c>
@@ -10519,8 +11053,14 @@
       <c r="G346" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H346" t="s">
+        <v>434</v>
+      </c>
+      <c r="I346" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="347" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>244</v>
       </c>
@@ -10542,8 +11082,11 @@
       <c r="G347" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="348" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H347" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="348" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>244</v>
       </c>
@@ -10565,8 +11108,11 @@
       <c r="G348" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="349" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H348" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="349" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>244</v>
       </c>
@@ -10588,8 +11134,11 @@
       <c r="G349" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="350" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I349" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="350" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>244</v>
       </c>
@@ -10611,8 +11160,11 @@
       <c r="G350" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H350" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="351" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>244</v>
       </c>
@@ -10634,8 +11186,11 @@
       <c r="G351" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H351" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="352" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>244</v>
       </c>
@@ -10657,8 +11212,11 @@
       <c r="G352" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="353" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H352" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="353" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>244</v>
       </c>
@@ -10680,8 +11238,14 @@
       <c r="G353" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="354" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H353" t="s">
+        <v>438</v>
+      </c>
+      <c r="I353" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="354" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>244</v>
       </c>
@@ -10703,8 +11267,11 @@
       <c r="G354" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="355" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H354" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="355" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>244</v>
       </c>
@@ -10726,8 +11293,11 @@
       <c r="G355" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="356" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H355" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="356" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>244</v>
       </c>
@@ -10749,8 +11319,11 @@
       <c r="G356" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="357" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I356" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="357" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>244</v>
       </c>
@@ -10772,8 +11345,11 @@
       <c r="G357" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="358" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H357" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="358" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>244</v>
       </c>
@@ -10795,8 +11371,11 @@
       <c r="G358" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="359" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H358" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="359" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>244</v>
       </c>
@@ -10818,8 +11397,11 @@
       <c r="G359" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="360" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H359" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="360" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>244</v>
       </c>
@@ -10841,8 +11423,11 @@
       <c r="G360" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="361" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H360" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="361" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>244</v>
       </c>
@@ -10864,8 +11449,11 @@
       <c r="G361" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="362" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H361" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="362" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>244</v>
       </c>
@@ -10887,8 +11475,11 @@
       <c r="G362" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="363" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H362" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="363" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>244</v>
       </c>
@@ -10910,8 +11501,11 @@
       <c r="G363" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="364" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H363" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="364" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>244</v>
       </c>
@@ -10933,8 +11527,11 @@
       <c r="G364" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="365" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H364" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="365" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>244</v>
       </c>
@@ -10956,8 +11553,14 @@
       <c r="G365" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="366" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H365" t="s">
+        <v>5</v>
+      </c>
+      <c r="I365" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="366" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>244</v>
       </c>
@@ -10979,8 +11582,14 @@
       <c r="G366" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="367" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H366" t="s">
+        <v>445</v>
+      </c>
+      <c r="I366" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="367" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>244</v>
       </c>
@@ -11002,8 +11611,11 @@
       <c r="G367" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="368" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H367" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="368" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>244</v>
       </c>
@@ -11025,8 +11637,11 @@
       <c r="G368" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H368" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="369" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>244</v>
       </c>
@@ -11048,8 +11663,14 @@
       <c r="G369" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="370" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H369" t="s">
+        <v>448</v>
+      </c>
+      <c r="I369" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="370" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>244</v>
       </c>
@@ -11071,8 +11692,11 @@
       <c r="G370" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="371" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I370" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="371" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>244</v>
       </c>
@@ -11094,8 +11718,11 @@
       <c r="G371" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="372" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I371" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="372" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>244</v>
       </c>
@@ -11117,8 +11744,11 @@
       <c r="G372" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="373" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H372" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="373" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>244</v>
       </c>
@@ -11140,8 +11770,11 @@
       <c r="G373" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="374" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H373" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="374" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>244</v>
       </c>
@@ -11163,8 +11796,11 @@
       <c r="G374" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="375" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H374" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="375" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>244</v>
       </c>
@@ -11186,8 +11822,11 @@
       <c r="G375" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="376" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H375" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="376" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>244</v>
       </c>
@@ -11209,8 +11848,11 @@
       <c r="G376" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="377" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H376" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="377" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>244</v>
       </c>
@@ -11232,8 +11874,11 @@
       <c r="G377" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="378" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H377" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="378" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>244</v>
       </c>
@@ -11255,8 +11900,11 @@
       <c r="G378" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="379" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H378" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="379" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>244</v>
       </c>
@@ -11278,8 +11926,11 @@
       <c r="G379" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="380" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H379" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="380" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>244</v>
       </c>
@@ -11301,8 +11952,11 @@
       <c r="G380" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="381" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H380" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="381" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>244</v>
       </c>
@@ -11324,8 +11978,11 @@
       <c r="G381" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="382" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H381" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="382" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>244</v>
       </c>
@@ -11347,8 +12004,11 @@
       <c r="G382" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="383" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H382" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="383" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>244</v>
       </c>
@@ -11370,8 +12030,11 @@
       <c r="G383" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="384" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H383" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="384" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>244</v>
       </c>
@@ -11393,8 +12056,11 @@
       <c r="G384" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="385" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H384" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="385" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>244</v>
       </c>
@@ -11416,8 +12082,11 @@
       <c r="G385" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="386" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H385" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="386" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>244</v>
       </c>
@@ -11439,8 +12108,11 @@
       <c r="G386" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="387" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H386" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="387" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>244</v>
       </c>
@@ -11462,8 +12134,11 @@
       <c r="G387" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="388" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H387" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="388" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>244</v>
       </c>
@@ -11485,8 +12160,11 @@
       <c r="G388" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="389" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H388" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="389" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>244</v>
       </c>
@@ -11508,8 +12186,11 @@
       <c r="G389" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="390" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H389" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="390" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>244</v>
       </c>
@@ -11531,8 +12212,11 @@
       <c r="G390" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="391" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H390" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="391" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>244</v>
       </c>
@@ -11554,8 +12238,11 @@
       <c r="G391" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="392" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I391" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="392" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>244</v>
       </c>
@@ -11577,8 +12264,11 @@
       <c r="G392" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="393" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H392" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="393" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>244</v>
       </c>
@@ -11600,8 +12290,11 @@
       <c r="G393" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="394" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H393" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="394" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>244</v>
       </c>
@@ -11623,8 +12316,11 @@
       <c r="G394" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="395" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H394" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="395" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>244</v>
       </c>
@@ -11646,8 +12342,11 @@
       <c r="G395" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="396" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H395" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="396" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>244</v>
       </c>
@@ -11669,8 +12368,11 @@
       <c r="G396" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="397" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H396" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="397" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>244</v>
       </c>
@@ -11692,8 +12394,11 @@
       <c r="G397" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="398" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H397" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="398" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>244</v>
       </c>
@@ -11715,8 +12420,11 @@
       <c r="G398" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="399" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H398" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="399" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>244</v>
       </c>
@@ -11738,8 +12446,11 @@
       <c r="G399" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="400" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H399" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="400" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>244</v>
       </c>
@@ -11761,8 +12472,11 @@
       <c r="G400" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="401" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H400" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="401" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>244</v>
       </c>
@@ -11784,8 +12498,11 @@
       <c r="G401" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="402" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H401" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="402" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>244</v>
       </c>
@@ -11807,8 +12524,11 @@
       <c r="G402" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="403" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H402" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="403" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>244</v>
       </c>
@@ -11830,8 +12550,11 @@
       <c r="G403" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="404" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H403" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="404" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>244</v>
       </c>
@@ -11853,8 +12576,11 @@
       <c r="G404" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="405" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H404" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="405" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>244</v>
       </c>
@@ -11876,8 +12602,11 @@
       <c r="G405" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="406" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H405" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="406" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>244</v>
       </c>
@@ -11899,8 +12628,11 @@
       <c r="G406" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="407" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H406" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="407" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>244</v>
       </c>
@@ -11922,8 +12654,11 @@
       <c r="G407" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="408" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H407" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="408" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>244</v>
       </c>
@@ -11945,8 +12680,11 @@
       <c r="G408" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="409" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H408" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="409" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>244</v>
       </c>
@@ -11968,8 +12706,11 @@
       <c r="G409" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="410" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H409" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="410" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>244</v>
       </c>
@@ -11991,8 +12732,14 @@
       <c r="G410" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="411" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H410" t="s">
+        <v>466</v>
+      </c>
+      <c r="I410" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="411" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>244</v>
       </c>
@@ -12014,8 +12761,11 @@
       <c r="G411" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="412" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H411" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="412" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>244</v>
       </c>
@@ -12037,8 +12787,11 @@
       <c r="G412" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="413" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H412" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="413" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>244</v>
       </c>
@@ -12060,8 +12813,11 @@
       <c r="G413" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="414" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H413" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="414" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>244</v>
       </c>
@@ -12083,8 +12839,11 @@
       <c r="G414" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="415" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H414" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="415" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>244</v>
       </c>
@@ -12106,8 +12865,11 @@
       <c r="G415" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="416" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H415" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="416" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>244</v>
       </c>
@@ -12129,8 +12891,11 @@
       <c r="G416" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="417" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H416" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="417" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>244</v>
       </c>
@@ -12152,8 +12917,11 @@
       <c r="G417" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="418" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H417" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="418" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>244</v>
       </c>
@@ -12175,8 +12943,11 @@
       <c r="G418" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="419" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H418" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="419" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>244</v>
       </c>
@@ -12198,8 +12969,11 @@
       <c r="G419" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="420" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H419" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="420" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>244</v>
       </c>
@@ -12221,8 +12995,11 @@
       <c r="G420" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="421" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H420" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="421" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>244</v>
       </c>
@@ -12244,8 +13021,11 @@
       <c r="G421" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="422" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H421" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="422" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>244</v>
       </c>
@@ -12268,7 +13048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="423" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>244</v>
       </c>
@@ -12291,7 +13071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="424" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>244</v>
       </c>
@@ -12314,7 +13094,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="425" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>244</v>
       </c>
@@ -12337,7 +13117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="426" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>244</v>
       </c>
@@ -12360,7 +13140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="427" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>244</v>
       </c>
@@ -12383,7 +13163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="428" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>244</v>
       </c>
@@ -12406,7 +13186,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="429" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>244</v>
       </c>
@@ -12429,7 +13209,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="430" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
         <v>244</v>
       </c>
@@ -12452,7 +13232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="431" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>244</v>
       </c>
@@ -12475,7 +13255,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="432" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>244</v>
       </c>

</xml_diff>

<commit_message>
Finished Nit neg, needs rescuing
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0131ED56-A00C-49F8-ABFC-59816B7ECD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDB7EBD-0820-4724-B188-0B12E1E2F69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4853" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4982" uniqueCount="499">
   <si>
     <t>Amm</t>
   </si>
@@ -1432,6 +1432,96 @@
   </si>
   <si>
     <t>FT5606</t>
+  </si>
+  <si>
+    <t>FT0288</t>
+  </si>
+  <si>
+    <t>Check grouping</t>
+  </si>
+  <si>
+    <t>FT0323</t>
+  </si>
+  <si>
+    <t>FT1100</t>
+  </si>
+  <si>
+    <t>FT1186</t>
+  </si>
+  <si>
+    <t>FT1259</t>
+  </si>
+  <si>
+    <t>FT1461</t>
+  </si>
+  <si>
+    <t>FT1477</t>
+  </si>
+  <si>
+    <t>Looks gross :(</t>
+  </si>
+  <si>
+    <t>FT1484</t>
+  </si>
+  <si>
+    <t>There's a super spread out peak here but looks gross</t>
+  </si>
+  <si>
+    <t>FT1662</t>
+  </si>
+  <si>
+    <t>FT1719</t>
+  </si>
+  <si>
+    <t>FT1767</t>
+  </si>
+  <si>
+    <t>FT1769</t>
+  </si>
+  <si>
+    <t>Could be rescued</t>
+  </si>
+  <si>
+    <t>FT2197</t>
+  </si>
+  <si>
+    <t>FT2255</t>
+  </si>
+  <si>
+    <t>Maybe?</t>
+  </si>
+  <si>
+    <t>FT2284</t>
+  </si>
+  <si>
+    <t>Check edges</t>
+  </si>
+  <si>
+    <t>FT2687</t>
+  </si>
+  <si>
+    <t>FT2716</t>
+  </si>
+  <si>
+    <t>FT2895</t>
+  </si>
+  <si>
+    <t>FT3054</t>
+  </si>
+  <si>
+    <t>Weird in pooled</t>
+  </si>
+  <si>
+    <t>FT3996</t>
+  </si>
+  <si>
+    <t>Other peak present but too far off in RT</t>
+  </si>
+  <si>
+    <t>FT4499</t>
+  </si>
+  <si>
+    <t>FT4500</t>
   </si>
 </sst>
 </file>
@@ -1751,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A395" workbookViewId="0">
-      <selection activeCell="D404" sqref="D404"/>
+    <sheetView tabSelected="1" topLeftCell="A515" workbookViewId="0">
+      <selection activeCell="I533" sqref="I533"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12895,7 +12985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="417" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>244</v>
       </c>
@@ -12921,7 +13011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>244</v>
       </c>
@@ -12947,7 +13037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>244</v>
       </c>
@@ -12973,7 +13063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="420" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>244</v>
       </c>
@@ -12999,7 +13089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>244</v>
       </c>
@@ -13025,7 +13115,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="422" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>244</v>
       </c>
@@ -13047,8 +13137,14 @@
       <c r="G422" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H422" t="s">
+        <v>469</v>
+      </c>
+      <c r="I422" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="423" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>244</v>
       </c>
@@ -13070,8 +13166,11 @@
       <c r="G423" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H423" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="424" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>244</v>
       </c>
@@ -13093,8 +13192,11 @@
       <c r="G424" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H424" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="425" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>244</v>
       </c>
@@ -13116,8 +13218,11 @@
       <c r="G425" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="426" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H425" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="426" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>244</v>
       </c>
@@ -13139,8 +13244,11 @@
       <c r="G426" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="427" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I426" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="427" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>244</v>
       </c>
@@ -13162,8 +13270,11 @@
       <c r="G427" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="428" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H427" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="428" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>244</v>
       </c>
@@ -13185,8 +13296,11 @@
       <c r="G428" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="429" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H428" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="429" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>244</v>
       </c>
@@ -13208,8 +13322,11 @@
       <c r="G429" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H429" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="430" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
         <v>244</v>
       </c>
@@ -13231,8 +13348,11 @@
       <c r="G430" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="431" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H430" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="431" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>244</v>
       </c>
@@ -13254,8 +13374,11 @@
       <c r="G431" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="432" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H431" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="432" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>244</v>
       </c>
@@ -13277,8 +13400,11 @@
       <c r="G432" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="433" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H432" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="433" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
         <v>244</v>
       </c>
@@ -13300,8 +13426,11 @@
       <c r="G433" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="434" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H433" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="434" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
         <v>244</v>
       </c>
@@ -13323,8 +13452,11 @@
       <c r="G434" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="435" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H434" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="435" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
         <v>244</v>
       </c>
@@ -13346,8 +13478,11 @@
       <c r="G435" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="436" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H435" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="436" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
         <v>244</v>
       </c>
@@ -13369,8 +13504,11 @@
       <c r="G436" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="437" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H436" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="437" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
         <v>244</v>
       </c>
@@ -13392,8 +13530,14 @@
       <c r="G437" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="438" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H437" t="s">
+        <v>475</v>
+      </c>
+      <c r="I437" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="438" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
         <v>244</v>
       </c>
@@ -13415,8 +13559,14 @@
       <c r="G438" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="439" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H438" t="s">
+        <v>476</v>
+      </c>
+      <c r="I438" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="439" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
         <v>244</v>
       </c>
@@ -13438,8 +13588,11 @@
       <c r="G439" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="440" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H439" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="440" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
         <v>244</v>
       </c>
@@ -13461,8 +13614,14 @@
       <c r="G440" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="441" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H440" t="s">
+        <v>5</v>
+      </c>
+      <c r="I440" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="441" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
         <v>244</v>
       </c>
@@ -13484,8 +13643,11 @@
       <c r="G441" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="442" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H441" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="442" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
         <v>244</v>
       </c>
@@ -13507,8 +13669,11 @@
       <c r="G442" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="443" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I442" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="443" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
         <v>244</v>
       </c>
@@ -13530,8 +13695,11 @@
       <c r="G443" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="444" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H443" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="444" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
         <v>244</v>
       </c>
@@ -13553,8 +13721,11 @@
       <c r="G444" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="445" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H444" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="445" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
         <v>244</v>
       </c>
@@ -13576,8 +13747,11 @@
       <c r="G445" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="446" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H445" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="446" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
         <v>244</v>
       </c>
@@ -13599,8 +13773,11 @@
       <c r="G446" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="447" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H446" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="447" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
         <v>244</v>
       </c>
@@ -13622,8 +13799,11 @@
       <c r="G447" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="448" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H447" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="448" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
         <v>244</v>
       </c>
@@ -13645,8 +13825,11 @@
       <c r="G448" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="449" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H448" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="449" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
         <v>244</v>
       </c>
@@ -13668,8 +13851,11 @@
       <c r="G449" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="450" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H449" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="450" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
         <v>244</v>
       </c>
@@ -13691,8 +13877,11 @@
       <c r="G450" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="451" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H450" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="451" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
         <v>244</v>
       </c>
@@ -13714,8 +13903,14 @@
       <c r="G451" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="452" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H451" t="s">
+        <v>5</v>
+      </c>
+      <c r="I451" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="452" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A452" t="s">
         <v>244</v>
       </c>
@@ -13737,8 +13932,11 @@
       <c r="G452" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="453" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H452" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="453" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
         <v>244</v>
       </c>
@@ -13760,8 +13958,11 @@
       <c r="G453" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="454" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H453" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="454" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
         <v>244</v>
       </c>
@@ -13783,8 +13984,11 @@
       <c r="G454" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="455" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H454" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="455" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
         <v>244</v>
       </c>
@@ -13806,8 +14010,11 @@
       <c r="G455" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="456" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H455" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="456" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
         <v>244</v>
       </c>
@@ -13829,8 +14036,11 @@
       <c r="G456" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="457" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H456" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="457" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
         <v>244</v>
       </c>
@@ -13852,8 +14062,11 @@
       <c r="G457" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="458" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H457" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="458" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
         <v>244</v>
       </c>
@@ -13875,8 +14088,11 @@
       <c r="G458" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="459" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H458" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="459" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
         <v>244</v>
       </c>
@@ -13898,8 +14114,11 @@
       <c r="G459" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="460" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H459" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="460" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
         <v>244</v>
       </c>
@@ -13921,8 +14140,11 @@
       <c r="G460" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="461" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H460" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="461" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
         <v>244</v>
       </c>
@@ -13944,8 +14166,11 @@
       <c r="G461" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="462" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H461" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="462" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
         <v>244</v>
       </c>
@@ -13967,8 +14192,11 @@
       <c r="G462" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="463" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H462" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="463" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
         <v>244</v>
       </c>
@@ -13990,8 +14218,11 @@
       <c r="G463" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="464" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H463" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="464" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
         <v>244</v>
       </c>
@@ -14013,8 +14244,11 @@
       <c r="G464" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="465" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H464" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="465" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
         <v>244</v>
       </c>
@@ -14036,8 +14270,11 @@
       <c r="G465" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="466" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H465" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="466" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
         <v>244</v>
       </c>
@@ -14059,8 +14296,14 @@
       <c r="G466" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="467" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H466" t="s">
+        <v>486</v>
+      </c>
+      <c r="I466" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="467" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
         <v>244</v>
       </c>
@@ -14082,8 +14325,11 @@
       <c r="G467" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="468" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H467" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="468" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
         <v>244</v>
       </c>
@@ -14105,8 +14351,14 @@
       <c r="G468" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="469" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H468" t="s">
+        <v>488</v>
+      </c>
+      <c r="I468" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="469" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
         <v>244</v>
       </c>
@@ -14128,8 +14380,11 @@
       <c r="G469" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="470" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H469" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="470" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A470" t="s">
         <v>244</v>
       </c>
@@ -14151,8 +14406,11 @@
       <c r="G470" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="471" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H470" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="471" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A471" t="s">
         <v>244</v>
       </c>
@@ -14174,8 +14432,11 @@
       <c r="G471" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="472" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H471" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="472" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
         <v>244</v>
       </c>
@@ -14197,8 +14458,11 @@
       <c r="G472" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="473" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H472" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="473" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
         <v>244</v>
       </c>
@@ -14220,8 +14484,11 @@
       <c r="G473" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="474" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H473" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="474" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A474" t="s">
         <v>244</v>
       </c>
@@ -14243,8 +14510,11 @@
       <c r="G474" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="475" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H474" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="475" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A475" t="s">
         <v>244</v>
       </c>
@@ -14266,8 +14536,11 @@
       <c r="G475" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="476" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H475" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="476" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
         <v>244</v>
       </c>
@@ -14289,8 +14562,11 @@
       <c r="G476" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="477" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H476" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="477" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
         <v>244</v>
       </c>
@@ -14312,8 +14588,11 @@
       <c r="G477" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="478" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H477" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="478" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
         <v>244</v>
       </c>
@@ -14335,8 +14614,11 @@
       <c r="G478" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="479" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H478" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="479" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
         <v>244</v>
       </c>
@@ -14358,8 +14640,11 @@
       <c r="G479" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="480" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H479" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="480" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
         <v>244</v>
       </c>
@@ -14381,8 +14666,11 @@
       <c r="G480" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="481" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H480" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="481" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
         <v>244</v>
       </c>
@@ -14404,8 +14692,11 @@
       <c r="G481" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="482" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H481" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="482" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
         <v>244</v>
       </c>
@@ -14427,8 +14718,11 @@
       <c r="G482" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="483" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H482" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="483" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
         <v>244</v>
       </c>
@@ -14450,8 +14744,11 @@
       <c r="G483" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="484" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H483" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="484" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
         <v>244</v>
       </c>
@@ -14473,8 +14770,11 @@
       <c r="G484" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="485" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H484" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="485" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
         <v>244</v>
       </c>
@@ -14496,8 +14796,11 @@
       <c r="G485" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="486" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H485" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="486" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
         <v>244</v>
       </c>
@@ -14519,8 +14822,11 @@
       <c r="G486" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="487" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H486" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="487" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
         <v>244</v>
       </c>
@@ -14542,8 +14848,11 @@
       <c r="G487" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="488" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H487" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="488" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A488" t="s">
         <v>244</v>
       </c>
@@ -14565,8 +14874,11 @@
       <c r="G488" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="489" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H488" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="489" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
         <v>244</v>
       </c>
@@ -14588,8 +14900,11 @@
       <c r="G489" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="490" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H489" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="490" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
         <v>244</v>
       </c>
@@ -14611,8 +14926,14 @@
       <c r="G490" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="491" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H490" t="s">
+        <v>493</v>
+      </c>
+      <c r="I490" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="491" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
         <v>244</v>
       </c>
@@ -14634,8 +14955,11 @@
       <c r="G491" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="492" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H491" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="492" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
         <v>244</v>
       </c>
@@ -14657,8 +14981,11 @@
       <c r="G492" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="493" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H492" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="493" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>244</v>
       </c>
@@ -14680,8 +15007,11 @@
       <c r="G493" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="494" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H493" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="494" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
         <v>244</v>
       </c>
@@ -14703,8 +15033,11 @@
       <c r="G494" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="495" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H494" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="495" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
         <v>244</v>
       </c>
@@ -14726,8 +15059,11 @@
       <c r="G495" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="496" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H495" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="496" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
         <v>244</v>
       </c>
@@ -14749,8 +15085,11 @@
       <c r="G496" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="497" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H496" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="497" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>244</v>
       </c>
@@ -14772,8 +15111,11 @@
       <c r="G497" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="498" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H497" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="498" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
         <v>244</v>
       </c>
@@ -14795,8 +15137,11 @@
       <c r="G498" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="499" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H498" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="499" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
         <v>244</v>
       </c>
@@ -14818,8 +15163,11 @@
       <c r="G499" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="500" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H499" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="500" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
         <v>244</v>
       </c>
@@ -14841,8 +15189,11 @@
       <c r="G500" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="501" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H500" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="501" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
         <v>244</v>
       </c>
@@ -14864,8 +15215,11 @@
       <c r="G501" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="502" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H501" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="502" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
         <v>244</v>
       </c>
@@ -14887,8 +15241,11 @@
       <c r="G502" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="503" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H502" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="503" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
         <v>244</v>
       </c>
@@ -14910,8 +15267,11 @@
       <c r="G503" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="504" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H503" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="504" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
         <v>244</v>
       </c>
@@ -14933,8 +15293,11 @@
       <c r="G504" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="505" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H504" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="505" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>244</v>
       </c>
@@ -14956,8 +15319,11 @@
       <c r="G505" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="506" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H505" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="506" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
         <v>244</v>
       </c>
@@ -14979,8 +15345,11 @@
       <c r="G506" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="507" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H506" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="507" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
         <v>244</v>
       </c>
@@ -15002,8 +15371,14 @@
       <c r="G507" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="508" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H507" t="s">
+        <v>5</v>
+      </c>
+      <c r="I507" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="508" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
         <v>244</v>
       </c>
@@ -15025,8 +15400,11 @@
       <c r="G508" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="509" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H508" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="509" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
         <v>244</v>
       </c>
@@ -15048,8 +15426,11 @@
       <c r="G509" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="510" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H509" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="510" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
         <v>244</v>
       </c>
@@ -15071,8 +15452,11 @@
       <c r="G510" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="511" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H510" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="511" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>244</v>
       </c>
@@ -15094,8 +15478,11 @@
       <c r="G511" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="512" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H511" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="512" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
         <v>244</v>
       </c>
@@ -15117,8 +15504,11 @@
       <c r="G512" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="513" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H512" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="513" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>244</v>
       </c>
@@ -15140,8 +15530,11 @@
       <c r="G513" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="514" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H513" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
         <v>244</v>
       </c>
@@ -15163,8 +15556,11 @@
       <c r="G514" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="515" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H514" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
         <v>244</v>
       </c>
@@ -15186,8 +15582,11 @@
       <c r="G515" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="516" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H515" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
         <v>244</v>
       </c>
@@ -15209,8 +15608,11 @@
       <c r="G516" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="517" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H516" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="517" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A517" t="s">
         <v>244</v>
       </c>
@@ -15232,8 +15634,11 @@
       <c r="G517" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="518" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H517" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="518" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A518" t="s">
         <v>244</v>
       </c>
@@ -15255,8 +15660,11 @@
       <c r="G518" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="519" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H518" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="519" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
         <v>244</v>
       </c>
@@ -15278,8 +15686,11 @@
       <c r="G519" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="520" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H519" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="520" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A520" t="s">
         <v>244</v>
       </c>
@@ -15301,8 +15712,11 @@
       <c r="G520" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="521" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H520" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="521" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A521" t="s">
         <v>244</v>
       </c>
@@ -15324,8 +15738,11 @@
       <c r="G521" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="522" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H521" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="522" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A522" t="s">
         <v>244</v>
       </c>
@@ -15347,8 +15764,11 @@
       <c r="G522" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="523" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H522" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="523" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A523" t="s">
         <v>244</v>
       </c>
@@ -15370,8 +15790,11 @@
       <c r="G523" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="524" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H523" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="524" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A524" t="s">
         <v>244</v>
       </c>
@@ -15393,8 +15816,11 @@
       <c r="G524" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="525" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H524" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="525" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A525" t="s">
         <v>244</v>
       </c>
@@ -15416,8 +15842,11 @@
       <c r="G525" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="526" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H525" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="526" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A526" t="s">
         <v>244</v>
       </c>
@@ -15439,8 +15868,11 @@
       <c r="G526" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="527" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H526" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="527" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A527" t="s">
         <v>244</v>
       </c>
@@ -15462,8 +15894,11 @@
       <c r="G527" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="528" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H527" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="528" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A528" t="s">
         <v>244</v>
       </c>
@@ -15485,8 +15920,11 @@
       <c r="G528" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="529" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H528" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="529" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A529" t="s">
         <v>244</v>
       </c>
@@ -15508,8 +15946,11 @@
       <c r="G529" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="530" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H529" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="530" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A530" t="s">
         <v>244</v>
       </c>
@@ -15531,8 +15972,11 @@
       <c r="G530" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="531" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H530" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="531" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A531" t="s">
         <v>244</v>
       </c>
@@ -15554,8 +15998,11 @@
       <c r="G531" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="532" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H531" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="532" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
         <v>244</v>
       </c>
@@ -15577,8 +16024,11 @@
       <c r="G532" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="533" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H532" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="533" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A533" t="s">
         <v>244</v>
       </c>
@@ -15600,8 +16050,11 @@
       <c r="G533" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="534" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H533" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="534" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A534" t="s">
         <v>244</v>
       </c>
@@ -15623,8 +16076,11 @@
       <c r="G534" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="535" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H534" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="535" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
         <v>244</v>
       </c>
@@ -15646,8 +16102,11 @@
       <c r="G535" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="536" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H535" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="536" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A536" t="s">
         <v>244</v>
       </c>
@@ -15669,8 +16128,11 @@
       <c r="G536" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="537" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H536" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="537" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
         <v>244</v>
       </c>
@@ -15692,8 +16154,11 @@
       <c r="G537" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="538" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H537" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="538" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A538" t="s">
         <v>244</v>
       </c>
@@ -15715,8 +16180,11 @@
       <c r="G538" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="539" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H538" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="539" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A539" t="s">
         <v>244</v>
       </c>
@@ -15738,8 +16206,11 @@
       <c r="G539" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="540" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H539" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="540" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A540" t="s">
         <v>244</v>
       </c>
@@ -15761,8 +16232,11 @@
       <c r="G540" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="541" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H540" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="541" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A541" t="s">
         <v>244</v>
       </c>
@@ -15784,8 +16258,11 @@
       <c r="G541" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="542" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H541" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="542" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A542" t="s">
         <v>245</v>
       </c>
@@ -15808,7 +16285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="543" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A543" t="s">
         <v>245</v>
       </c>
@@ -15831,7 +16308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="544" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A544" t="s">
         <v>245</v>
       </c>

</xml_diff>

<commit_message>
Finished rescuing Nit neg after some confusion
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDB7EBD-0820-4724-B188-0B12E1E2F69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32831AF-A08A-44B8-8805-AEF80A417C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4982" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4983" uniqueCount="499">
   <si>
     <t>Amm</t>
   </si>
@@ -1479,9 +1479,6 @@
     <t>FT1769</t>
   </si>
   <si>
-    <t>Could be rescued</t>
-  </si>
-  <si>
     <t>FT2197</t>
   </si>
   <si>
@@ -1522,6 +1519,9 @@
   </si>
   <si>
     <t>FT4500</t>
+  </si>
+  <si>
+    <t>Rescued</t>
   </si>
 </sst>
 </file>
@@ -1841,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A515" workbookViewId="0">
-      <selection activeCell="I533" sqref="I533"/>
+    <sheetView tabSelected="1" topLeftCell="A413" workbookViewId="0">
+      <selection activeCell="I427" sqref="I427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13244,8 +13244,11 @@
       <c r="G426" t="s">
         <v>5</v>
       </c>
+      <c r="H426" t="s">
+        <v>5</v>
+      </c>
       <c r="I426" t="s">
-        <v>394</v>
+        <v>498</v>
       </c>
     </row>
     <row r="427" spans="1:9" x14ac:dyDescent="0.3">
@@ -13670,7 +13673,7 @@
         <v>5</v>
       </c>
       <c r="I442" t="s">
-        <v>394</v>
+        <v>498</v>
       </c>
     </row>
     <row r="443" spans="1:9" x14ac:dyDescent="0.3">
@@ -13907,7 +13910,7 @@
         <v>5</v>
       </c>
       <c r="I451" t="s">
-        <v>484</v>
+        <v>498</v>
       </c>
     </row>
     <row r="452" spans="1:9" x14ac:dyDescent="0.3">
@@ -14219,7 +14222,7 @@
         <v>11</v>
       </c>
       <c r="H463" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="464" spans="1:9" x14ac:dyDescent="0.3">
@@ -14297,10 +14300,10 @@
         <v>11</v>
       </c>
       <c r="H466" t="s">
+        <v>485</v>
+      </c>
+      <c r="I466" t="s">
         <v>486</v>
-      </c>
-      <c r="I466" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="467" spans="1:9" x14ac:dyDescent="0.3">
@@ -14352,10 +14355,10 @@
         <v>11</v>
       </c>
       <c r="H468" t="s">
+        <v>487</v>
+      </c>
+      <c r="I468" t="s">
         <v>488</v>
-      </c>
-      <c r="I468" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="469" spans="1:9" x14ac:dyDescent="0.3">
@@ -14667,7 +14670,7 @@
         <v>11</v>
       </c>
       <c r="H480" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="481" spans="1:9" x14ac:dyDescent="0.3">
@@ -14693,7 +14696,7 @@
         <v>11</v>
       </c>
       <c r="H481" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="482" spans="1:9" x14ac:dyDescent="0.3">
@@ -14797,7 +14800,7 @@
         <v>5</v>
       </c>
       <c r="H485" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="486" spans="1:9" x14ac:dyDescent="0.3">
@@ -14927,10 +14930,10 @@
         <v>3</v>
       </c>
       <c r="H490" t="s">
+        <v>492</v>
+      </c>
+      <c r="I490" t="s">
         <v>493</v>
-      </c>
-      <c r="I490" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="491" spans="1:9" x14ac:dyDescent="0.3">
@@ -15346,7 +15349,7 @@
         <v>5</v>
       </c>
       <c r="H506" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="507" spans="1:9" x14ac:dyDescent="0.3">
@@ -15375,7 +15378,7 @@
         <v>5</v>
       </c>
       <c r="I507" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="508" spans="1:9" x14ac:dyDescent="0.3">
@@ -15505,7 +15508,7 @@
         <v>3</v>
       </c>
       <c r="H512" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="513" spans="1:8" x14ac:dyDescent="0.3">
@@ -15583,7 +15586,7 @@
         <v>11</v>
       </c>
       <c r="H515" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="516" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Finished rescuing Nit pos
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32831AF-A08A-44B8-8805-AEF80A417C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59DEF64-D510-41B2-BF59-33624D543E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4983" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4994" uniqueCount="507">
   <si>
     <t>Amm</t>
   </si>
@@ -1215,9 +1215,6 @@
     <t>FT1419</t>
   </si>
   <si>
-    <t>Rescue (optional)</t>
-  </si>
-  <si>
     <t>FT1478</t>
   </si>
   <si>
@@ -1311,9 +1308,6 @@
     <t>FT2482</t>
   </si>
   <si>
-    <t>Rescue?</t>
-  </si>
-  <si>
     <t>FT2521</t>
   </si>
   <si>
@@ -1377,9 +1371,6 @@
     <t>Check on grouping (do this first)</t>
   </si>
   <si>
-    <t>Could be worth rescuing</t>
-  </si>
-  <si>
     <t>FT3542</t>
   </si>
   <si>
@@ -1522,6 +1513,39 @@
   </si>
   <si>
     <t>Rescued</t>
+  </si>
+  <si>
+    <t>FT1339</t>
+  </si>
+  <si>
+    <t>FT1444</t>
+  </si>
+  <si>
+    <t>FT1956</t>
+  </si>
+  <si>
+    <t>FT1980</t>
+  </si>
+  <si>
+    <t>FT2404</t>
+  </si>
+  <si>
+    <t>Unable to rescue, no peaks picked at all</t>
+  </si>
+  <si>
+    <t>FT2706</t>
+  </si>
+  <si>
+    <t>Not rescued</t>
+  </si>
+  <si>
+    <t>FT3317</t>
+  </si>
+  <si>
+    <t>Could be worth rescuing (it's not)</t>
+  </si>
+  <si>
+    <t>FT4428</t>
   </si>
 </sst>
 </file>
@@ -1841,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A413" workbookViewId="0">
-      <selection activeCell="I427" sqref="I427"/>
+    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
+      <selection activeCell="I392" sqref="I392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9570,8 +9594,11 @@
       <c r="G287" t="s">
         <v>3</v>
       </c>
+      <c r="H287" t="s">
+        <v>496</v>
+      </c>
       <c r="I287" t="s">
-        <v>394</v>
+        <v>495</v>
       </c>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.3">
@@ -9648,8 +9675,11 @@
       <c r="G290" t="s">
         <v>3</v>
       </c>
+      <c r="H290" t="s">
+        <v>497</v>
+      </c>
       <c r="I290" t="s">
-        <v>396</v>
+        <v>495</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.3">
@@ -9675,7 +9705,7 @@
         <v>3</v>
       </c>
       <c r="H291" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.3">
@@ -9727,10 +9757,10 @@
         <v>3</v>
       </c>
       <c r="H293" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I293" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">
@@ -9756,10 +9786,10 @@
         <v>3</v>
       </c>
       <c r="H294" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I294" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.3">
@@ -9785,7 +9815,7 @@
         <v>11</v>
       </c>
       <c r="H295" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.3">
@@ -9866,7 +9896,7 @@
         <v>5</v>
       </c>
       <c r="I298" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.3">
@@ -9918,10 +9948,10 @@
         <v>11</v>
       </c>
       <c r="H300" t="s">
+        <v>401</v>
+      </c>
+      <c r="I300" t="s">
         <v>402</v>
-      </c>
-      <c r="I300" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.3">
@@ -9973,7 +10003,7 @@
         <v>11</v>
       </c>
       <c r="H302" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.3">
@@ -10054,7 +10084,7 @@
         <v>5</v>
       </c>
       <c r="I305" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.3">
@@ -10080,7 +10110,7 @@
         <v>3</v>
       </c>
       <c r="H306" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="307" spans="1:9" x14ac:dyDescent="0.3">
@@ -10106,7 +10136,7 @@
         <v>3</v>
       </c>
       <c r="H307" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.3">
@@ -10131,8 +10161,11 @@
       <c r="G308" t="s">
         <v>3</v>
       </c>
+      <c r="H308" t="s">
+        <v>498</v>
+      </c>
       <c r="I308" t="s">
-        <v>394</v>
+        <v>495</v>
       </c>
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.3">
@@ -10158,10 +10191,10 @@
         <v>3</v>
       </c>
       <c r="H309" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I309" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.3">
@@ -10187,7 +10220,7 @@
         <v>11</v>
       </c>
       <c r="H310" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.3">
@@ -10213,10 +10246,10 @@
         <v>3</v>
       </c>
       <c r="H311" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I311" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.3">
@@ -10241,8 +10274,11 @@
       <c r="G312" t="s">
         <v>3</v>
       </c>
+      <c r="H312" t="s">
+        <v>499</v>
+      </c>
       <c r="I312" t="s">
-        <v>394</v>
+        <v>495</v>
       </c>
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.3">
@@ -10268,10 +10304,10 @@
         <v>3</v>
       </c>
       <c r="H313" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I313" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="314" spans="1:9" x14ac:dyDescent="0.3">
@@ -10297,7 +10333,7 @@
         <v>11</v>
       </c>
       <c r="H314" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.3">
@@ -10349,7 +10385,7 @@
         <v>11</v>
       </c>
       <c r="H316" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="317" spans="1:9" x14ac:dyDescent="0.3">
@@ -10375,7 +10411,7 @@
         <v>3</v>
       </c>
       <c r="H317" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="318" spans="1:9" x14ac:dyDescent="0.3">
@@ -10401,7 +10437,7 @@
         <v>11</v>
       </c>
       <c r="H318" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="319" spans="1:9" x14ac:dyDescent="0.3">
@@ -10427,7 +10463,7 @@
         <v>11</v>
       </c>
       <c r="H319" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="320" spans="1:9" x14ac:dyDescent="0.3">
@@ -10453,7 +10489,7 @@
         <v>11</v>
       </c>
       <c r="H320" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.3">
@@ -10479,7 +10515,7 @@
         <v>3</v>
       </c>
       <c r="H321" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="322" spans="1:9" x14ac:dyDescent="0.3">
@@ -10505,10 +10541,10 @@
         <v>11</v>
       </c>
       <c r="H322" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I322" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.3">
@@ -10586,7 +10622,7 @@
         <v>11</v>
       </c>
       <c r="H325" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.3">
@@ -10612,7 +10648,7 @@
         <v>3</v>
       </c>
       <c r="H326" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.3">
@@ -10638,7 +10674,7 @@
         <v>3</v>
       </c>
       <c r="H327" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.3">
@@ -10667,7 +10703,7 @@
         <v>5</v>
       </c>
       <c r="I328" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.3">
@@ -10693,7 +10729,7 @@
         <v>3</v>
       </c>
       <c r="H329" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.3">
@@ -10718,8 +10754,11 @@
       <c r="G330" t="s">
         <v>3</v>
       </c>
+      <c r="H330" t="s">
+        <v>500</v>
+      </c>
       <c r="I330" t="s">
-        <v>394</v>
+        <v>495</v>
       </c>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.3">
@@ -10771,10 +10810,10 @@
         <v>11</v>
       </c>
       <c r="H332" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I332" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.3">
@@ -10800,10 +10839,10 @@
         <v>3</v>
       </c>
       <c r="H333" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I333" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.3">
@@ -10829,7 +10868,7 @@
         <v>11</v>
       </c>
       <c r="H334" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.3">
@@ -10855,10 +10894,10 @@
         <v>3</v>
       </c>
       <c r="H335" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I335" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.3">
@@ -10909,8 +10948,11 @@
       <c r="G337" t="s">
         <v>5</v>
       </c>
+      <c r="H337" t="s">
+        <v>5</v>
+      </c>
       <c r="I337" t="s">
-        <v>428</v>
+        <v>501</v>
       </c>
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.3">
@@ -10936,7 +10978,7 @@
         <v>5</v>
       </c>
       <c r="H338" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.3">
@@ -10988,7 +11030,7 @@
         <v>11</v>
       </c>
       <c r="H340" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.3">
@@ -11066,7 +11108,7 @@
         <v>3</v>
       </c>
       <c r="H343" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.3">
@@ -11092,7 +11134,7 @@
         <v>11</v>
       </c>
       <c r="H344" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.3">
@@ -11118,7 +11160,7 @@
         <v>11</v>
       </c>
       <c r="H345" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.3">
@@ -11144,10 +11186,10 @@
         <v>5</v>
       </c>
       <c r="H346" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="I346" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.3">
@@ -11224,8 +11266,11 @@
       <c r="G349" t="s">
         <v>5</v>
       </c>
+      <c r="H349" t="s">
+        <v>502</v>
+      </c>
       <c r="I349" t="s">
-        <v>394</v>
+        <v>495</v>
       </c>
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.3">
@@ -11251,7 +11296,7 @@
         <v>5</v>
       </c>
       <c r="H350" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.3">
@@ -11277,7 +11322,7 @@
         <v>3</v>
       </c>
       <c r="H351" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="352" spans="1:9" x14ac:dyDescent="0.3">
@@ -11329,10 +11374,10 @@
         <v>3</v>
       </c>
       <c r="H353" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="I353" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="354" spans="1:9" x14ac:dyDescent="0.3">
@@ -11409,8 +11454,11 @@
       <c r="G356" t="s">
         <v>3</v>
       </c>
+      <c r="H356" t="s">
+        <v>5</v>
+      </c>
       <c r="I356" t="s">
-        <v>394</v>
+        <v>503</v>
       </c>
     </row>
     <row r="357" spans="1:9" x14ac:dyDescent="0.3">
@@ -11462,7 +11510,7 @@
         <v>5</v>
       </c>
       <c r="H358" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="359" spans="1:9" x14ac:dyDescent="0.3">
@@ -11488,7 +11536,7 @@
         <v>3</v>
       </c>
       <c r="H359" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.3">
@@ -11540,7 +11588,7 @@
         <v>3</v>
       </c>
       <c r="H361" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.3">
@@ -11566,7 +11614,7 @@
         <v>11</v>
       </c>
       <c r="H362" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.3">
@@ -11618,7 +11666,7 @@
         <v>11</v>
       </c>
       <c r="H364" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.3">
@@ -11647,7 +11695,7 @@
         <v>5</v>
       </c>
       <c r="I365" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.3">
@@ -11673,10 +11721,10 @@
         <v>3</v>
       </c>
       <c r="H366" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="I366" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="367" spans="1:9" x14ac:dyDescent="0.3">
@@ -11702,7 +11750,7 @@
         <v>3</v>
       </c>
       <c r="H367" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="368" spans="1:9" x14ac:dyDescent="0.3">
@@ -11728,7 +11776,7 @@
         <v>3</v>
       </c>
       <c r="H368" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="369" spans="1:9" x14ac:dyDescent="0.3">
@@ -11754,10 +11802,10 @@
         <v>3</v>
       </c>
       <c r="H369" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="I369" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="370" spans="1:9" x14ac:dyDescent="0.3">
@@ -11782,6 +11830,9 @@
       <c r="G370" t="s">
         <v>11</v>
       </c>
+      <c r="H370" t="s">
+        <v>504</v>
+      </c>
       <c r="I370" t="s">
         <v>394</v>
       </c>
@@ -11808,8 +11859,11 @@
       <c r="G371" t="s">
         <v>3</v>
       </c>
+      <c r="H371" t="s">
+        <v>5</v>
+      </c>
       <c r="I371" t="s">
-        <v>450</v>
+        <v>505</v>
       </c>
     </row>
     <row r="372" spans="1:9" x14ac:dyDescent="0.3">
@@ -11835,7 +11889,7 @@
         <v>3</v>
       </c>
       <c r="H372" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="373" spans="1:9" x14ac:dyDescent="0.3">
@@ -12043,7 +12097,7 @@
         <v>5</v>
       </c>
       <c r="H380" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="381" spans="1:9" x14ac:dyDescent="0.3">
@@ -12173,7 +12227,7 @@
         <v>11</v>
       </c>
       <c r="H385" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="386" spans="1:9" x14ac:dyDescent="0.3">
@@ -12199,7 +12253,7 @@
         <v>5</v>
       </c>
       <c r="H386" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="387" spans="1:9" x14ac:dyDescent="0.3">
@@ -12251,7 +12305,7 @@
         <v>5</v>
       </c>
       <c r="H388" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="389" spans="1:9" x14ac:dyDescent="0.3">
@@ -12277,7 +12331,7 @@
         <v>3</v>
       </c>
       <c r="H389" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="390" spans="1:9" x14ac:dyDescent="0.3">
@@ -12303,7 +12357,7 @@
         <v>11</v>
       </c>
       <c r="H390" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="391" spans="1:9" x14ac:dyDescent="0.3">
@@ -12328,8 +12382,11 @@
       <c r="G391" t="s">
         <v>11</v>
       </c>
+      <c r="H391" t="s">
+        <v>506</v>
+      </c>
       <c r="I391" t="s">
-        <v>394</v>
+        <v>495</v>
       </c>
     </row>
     <row r="392" spans="1:9" x14ac:dyDescent="0.3">
@@ -12355,7 +12412,7 @@
         <v>3</v>
       </c>
       <c r="H392" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="393" spans="1:9" x14ac:dyDescent="0.3">
@@ -12433,7 +12490,7 @@
         <v>11</v>
       </c>
       <c r="H395" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="396" spans="1:9" x14ac:dyDescent="0.3">
@@ -12459,7 +12516,7 @@
         <v>5</v>
       </c>
       <c r="H396" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="397" spans="1:9" x14ac:dyDescent="0.3">
@@ -12511,7 +12568,7 @@
         <v>11</v>
       </c>
       <c r="H398" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="399" spans="1:9" x14ac:dyDescent="0.3">
@@ -12537,7 +12594,7 @@
         <v>11</v>
       </c>
       <c r="H399" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="400" spans="1:9" x14ac:dyDescent="0.3">
@@ -12563,7 +12620,7 @@
         <v>5</v>
       </c>
       <c r="H400" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="401" spans="1:9" x14ac:dyDescent="0.3">
@@ -12589,7 +12646,7 @@
         <v>5</v>
       </c>
       <c r="H401" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="402" spans="1:9" x14ac:dyDescent="0.3">
@@ -12745,7 +12802,7 @@
         <v>5</v>
       </c>
       <c r="H407" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="408" spans="1:9" x14ac:dyDescent="0.3">
@@ -12797,7 +12854,7 @@
         <v>5</v>
       </c>
       <c r="H409" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="410" spans="1:9" x14ac:dyDescent="0.3">
@@ -12823,10 +12880,10 @@
         <v>5</v>
       </c>
       <c r="H410" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="I410" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="411" spans="1:9" x14ac:dyDescent="0.3">
@@ -12904,7 +12961,7 @@
         <v>5</v>
       </c>
       <c r="H413" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="414" spans="1:9" x14ac:dyDescent="0.3">
@@ -13138,10 +13195,10 @@
         <v>5</v>
       </c>
       <c r="H422" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I422" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="423" spans="1:9" x14ac:dyDescent="0.3">
@@ -13167,7 +13224,7 @@
         <v>5</v>
       </c>
       <c r="H423" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="424" spans="1:9" x14ac:dyDescent="0.3">
@@ -13248,7 +13305,7 @@
         <v>5</v>
       </c>
       <c r="I426" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="427" spans="1:9" x14ac:dyDescent="0.3">
@@ -13352,7 +13409,7 @@
         <v>11</v>
       </c>
       <c r="H430" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="431" spans="1:9" x14ac:dyDescent="0.3">
@@ -13404,7 +13461,7 @@
         <v>3</v>
       </c>
       <c r="H432" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="433" spans="1:9" x14ac:dyDescent="0.3">
@@ -13456,7 +13513,7 @@
         <v>3</v>
       </c>
       <c r="H434" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="435" spans="1:9" x14ac:dyDescent="0.3">
@@ -13534,10 +13591,10 @@
         <v>11</v>
       </c>
       <c r="H437" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I437" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="438" spans="1:9" x14ac:dyDescent="0.3">
@@ -13563,10 +13620,10 @@
         <v>11</v>
       </c>
       <c r="H438" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I438" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="439" spans="1:9" x14ac:dyDescent="0.3">
@@ -13592,7 +13649,7 @@
         <v>11</v>
       </c>
       <c r="H439" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="440" spans="1:9" x14ac:dyDescent="0.3">
@@ -13621,7 +13678,7 @@
         <v>5</v>
       </c>
       <c r="I440" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="441" spans="1:9" x14ac:dyDescent="0.3">
@@ -13673,7 +13730,7 @@
         <v>5</v>
       </c>
       <c r="I442" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="443" spans="1:9" x14ac:dyDescent="0.3">
@@ -13777,7 +13834,7 @@
         <v>3</v>
       </c>
       <c r="H446" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="447" spans="1:9" x14ac:dyDescent="0.3">
@@ -13803,7 +13860,7 @@
         <v>3</v>
       </c>
       <c r="H447" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="448" spans="1:9" x14ac:dyDescent="0.3">
@@ -13829,7 +13886,7 @@
         <v>3</v>
       </c>
       <c r="H448" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="449" spans="1:9" x14ac:dyDescent="0.3">
@@ -13855,7 +13912,7 @@
         <v>11</v>
       </c>
       <c r="H449" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="450" spans="1:9" x14ac:dyDescent="0.3">
@@ -13910,7 +13967,7 @@
         <v>5</v>
       </c>
       <c r="I451" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="452" spans="1:9" x14ac:dyDescent="0.3">
@@ -14222,7 +14279,7 @@
         <v>11</v>
       </c>
       <c r="H463" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="464" spans="1:9" x14ac:dyDescent="0.3">
@@ -14300,10 +14357,10 @@
         <v>11</v>
       </c>
       <c r="H466" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="I466" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="467" spans="1:9" x14ac:dyDescent="0.3">
@@ -14355,10 +14412,10 @@
         <v>11</v>
       </c>
       <c r="H468" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="I468" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="469" spans="1:9" x14ac:dyDescent="0.3">
@@ -14670,7 +14727,7 @@
         <v>11</v>
       </c>
       <c r="H480" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="481" spans="1:9" x14ac:dyDescent="0.3">
@@ -14696,7 +14753,7 @@
         <v>11</v>
       </c>
       <c r="H481" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="482" spans="1:9" x14ac:dyDescent="0.3">
@@ -14800,7 +14857,7 @@
         <v>5</v>
       </c>
       <c r="H485" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="486" spans="1:9" x14ac:dyDescent="0.3">
@@ -14930,10 +14987,10 @@
         <v>3</v>
       </c>
       <c r="H490" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="I490" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="491" spans="1:9" x14ac:dyDescent="0.3">
@@ -15349,7 +15406,7 @@
         <v>5</v>
       </c>
       <c r="H506" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="507" spans="1:9" x14ac:dyDescent="0.3">
@@ -15378,7 +15435,7 @@
         <v>5</v>
       </c>
       <c r="I507" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="508" spans="1:9" x14ac:dyDescent="0.3">
@@ -15508,7 +15565,7 @@
         <v>3</v>
       </c>
       <c r="H512" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="513" spans="1:8" x14ac:dyDescent="0.3">
@@ -15586,7 +15643,7 @@
         <v>11</v>
       </c>
       <c r="H515" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="516" spans="1:8" x14ac:dyDescent="0.3">
@@ -28687,5 +28744,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed hypoxanthine/allopurinol annotation after Anitra comment
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59DEF64-D510-41B2-BF59-33624D543E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944F7E34-A0A0-4A2A-89AE-4E29A66D9982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4994" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4997" uniqueCount="506">
   <si>
     <t>Amm</t>
   </si>
@@ -912,9 +912,6 @@
     <t>FT1319</t>
   </si>
   <si>
-    <t>FT1321</t>
-  </si>
-  <si>
     <t>Shifted late in RT</t>
   </si>
   <si>
@@ -1272,9 +1269,6 @@
     <t>FT2034</t>
   </si>
   <si>
-    <t>FT2036</t>
-  </si>
-  <si>
     <t>FT2060</t>
   </si>
   <si>
@@ -1546,6 +1540,9 @@
   </si>
   <si>
     <t>FT4428</t>
+  </si>
+  <si>
+    <t>Peak at 4.2</t>
   </si>
 </sst>
 </file>
@@ -1865,8 +1862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
-      <selection activeCell="I392" sqref="I392"/>
+    <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
+      <selection activeCell="H451" sqref="H451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3204,10 +3201,10 @@
         <v>11</v>
       </c>
       <c r="H48" t="s">
-        <v>294</v>
+        <v>5</v>
       </c>
       <c r="I48" t="s">
-        <v>296</v>
+        <v>505</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -3233,10 +3230,10 @@
         <v>11</v>
       </c>
       <c r="H49" t="s">
+        <v>294</v>
+      </c>
+      <c r="I49" t="s">
         <v>295</v>
-      </c>
-      <c r="I49" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -3262,7 +3259,7 @@
         <v>11</v>
       </c>
       <c r="H50" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -3288,7 +3285,7 @@
         <v>3</v>
       </c>
       <c r="H51" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -3314,10 +3311,10 @@
         <v>11</v>
       </c>
       <c r="H52" t="s">
+        <v>298</v>
+      </c>
+      <c r="I52" t="s">
         <v>299</v>
-      </c>
-      <c r="I52" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -3401,7 +3398,7 @@
         <v>11</v>
       </c>
       <c r="H55" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -3427,7 +3424,7 @@
         <v>3</v>
       </c>
       <c r="H56" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -3453,7 +3450,7 @@
         <v>3</v>
       </c>
       <c r="H57" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -3479,10 +3476,10 @@
         <v>11</v>
       </c>
       <c r="H58" t="s">
+        <v>303</v>
+      </c>
+      <c r="I58" t="s">
         <v>304</v>
-      </c>
-      <c r="I58" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -3508,7 +3505,7 @@
         <v>3</v>
       </c>
       <c r="H59" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
@@ -3592,10 +3589,10 @@
         <v>11</v>
       </c>
       <c r="H62" t="s">
+        <v>306</v>
+      </c>
+      <c r="I62" t="s">
         <v>307</v>
-      </c>
-      <c r="I62" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
@@ -3621,10 +3618,10 @@
         <v>3</v>
       </c>
       <c r="H63" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I63" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -3650,7 +3647,7 @@
         <v>11</v>
       </c>
       <c r="H64" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -3676,7 +3673,7 @@
         <v>3</v>
       </c>
       <c r="H65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -3731,7 +3728,7 @@
         <v>5</v>
       </c>
       <c r="H67" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -3815,7 +3812,7 @@
         <v>11</v>
       </c>
       <c r="H70" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
@@ -3841,7 +3838,7 @@
         <v>11</v>
       </c>
       <c r="H71" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
@@ -3896,7 +3893,7 @@
         <v>3</v>
       </c>
       <c r="H73" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -3922,7 +3919,7 @@
         <v>11</v>
       </c>
       <c r="H74" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -3948,7 +3945,7 @@
         <v>11</v>
       </c>
       <c r="H75" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -3974,10 +3971,10 @@
         <v>5</v>
       </c>
       <c r="H76" t="s">
+        <v>315</v>
+      </c>
+      <c r="I76" t="s">
         <v>316</v>
-      </c>
-      <c r="I76" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
@@ -4003,10 +4000,10 @@
         <v>5</v>
       </c>
       <c r="H77" t="s">
+        <v>315</v>
+      </c>
+      <c r="I77" t="s">
         <v>316</v>
-      </c>
-      <c r="I77" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
@@ -4032,10 +4029,10 @@
         <v>5</v>
       </c>
       <c r="H78" t="s">
+        <v>315</v>
+      </c>
+      <c r="I78" t="s">
         <v>316</v>
-      </c>
-      <c r="I78" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -4061,7 +4058,7 @@
         <v>5</v>
       </c>
       <c r="H79" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
@@ -4087,7 +4084,7 @@
         <v>5</v>
       </c>
       <c r="H80" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -4113,7 +4110,7 @@
         <v>3</v>
       </c>
       <c r="H81" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -4168,10 +4165,10 @@
         <v>3</v>
       </c>
       <c r="H83" t="s">
+        <v>320</v>
+      </c>
+      <c r="I83" t="s">
         <v>321</v>
-      </c>
-      <c r="I83" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
@@ -4200,7 +4197,7 @@
         <v>5</v>
       </c>
       <c r="I84" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
@@ -4258,7 +4255,7 @@
         <v>5</v>
       </c>
       <c r="I86" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
@@ -4313,7 +4310,7 @@
         <v>5</v>
       </c>
       <c r="H88" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
@@ -4339,7 +4336,7 @@
         <v>3</v>
       </c>
       <c r="H89" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
@@ -4394,7 +4391,7 @@
         <v>3</v>
       </c>
       <c r="H91" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
@@ -4420,7 +4417,7 @@
         <v>11</v>
       </c>
       <c r="H92" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
@@ -4475,7 +4472,7 @@
         <v>11</v>
       </c>
       <c r="H94" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
@@ -4530,7 +4527,7 @@
         <v>3</v>
       </c>
       <c r="H96" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -4556,7 +4553,7 @@
         <v>3</v>
       </c>
       <c r="H97" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
@@ -4582,7 +4579,7 @@
         <v>3</v>
       </c>
       <c r="H98" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
@@ -4608,10 +4605,10 @@
         <v>3</v>
       </c>
       <c r="H99" t="s">
+        <v>330</v>
+      </c>
+      <c r="I99" t="s">
         <v>331</v>
-      </c>
-      <c r="I99" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
@@ -4637,7 +4634,7 @@
         <v>11</v>
       </c>
       <c r="H100" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
@@ -4692,7 +4689,7 @@
         <v>3</v>
       </c>
       <c r="H102" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
@@ -4718,7 +4715,7 @@
         <v>11</v>
       </c>
       <c r="H103" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
@@ -4918,7 +4915,7 @@
         <v>5</v>
       </c>
       <c r="H110" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
@@ -5060,7 +5057,7 @@
         <v>11</v>
       </c>
       <c r="H115" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
@@ -5086,7 +5083,7 @@
         <v>5</v>
       </c>
       <c r="H116" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
@@ -5141,7 +5138,7 @@
         <v>5</v>
       </c>
       <c r="H118" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
@@ -5196,7 +5193,7 @@
         <v>11</v>
       </c>
       <c r="H120" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
@@ -5251,7 +5248,7 @@
         <v>3</v>
       </c>
       <c r="H122" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
@@ -5335,7 +5332,7 @@
         <v>11</v>
       </c>
       <c r="H125" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
@@ -5361,7 +5358,7 @@
         <v>5</v>
       </c>
       <c r="H126" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
@@ -5416,7 +5413,7 @@
         <v>11</v>
       </c>
       <c r="H128" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
@@ -5442,7 +5439,7 @@
         <v>11</v>
       </c>
       <c r="H129" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
@@ -5471,7 +5468,7 @@
         <v>5</v>
       </c>
       <c r="I130" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
@@ -5500,7 +5497,7 @@
         <v>5</v>
       </c>
       <c r="I131" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
@@ -5526,7 +5523,7 @@
         <v>5</v>
       </c>
       <c r="H132" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
@@ -5656,10 +5653,10 @@
         <v>5</v>
       </c>
       <c r="H137" t="s">
+        <v>341</v>
+      </c>
+      <c r="I137" t="s">
         <v>342</v>
-      </c>
-      <c r="I137" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
@@ -5711,7 +5708,7 @@
         <v>5</v>
       </c>
       <c r="H139" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
@@ -5815,10 +5812,10 @@
         <v>5</v>
       </c>
       <c r="H143" t="s">
+        <v>344</v>
+      </c>
+      <c r="I143" t="s">
         <v>345</v>
-      </c>
-      <c r="I143" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
@@ -6052,10 +6049,10 @@
         <v>5</v>
       </c>
       <c r="H152" t="s">
+        <v>356</v>
+      </c>
+      <c r="I152" t="s">
         <v>357</v>
-      </c>
-      <c r="I152" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
@@ -6081,7 +6078,7 @@
         <v>5</v>
       </c>
       <c r="H153" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
@@ -6159,7 +6156,7 @@
         <v>5</v>
       </c>
       <c r="I156" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
@@ -6315,7 +6312,7 @@
         <v>3</v>
       </c>
       <c r="I162" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
@@ -6367,7 +6364,7 @@
         <v>3</v>
       </c>
       <c r="H164" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
@@ -6445,7 +6442,7 @@
         <v>11</v>
       </c>
       <c r="H167" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
@@ -6471,7 +6468,7 @@
         <v>11</v>
       </c>
       <c r="H168" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
@@ -6497,7 +6494,7 @@
         <v>11</v>
       </c>
       <c r="H169" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
@@ -6523,7 +6520,7 @@
         <v>3</v>
       </c>
       <c r="I170" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
@@ -6575,7 +6572,7 @@
         <v>5</v>
       </c>
       <c r="H172" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
@@ -6679,10 +6676,10 @@
         <v>3</v>
       </c>
       <c r="H176" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>0</v>
       </c>
@@ -6705,10 +6702,10 @@
         <v>3</v>
       </c>
       <c r="H177" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>0</v>
       </c>
@@ -6731,10 +6728,10 @@
         <v>3</v>
       </c>
       <c r="H178" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>0</v>
       </c>
@@ -6759,8 +6756,11 @@
       <c r="H179" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I179" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>0</v>
       </c>
@@ -6783,10 +6783,10 @@
         <v>11</v>
       </c>
       <c r="H180" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>0</v>
       </c>
@@ -6809,10 +6809,10 @@
         <v>3</v>
       </c>
       <c r="H181" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>0</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>0</v>
       </c>
@@ -6864,7 +6864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>0</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>0</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>0</v>
       </c>
@@ -6939,10 +6939,10 @@
         <v>11</v>
       </c>
       <c r="H186" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>0</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>0</v>
       </c>
@@ -6991,10 +6991,10 @@
         <v>3</v>
       </c>
       <c r="H188" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>0</v>
       </c>
@@ -7020,7 +7020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>0</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>0</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>0</v>
       </c>
@@ -7121,7 +7121,7 @@
         <v>11</v>
       </c>
       <c r="H193" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.3">
@@ -7202,7 +7202,7 @@
         <v>5</v>
       </c>
       <c r="I196" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.3">
@@ -7257,7 +7257,7 @@
         <v>5</v>
       </c>
       <c r="I198" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
@@ -7569,10 +7569,10 @@
         <v>11</v>
       </c>
       <c r="H210" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I210" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
@@ -7702,10 +7702,10 @@
         <v>5</v>
       </c>
       <c r="H215" t="s">
+        <v>375</v>
+      </c>
+      <c r="I215" t="s">
         <v>376</v>
-      </c>
-      <c r="I215" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
@@ -8043,10 +8043,10 @@
         <v>3</v>
       </c>
       <c r="H228" t="s">
+        <v>377</v>
+      </c>
+      <c r="I228" t="s">
         <v>378</v>
-      </c>
-      <c r="I228" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
@@ -8075,7 +8075,7 @@
         <v>5</v>
       </c>
       <c r="I229" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
@@ -8413,7 +8413,7 @@
         <v>3</v>
       </c>
       <c r="H242" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.3">
@@ -9245,10 +9245,10 @@
         <v>3</v>
       </c>
       <c r="H274" t="s">
+        <v>381</v>
+      </c>
+      <c r="I274" t="s">
         <v>382</v>
-      </c>
-      <c r="I274" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.3">
@@ -9300,10 +9300,10 @@
         <v>3</v>
       </c>
       <c r="H276" t="s">
+        <v>383</v>
+      </c>
+      <c r="I276" t="s">
         <v>384</v>
-      </c>
-      <c r="I276" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.3">
@@ -9329,7 +9329,7 @@
         <v>3</v>
       </c>
       <c r="H277" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.3">
@@ -9355,7 +9355,7 @@
         <v>11</v>
       </c>
       <c r="H278" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.3">
@@ -9381,7 +9381,7 @@
         <v>3</v>
       </c>
       <c r="H279" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.3">
@@ -9407,7 +9407,7 @@
         <v>11</v>
       </c>
       <c r="H280" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.3">
@@ -9488,7 +9488,7 @@
         <v>5</v>
       </c>
       <c r="I283" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.3">
@@ -9514,10 +9514,10 @@
         <v>3</v>
       </c>
       <c r="H284" t="s">
+        <v>390</v>
+      </c>
+      <c r="I284" t="s">
         <v>391</v>
-      </c>
-      <c r="I284" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.3">
@@ -9569,7 +9569,7 @@
         <v>11</v>
       </c>
       <c r="H286" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.3">
@@ -9595,10 +9595,10 @@
         <v>3</v>
       </c>
       <c r="H287" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I287" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.3">
@@ -9650,7 +9650,7 @@
         <v>3</v>
       </c>
       <c r="H289" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.3">
@@ -9676,10 +9676,10 @@
         <v>3</v>
       </c>
       <c r="H290" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I290" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.3">
@@ -9705,7 +9705,7 @@
         <v>3</v>
       </c>
       <c r="H291" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.3">
@@ -9757,10 +9757,10 @@
         <v>3</v>
       </c>
       <c r="H293" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I293" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">
@@ -9786,10 +9786,10 @@
         <v>3</v>
       </c>
       <c r="H294" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I294" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.3">
@@ -9815,7 +9815,7 @@
         <v>11</v>
       </c>
       <c r="H295" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.3">
@@ -9896,7 +9896,7 @@
         <v>5</v>
       </c>
       <c r="I298" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.3">
@@ -9948,10 +9948,10 @@
         <v>11</v>
       </c>
       <c r="H300" t="s">
+        <v>400</v>
+      </c>
+      <c r="I300" t="s">
         <v>401</v>
-      </c>
-      <c r="I300" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.3">
@@ -10003,7 +10003,7 @@
         <v>11</v>
       </c>
       <c r="H302" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.3">
@@ -10084,7 +10084,7 @@
         <v>5</v>
       </c>
       <c r="I305" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.3">
@@ -10110,7 +10110,7 @@
         <v>3</v>
       </c>
       <c r="H306" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="307" spans="1:9" x14ac:dyDescent="0.3">
@@ -10136,7 +10136,7 @@
         <v>3</v>
       </c>
       <c r="H307" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.3">
@@ -10162,10 +10162,10 @@
         <v>3</v>
       </c>
       <c r="H308" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I308" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.3">
@@ -10191,10 +10191,10 @@
         <v>3</v>
       </c>
       <c r="H309" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I309" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.3">
@@ -10220,7 +10220,7 @@
         <v>11</v>
       </c>
       <c r="H310" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.3">
@@ -10246,10 +10246,10 @@
         <v>3</v>
       </c>
       <c r="H311" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="I311" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.3">
@@ -10275,10 +10275,10 @@
         <v>3</v>
       </c>
       <c r="H312" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I312" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.3">
@@ -10304,10 +10304,10 @@
         <v>3</v>
       </c>
       <c r="H313" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I313" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="314" spans="1:9" x14ac:dyDescent="0.3">
@@ -10333,7 +10333,7 @@
         <v>11</v>
       </c>
       <c r="H314" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.3">
@@ -10385,7 +10385,7 @@
         <v>11</v>
       </c>
       <c r="H316" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="317" spans="1:9" x14ac:dyDescent="0.3">
@@ -10411,7 +10411,7 @@
         <v>3</v>
       </c>
       <c r="H317" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="318" spans="1:9" x14ac:dyDescent="0.3">
@@ -10437,7 +10437,10 @@
         <v>11</v>
       </c>
       <c r="H318" t="s">
-        <v>414</v>
+        <v>5</v>
+      </c>
+      <c r="I318" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="319" spans="1:9" x14ac:dyDescent="0.3">
@@ -10463,7 +10466,7 @@
         <v>11</v>
       </c>
       <c r="H319" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="320" spans="1:9" x14ac:dyDescent="0.3">
@@ -10489,7 +10492,7 @@
         <v>11</v>
       </c>
       <c r="H320" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.3">
@@ -10515,7 +10518,7 @@
         <v>3</v>
       </c>
       <c r="H321" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="322" spans="1:9" x14ac:dyDescent="0.3">
@@ -10541,10 +10544,10 @@
         <v>11</v>
       </c>
       <c r="H322" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="I322" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.3">
@@ -10622,7 +10625,7 @@
         <v>11</v>
       </c>
       <c r="H325" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.3">
@@ -10648,7 +10651,7 @@
         <v>3</v>
       </c>
       <c r="H326" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.3">
@@ -10674,7 +10677,7 @@
         <v>3</v>
       </c>
       <c r="H327" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.3">
@@ -10703,7 +10706,7 @@
         <v>5</v>
       </c>
       <c r="I328" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.3">
@@ -10729,7 +10732,7 @@
         <v>3</v>
       </c>
       <c r="H329" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.3">
@@ -10755,10 +10758,10 @@
         <v>3</v>
       </c>
       <c r="H330" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="I330" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.3">
@@ -10810,10 +10813,10 @@
         <v>11</v>
       </c>
       <c r="H332" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="I332" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.3">
@@ -10839,10 +10842,10 @@
         <v>3</v>
       </c>
       <c r="H333" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="I333" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.3">
@@ -10868,7 +10871,7 @@
         <v>11</v>
       </c>
       <c r="H334" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.3">
@@ -10894,10 +10897,10 @@
         <v>3</v>
       </c>
       <c r="H335" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="I335" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.3">
@@ -10952,7 +10955,7 @@
         <v>5</v>
       </c>
       <c r="I337" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.3">
@@ -10978,7 +10981,7 @@
         <v>5</v>
       </c>
       <c r="H338" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.3">
@@ -11030,7 +11033,7 @@
         <v>11</v>
       </c>
       <c r="H340" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.3">
@@ -11108,7 +11111,7 @@
         <v>3</v>
       </c>
       <c r="H343" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.3">
@@ -11134,7 +11137,7 @@
         <v>11</v>
       </c>
       <c r="H344" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.3">
@@ -11160,7 +11163,7 @@
         <v>11</v>
       </c>
       <c r="H345" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.3">
@@ -11186,10 +11189,10 @@
         <v>5</v>
       </c>
       <c r="H346" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I346" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.3">
@@ -11267,10 +11270,10 @@
         <v>5</v>
       </c>
       <c r="H349" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I349" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.3">
@@ -11296,7 +11299,7 @@
         <v>5</v>
       </c>
       <c r="H350" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.3">
@@ -11322,7 +11325,7 @@
         <v>3</v>
       </c>
       <c r="H351" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="352" spans="1:9" x14ac:dyDescent="0.3">
@@ -11374,10 +11377,10 @@
         <v>3</v>
       </c>
       <c r="H353" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I353" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="354" spans="1:9" x14ac:dyDescent="0.3">
@@ -11458,7 +11461,7 @@
         <v>5</v>
       </c>
       <c r="I356" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="357" spans="1:9" x14ac:dyDescent="0.3">
@@ -11510,7 +11513,7 @@
         <v>5</v>
       </c>
       <c r="H358" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="359" spans="1:9" x14ac:dyDescent="0.3">
@@ -11536,7 +11539,7 @@
         <v>3</v>
       </c>
       <c r="H359" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.3">
@@ -11588,7 +11591,7 @@
         <v>3</v>
       </c>
       <c r="H361" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.3">
@@ -11614,7 +11617,7 @@
         <v>11</v>
       </c>
       <c r="H362" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.3">
@@ -11666,7 +11669,7 @@
         <v>11</v>
       </c>
       <c r="H364" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.3">
@@ -11695,7 +11698,7 @@
         <v>5</v>
       </c>
       <c r="I365" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.3">
@@ -11721,10 +11724,10 @@
         <v>3</v>
       </c>
       <c r="H366" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="I366" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="367" spans="1:9" x14ac:dyDescent="0.3">
@@ -11750,7 +11753,7 @@
         <v>3</v>
       </c>
       <c r="H367" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="368" spans="1:9" x14ac:dyDescent="0.3">
@@ -11776,7 +11779,7 @@
         <v>3</v>
       </c>
       <c r="H368" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="369" spans="1:9" x14ac:dyDescent="0.3">
@@ -11802,10 +11805,10 @@
         <v>3</v>
       </c>
       <c r="H369" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="I369" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="370" spans="1:9" x14ac:dyDescent="0.3">
@@ -11831,10 +11834,10 @@
         <v>11</v>
       </c>
       <c r="H370" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="I370" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="371" spans="1:9" x14ac:dyDescent="0.3">
@@ -11863,7 +11866,7 @@
         <v>5</v>
       </c>
       <c r="I371" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="372" spans="1:9" x14ac:dyDescent="0.3">
@@ -11889,7 +11892,7 @@
         <v>3</v>
       </c>
       <c r="H372" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="373" spans="1:9" x14ac:dyDescent="0.3">
@@ -12097,7 +12100,7 @@
         <v>5</v>
       </c>
       <c r="H380" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="381" spans="1:9" x14ac:dyDescent="0.3">
@@ -12227,7 +12230,7 @@
         <v>11</v>
       </c>
       <c r="H385" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="386" spans="1:9" x14ac:dyDescent="0.3">
@@ -12253,7 +12256,7 @@
         <v>5</v>
       </c>
       <c r="H386" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="387" spans="1:9" x14ac:dyDescent="0.3">
@@ -12305,7 +12308,7 @@
         <v>5</v>
       </c>
       <c r="H388" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="389" spans="1:9" x14ac:dyDescent="0.3">
@@ -12331,7 +12334,7 @@
         <v>3</v>
       </c>
       <c r="H389" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="390" spans="1:9" x14ac:dyDescent="0.3">
@@ -12357,7 +12360,7 @@
         <v>11</v>
       </c>
       <c r="H390" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="391" spans="1:9" x14ac:dyDescent="0.3">
@@ -12383,10 +12386,10 @@
         <v>11</v>
       </c>
       <c r="H391" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="I391" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="392" spans="1:9" x14ac:dyDescent="0.3">
@@ -12412,7 +12415,7 @@
         <v>3</v>
       </c>
       <c r="H392" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="393" spans="1:9" x14ac:dyDescent="0.3">
@@ -12490,7 +12493,7 @@
         <v>11</v>
       </c>
       <c r="H395" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="396" spans="1:9" x14ac:dyDescent="0.3">
@@ -12516,7 +12519,7 @@
         <v>5</v>
       </c>
       <c r="H396" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="397" spans="1:9" x14ac:dyDescent="0.3">
@@ -12568,7 +12571,7 @@
         <v>11</v>
       </c>
       <c r="H398" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="399" spans="1:9" x14ac:dyDescent="0.3">
@@ -12594,7 +12597,7 @@
         <v>11</v>
       </c>
       <c r="H399" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="400" spans="1:9" x14ac:dyDescent="0.3">
@@ -12620,7 +12623,7 @@
         <v>5</v>
       </c>
       <c r="H400" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="401" spans="1:9" x14ac:dyDescent="0.3">
@@ -12646,7 +12649,7 @@
         <v>5</v>
       </c>
       <c r="H401" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="402" spans="1:9" x14ac:dyDescent="0.3">
@@ -12802,7 +12805,7 @@
         <v>5</v>
       </c>
       <c r="H407" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="408" spans="1:9" x14ac:dyDescent="0.3">
@@ -12854,7 +12857,7 @@
         <v>5</v>
       </c>
       <c r="H409" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="410" spans="1:9" x14ac:dyDescent="0.3">
@@ -12880,10 +12883,10 @@
         <v>5</v>
       </c>
       <c r="H410" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I410" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="411" spans="1:9" x14ac:dyDescent="0.3">
@@ -12961,7 +12964,7 @@
         <v>5</v>
       </c>
       <c r="H413" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="414" spans="1:9" x14ac:dyDescent="0.3">
@@ -13195,10 +13198,10 @@
         <v>5</v>
       </c>
       <c r="H422" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="I422" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="423" spans="1:9" x14ac:dyDescent="0.3">
@@ -13224,7 +13227,7 @@
         <v>5</v>
       </c>
       <c r="H423" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="424" spans="1:9" x14ac:dyDescent="0.3">
@@ -13305,7 +13308,7 @@
         <v>5</v>
       </c>
       <c r="I426" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="427" spans="1:9" x14ac:dyDescent="0.3">
@@ -13409,7 +13412,7 @@
         <v>11</v>
       </c>
       <c r="H430" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="431" spans="1:9" x14ac:dyDescent="0.3">
@@ -13461,7 +13464,7 @@
         <v>3</v>
       </c>
       <c r="H432" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="433" spans="1:9" x14ac:dyDescent="0.3">
@@ -13513,7 +13516,7 @@
         <v>3</v>
       </c>
       <c r="H434" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="435" spans="1:9" x14ac:dyDescent="0.3">
@@ -13591,10 +13594,10 @@
         <v>11</v>
       </c>
       <c r="H437" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="I437" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="438" spans="1:9" x14ac:dyDescent="0.3">
@@ -13620,10 +13623,10 @@
         <v>11</v>
       </c>
       <c r="H438" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I438" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="439" spans="1:9" x14ac:dyDescent="0.3">
@@ -13649,7 +13652,7 @@
         <v>11</v>
       </c>
       <c r="H439" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="440" spans="1:9" x14ac:dyDescent="0.3">
@@ -13678,7 +13681,7 @@
         <v>5</v>
       </c>
       <c r="I440" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="441" spans="1:9" x14ac:dyDescent="0.3">
@@ -13730,7 +13733,7 @@
         <v>5</v>
       </c>
       <c r="I442" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="443" spans="1:9" x14ac:dyDescent="0.3">
@@ -13834,7 +13837,7 @@
         <v>3</v>
       </c>
       <c r="H446" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="447" spans="1:9" x14ac:dyDescent="0.3">
@@ -13860,7 +13863,7 @@
         <v>3</v>
       </c>
       <c r="H447" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="448" spans="1:9" x14ac:dyDescent="0.3">
@@ -13886,7 +13889,7 @@
         <v>3</v>
       </c>
       <c r="H448" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="449" spans="1:9" x14ac:dyDescent="0.3">
@@ -13912,7 +13915,10 @@
         <v>11</v>
       </c>
       <c r="H449" t="s">
-        <v>480</v>
+        <v>5</v>
+      </c>
+      <c r="I449" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="450" spans="1:9" x14ac:dyDescent="0.3">
@@ -13938,7 +13944,7 @@
         <v>11</v>
       </c>
       <c r="H450" t="s">
-        <v>5</v>
+        <v>478</v>
       </c>
     </row>
     <row r="451" spans="1:9" x14ac:dyDescent="0.3">
@@ -13967,7 +13973,7 @@
         <v>5</v>
       </c>
       <c r="I451" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="452" spans="1:9" x14ac:dyDescent="0.3">
@@ -14279,7 +14285,7 @@
         <v>11</v>
       </c>
       <c r="H463" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="464" spans="1:9" x14ac:dyDescent="0.3">
@@ -14357,10 +14363,10 @@
         <v>11</v>
       </c>
       <c r="H466" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I466" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="467" spans="1:9" x14ac:dyDescent="0.3">
@@ -14412,10 +14418,10 @@
         <v>11</v>
       </c>
       <c r="H468" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I468" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="469" spans="1:9" x14ac:dyDescent="0.3">
@@ -14727,7 +14733,7 @@
         <v>11</v>
       </c>
       <c r="H480" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="481" spans="1:9" x14ac:dyDescent="0.3">
@@ -14753,7 +14759,7 @@
         <v>11</v>
       </c>
       <c r="H481" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="482" spans="1:9" x14ac:dyDescent="0.3">
@@ -14857,7 +14863,7 @@
         <v>5</v>
       </c>
       <c r="H485" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="486" spans="1:9" x14ac:dyDescent="0.3">
@@ -14987,10 +14993,10 @@
         <v>3</v>
       </c>
       <c r="H490" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="I490" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="491" spans="1:9" x14ac:dyDescent="0.3">
@@ -15406,7 +15412,7 @@
         <v>5</v>
       </c>
       <c r="H506" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="507" spans="1:9" x14ac:dyDescent="0.3">
@@ -15435,7 +15441,7 @@
         <v>5</v>
       </c>
       <c r="I507" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="508" spans="1:9" x14ac:dyDescent="0.3">
@@ -15565,7 +15571,7 @@
         <v>3</v>
       </c>
       <c r="H512" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="513" spans="1:8" x14ac:dyDescent="0.3">
@@ -15643,7 +15649,7 @@
         <v>11</v>
       </c>
       <c r="H515" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="516" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Deciding we don't see beta-Glu and just calling it Glu
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944F7E34-A0A0-4A2A-89AE-4E29A66D9982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECD1AE0-858D-455A-B822-FD87753D1757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1044" yWindow="2112" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4997" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4997" uniqueCount="505">
   <si>
     <t>Amm</t>
   </si>
@@ -946,9 +946,6 @@
   </si>
   <si>
     <t>FT1635</t>
-  </si>
-  <si>
-    <t>Combined with Glu</t>
   </si>
   <si>
     <t>Combined with beta-Glu</t>
@@ -1862,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
-      <selection activeCell="H451" sqref="H451"/>
+    <sheetView tabSelected="1" topLeftCell="A594" workbookViewId="0">
+      <selection activeCell="K603" sqref="K603"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3204,7 +3201,7 @@
         <v>5</v>
       </c>
       <c r="I48" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -3589,10 +3586,10 @@
         <v>11</v>
       </c>
       <c r="H62" t="s">
-        <v>306</v>
+        <v>5</v>
       </c>
       <c r="I62" t="s">
-        <v>307</v>
+        <v>256</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
@@ -3621,7 +3618,7 @@
         <v>306</v>
       </c>
       <c r="I63" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -3647,7 +3644,7 @@
         <v>11</v>
       </c>
       <c r="H64" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -3673,7 +3670,7 @@
         <v>3</v>
       </c>
       <c r="H65" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -3728,7 +3725,7 @@
         <v>5</v>
       </c>
       <c r="H67" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -3812,7 +3809,7 @@
         <v>11</v>
       </c>
       <c r="H70" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
@@ -3838,7 +3835,7 @@
         <v>11</v>
       </c>
       <c r="H71" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
@@ -3893,7 +3890,7 @@
         <v>3</v>
       </c>
       <c r="H73" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -3919,7 +3916,7 @@
         <v>11</v>
       </c>
       <c r="H74" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -3945,7 +3942,7 @@
         <v>11</v>
       </c>
       <c r="H75" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -3971,10 +3968,10 @@
         <v>5</v>
       </c>
       <c r="H76" t="s">
+        <v>314</v>
+      </c>
+      <c r="I76" t="s">
         <v>315</v>
-      </c>
-      <c r="I76" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
@@ -4000,10 +3997,10 @@
         <v>5</v>
       </c>
       <c r="H77" t="s">
+        <v>314</v>
+      </c>
+      <c r="I77" t="s">
         <v>315</v>
-      </c>
-      <c r="I77" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
@@ -4029,10 +4026,10 @@
         <v>5</v>
       </c>
       <c r="H78" t="s">
+        <v>314</v>
+      </c>
+      <c r="I78" t="s">
         <v>315</v>
-      </c>
-      <c r="I78" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -4058,7 +4055,7 @@
         <v>5</v>
       </c>
       <c r="H79" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
@@ -4084,7 +4081,7 @@
         <v>5</v>
       </c>
       <c r="H80" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -4110,7 +4107,7 @@
         <v>3</v>
       </c>
       <c r="H81" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -4165,10 +4162,10 @@
         <v>3</v>
       </c>
       <c r="H83" t="s">
+        <v>319</v>
+      </c>
+      <c r="I83" t="s">
         <v>320</v>
-      </c>
-      <c r="I83" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
@@ -4197,7 +4194,7 @@
         <v>5</v>
       </c>
       <c r="I84" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
@@ -4255,7 +4252,7 @@
         <v>5</v>
       </c>
       <c r="I86" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
@@ -4310,7 +4307,7 @@
         <v>5</v>
       </c>
       <c r="H88" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
@@ -4336,7 +4333,7 @@
         <v>3</v>
       </c>
       <c r="H89" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
@@ -4391,7 +4388,7 @@
         <v>3</v>
       </c>
       <c r="H91" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
@@ -4417,7 +4414,7 @@
         <v>11</v>
       </c>
       <c r="H92" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
@@ -4472,7 +4469,7 @@
         <v>11</v>
       </c>
       <c r="H94" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
@@ -4527,7 +4524,7 @@
         <v>3</v>
       </c>
       <c r="H96" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -4553,7 +4550,7 @@
         <v>3</v>
       </c>
       <c r="H97" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
@@ -4579,7 +4576,7 @@
         <v>3</v>
       </c>
       <c r="H98" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
@@ -4605,10 +4602,10 @@
         <v>3</v>
       </c>
       <c r="H99" t="s">
+        <v>329</v>
+      </c>
+      <c r="I99" t="s">
         <v>330</v>
-      </c>
-      <c r="I99" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
@@ -4634,7 +4631,7 @@
         <v>11</v>
       </c>
       <c r="H100" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
@@ -4689,7 +4686,7 @@
         <v>3</v>
       </c>
       <c r="H102" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
@@ -4715,7 +4712,7 @@
         <v>11</v>
       </c>
       <c r="H103" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
@@ -4915,7 +4912,7 @@
         <v>5</v>
       </c>
       <c r="H110" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
@@ -5057,7 +5054,7 @@
         <v>11</v>
       </c>
       <c r="H115" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
@@ -5083,7 +5080,7 @@
         <v>5</v>
       </c>
       <c r="H116" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
@@ -5138,7 +5135,7 @@
         <v>5</v>
       </c>
       <c r="H118" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
@@ -5193,7 +5190,7 @@
         <v>11</v>
       </c>
       <c r="H120" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
@@ -5248,7 +5245,7 @@
         <v>3</v>
       </c>
       <c r="H122" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
@@ -5332,7 +5329,7 @@
         <v>11</v>
       </c>
       <c r="H125" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
@@ -5358,7 +5355,7 @@
         <v>5</v>
       </c>
       <c r="H126" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
@@ -5413,7 +5410,7 @@
         <v>11</v>
       </c>
       <c r="H128" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
@@ -5439,7 +5436,7 @@
         <v>11</v>
       </c>
       <c r="H129" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
@@ -5468,7 +5465,7 @@
         <v>5</v>
       </c>
       <c r="I130" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
@@ -5497,7 +5494,7 @@
         <v>5</v>
       </c>
       <c r="I131" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
@@ -5523,7 +5520,7 @@
         <v>5</v>
       </c>
       <c r="H132" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
@@ -5653,10 +5650,10 @@
         <v>5</v>
       </c>
       <c r="H137" t="s">
+        <v>340</v>
+      </c>
+      <c r="I137" t="s">
         <v>341</v>
-      </c>
-      <c r="I137" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
@@ -5708,7 +5705,7 @@
         <v>5</v>
       </c>
       <c r="H139" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
@@ -5812,10 +5809,10 @@
         <v>5</v>
       </c>
       <c r="H143" t="s">
+        <v>343</v>
+      </c>
+      <c r="I143" t="s">
         <v>344</v>
-      </c>
-      <c r="I143" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
@@ -6049,10 +6046,10 @@
         <v>5</v>
       </c>
       <c r="H152" t="s">
+        <v>355</v>
+      </c>
+      <c r="I152" t="s">
         <v>356</v>
-      </c>
-      <c r="I152" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
@@ -6078,7 +6075,7 @@
         <v>5</v>
       </c>
       <c r="H153" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
@@ -6156,7 +6153,7 @@
         <v>5</v>
       </c>
       <c r="I156" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
@@ -6312,7 +6309,7 @@
         <v>3</v>
       </c>
       <c r="I162" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
@@ -6364,7 +6361,7 @@
         <v>3</v>
       </c>
       <c r="H164" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
@@ -6442,7 +6439,7 @@
         <v>11</v>
       </c>
       <c r="H167" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
@@ -6468,7 +6465,7 @@
         <v>11</v>
       </c>
       <c r="H168" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
@@ -6494,7 +6491,7 @@
         <v>11</v>
       </c>
       <c r="H169" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
@@ -6520,7 +6517,7 @@
         <v>3</v>
       </c>
       <c r="I170" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
@@ -6572,7 +6569,7 @@
         <v>5</v>
       </c>
       <c r="H172" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
@@ -6676,7 +6673,7 @@
         <v>3</v>
       </c>
       <c r="H176" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
@@ -6702,7 +6699,7 @@
         <v>3</v>
       </c>
       <c r="H177" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.3">
@@ -6728,7 +6725,7 @@
         <v>3</v>
       </c>
       <c r="H178" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
@@ -6757,7 +6754,7 @@
         <v>5</v>
       </c>
       <c r="I179" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.3">
@@ -6783,7 +6780,7 @@
         <v>11</v>
       </c>
       <c r="H180" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.3">
@@ -6809,7 +6806,7 @@
         <v>3</v>
       </c>
       <c r="H181" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
@@ -6939,7 +6936,7 @@
         <v>11</v>
       </c>
       <c r="H186" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
@@ -6991,7 +6988,7 @@
         <v>3</v>
       </c>
       <c r="H188" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
@@ -7121,7 +7118,7 @@
         <v>11</v>
       </c>
       <c r="H193" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.3">
@@ -7202,7 +7199,7 @@
         <v>5</v>
       </c>
       <c r="I196" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.3">
@@ -7257,7 +7254,7 @@
         <v>5</v>
       </c>
       <c r="I198" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
@@ -7569,10 +7566,10 @@
         <v>11</v>
       </c>
       <c r="H210" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I210" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
@@ -7702,10 +7699,10 @@
         <v>5</v>
       </c>
       <c r="H215" t="s">
+        <v>374</v>
+      </c>
+      <c r="I215" t="s">
         <v>375</v>
-      </c>
-      <c r="I215" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
@@ -8043,10 +8040,10 @@
         <v>3</v>
       </c>
       <c r="H228" t="s">
+        <v>376</v>
+      </c>
+      <c r="I228" t="s">
         <v>377</v>
-      </c>
-      <c r="I228" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
@@ -8075,7 +8072,7 @@
         <v>5</v>
       </c>
       <c r="I229" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
@@ -8413,7 +8410,7 @@
         <v>3</v>
       </c>
       <c r="H242" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.3">
@@ -9245,10 +9242,10 @@
         <v>3</v>
       </c>
       <c r="H274" t="s">
+        <v>380</v>
+      </c>
+      <c r="I274" t="s">
         <v>381</v>
-      </c>
-      <c r="I274" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.3">
@@ -9300,10 +9297,10 @@
         <v>3</v>
       </c>
       <c r="H276" t="s">
+        <v>382</v>
+      </c>
+      <c r="I276" t="s">
         <v>383</v>
-      </c>
-      <c r="I276" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.3">
@@ -9329,7 +9326,7 @@
         <v>3</v>
       </c>
       <c r="H277" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.3">
@@ -9355,7 +9352,7 @@
         <v>11</v>
       </c>
       <c r="H278" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.3">
@@ -9381,7 +9378,7 @@
         <v>3</v>
       </c>
       <c r="H279" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.3">
@@ -9407,7 +9404,7 @@
         <v>11</v>
       </c>
       <c r="H280" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.3">
@@ -9488,7 +9485,7 @@
         <v>5</v>
       </c>
       <c r="I283" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.3">
@@ -9514,10 +9511,10 @@
         <v>3</v>
       </c>
       <c r="H284" t="s">
+        <v>389</v>
+      </c>
+      <c r="I284" t="s">
         <v>390</v>
-      </c>
-      <c r="I284" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.3">
@@ -9569,7 +9566,7 @@
         <v>11</v>
       </c>
       <c r="H286" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.3">
@@ -9595,10 +9592,10 @@
         <v>3</v>
       </c>
       <c r="H287" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I287" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.3">
@@ -9650,7 +9647,7 @@
         <v>3</v>
       </c>
       <c r="H289" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.3">
@@ -9676,10 +9673,10 @@
         <v>3</v>
       </c>
       <c r="H290" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I290" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.3">
@@ -9705,7 +9702,7 @@
         <v>3</v>
       </c>
       <c r="H291" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.3">
@@ -9757,10 +9754,10 @@
         <v>3</v>
       </c>
       <c r="H293" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I293" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">
@@ -9786,10 +9783,10 @@
         <v>3</v>
       </c>
       <c r="H294" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I294" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.3">
@@ -9815,7 +9812,7 @@
         <v>11</v>
       </c>
       <c r="H295" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.3">
@@ -9896,7 +9893,7 @@
         <v>5</v>
       </c>
       <c r="I298" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.3">
@@ -9948,10 +9945,10 @@
         <v>11</v>
       </c>
       <c r="H300" t="s">
+        <v>399</v>
+      </c>
+      <c r="I300" t="s">
         <v>400</v>
-      </c>
-      <c r="I300" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.3">
@@ -10003,7 +10000,7 @@
         <v>11</v>
       </c>
       <c r="H302" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.3">
@@ -10084,7 +10081,7 @@
         <v>5</v>
       </c>
       <c r="I305" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.3">
@@ -10110,7 +10107,7 @@
         <v>3</v>
       </c>
       <c r="H306" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="307" spans="1:9" x14ac:dyDescent="0.3">
@@ -10136,7 +10133,7 @@
         <v>3</v>
       </c>
       <c r="H307" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.3">
@@ -10162,10 +10159,10 @@
         <v>3</v>
       </c>
       <c r="H308" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I308" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.3">
@@ -10191,10 +10188,10 @@
         <v>3</v>
       </c>
       <c r="H309" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I309" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.3">
@@ -10220,7 +10217,7 @@
         <v>11</v>
       </c>
       <c r="H310" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.3">
@@ -10246,10 +10243,10 @@
         <v>3</v>
       </c>
       <c r="H311" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I311" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.3">
@@ -10275,10 +10272,10 @@
         <v>3</v>
       </c>
       <c r="H312" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I312" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.3">
@@ -10304,10 +10301,10 @@
         <v>3</v>
       </c>
       <c r="H313" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="I313" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="314" spans="1:9" x14ac:dyDescent="0.3">
@@ -10333,7 +10330,7 @@
         <v>11</v>
       </c>
       <c r="H314" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.3">
@@ -10385,7 +10382,7 @@
         <v>11</v>
       </c>
       <c r="H316" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="317" spans="1:9" x14ac:dyDescent="0.3">
@@ -10411,7 +10408,7 @@
         <v>3</v>
       </c>
       <c r="H317" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="318" spans="1:9" x14ac:dyDescent="0.3">
@@ -10440,7 +10437,7 @@
         <v>5</v>
       </c>
       <c r="I318" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="319" spans="1:9" x14ac:dyDescent="0.3">
@@ -10466,7 +10463,7 @@
         <v>11</v>
       </c>
       <c r="H319" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="320" spans="1:9" x14ac:dyDescent="0.3">
@@ -10492,7 +10489,7 @@
         <v>11</v>
       </c>
       <c r="H320" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.3">
@@ -10518,7 +10515,7 @@
         <v>3</v>
       </c>
       <c r="H321" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="322" spans="1:9" x14ac:dyDescent="0.3">
@@ -10544,10 +10541,10 @@
         <v>11</v>
       </c>
       <c r="H322" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I322" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.3">
@@ -10625,7 +10622,7 @@
         <v>11</v>
       </c>
       <c r="H325" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.3">
@@ -10651,7 +10648,7 @@
         <v>3</v>
       </c>
       <c r="H326" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.3">
@@ -10677,7 +10674,7 @@
         <v>3</v>
       </c>
       <c r="H327" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.3">
@@ -10706,7 +10703,7 @@
         <v>5</v>
       </c>
       <c r="I328" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.3">
@@ -10732,7 +10729,7 @@
         <v>3</v>
       </c>
       <c r="H329" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.3">
@@ -10758,10 +10755,10 @@
         <v>3</v>
       </c>
       <c r="H330" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I330" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.3">
@@ -10813,10 +10810,10 @@
         <v>11</v>
       </c>
       <c r="H332" t="s">
-        <v>422</v>
+        <v>5</v>
       </c>
       <c r="I332" t="s">
-        <v>401</v>
+        <v>256</v>
       </c>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.3">
@@ -10842,10 +10839,10 @@
         <v>3</v>
       </c>
       <c r="H333" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I333" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.3">
@@ -10871,7 +10868,7 @@
         <v>11</v>
       </c>
       <c r="H334" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.3">
@@ -10897,10 +10894,10 @@
         <v>3</v>
       </c>
       <c r="H335" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="I335" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.3">
@@ -10955,7 +10952,7 @@
         <v>5</v>
       </c>
       <c r="I337" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.3">
@@ -10981,7 +10978,7 @@
         <v>5</v>
       </c>
       <c r="H338" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.3">
@@ -11033,7 +11030,7 @@
         <v>11</v>
       </c>
       <c r="H340" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.3">
@@ -11111,7 +11108,7 @@
         <v>3</v>
       </c>
       <c r="H343" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.3">
@@ -11137,7 +11134,7 @@
         <v>11</v>
       </c>
       <c r="H344" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.3">
@@ -11163,7 +11160,7 @@
         <v>11</v>
       </c>
       <c r="H345" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.3">
@@ -11189,10 +11186,10 @@
         <v>5</v>
       </c>
       <c r="H346" t="s">
+        <v>429</v>
+      </c>
+      <c r="I346" t="s">
         <v>430</v>
-      </c>
-      <c r="I346" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.3">
@@ -11270,10 +11267,10 @@
         <v>5</v>
       </c>
       <c r="H349" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I349" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.3">
@@ -11299,7 +11296,7 @@
         <v>5</v>
       </c>
       <c r="H350" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.3">
@@ -11325,7 +11322,7 @@
         <v>3</v>
       </c>
       <c r="H351" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="352" spans="1:9" x14ac:dyDescent="0.3">
@@ -11377,10 +11374,10 @@
         <v>3</v>
       </c>
       <c r="H353" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I353" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="354" spans="1:9" x14ac:dyDescent="0.3">
@@ -11461,7 +11458,7 @@
         <v>5</v>
       </c>
       <c r="I356" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="357" spans="1:9" x14ac:dyDescent="0.3">
@@ -11513,7 +11510,7 @@
         <v>5</v>
       </c>
       <c r="H358" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="359" spans="1:9" x14ac:dyDescent="0.3">
@@ -11539,7 +11536,7 @@
         <v>3</v>
       </c>
       <c r="H359" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.3">
@@ -11591,7 +11588,7 @@
         <v>3</v>
       </c>
       <c r="H361" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.3">
@@ -11617,7 +11614,7 @@
         <v>11</v>
       </c>
       <c r="H362" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.3">
@@ -11669,7 +11666,7 @@
         <v>11</v>
       </c>
       <c r="H364" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.3">
@@ -11698,7 +11695,7 @@
         <v>5</v>
       </c>
       <c r="I365" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.3">
@@ -11724,10 +11721,10 @@
         <v>3</v>
       </c>
       <c r="H366" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I366" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="367" spans="1:9" x14ac:dyDescent="0.3">
@@ -11753,7 +11750,7 @@
         <v>3</v>
       </c>
       <c r="H367" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="368" spans="1:9" x14ac:dyDescent="0.3">
@@ -11779,7 +11776,7 @@
         <v>3</v>
       </c>
       <c r="H368" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="369" spans="1:9" x14ac:dyDescent="0.3">
@@ -11805,10 +11802,10 @@
         <v>3</v>
       </c>
       <c r="H369" t="s">
+        <v>443</v>
+      </c>
+      <c r="I369" t="s">
         <v>444</v>
-      </c>
-      <c r="I369" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="370" spans="1:9" x14ac:dyDescent="0.3">
@@ -11834,10 +11831,10 @@
         <v>11</v>
       </c>
       <c r="H370" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I370" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="371" spans="1:9" x14ac:dyDescent="0.3">
@@ -11866,7 +11863,7 @@
         <v>5</v>
       </c>
       <c r="I371" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="372" spans="1:9" x14ac:dyDescent="0.3">
@@ -11892,7 +11889,7 @@
         <v>3</v>
       </c>
       <c r="H372" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="373" spans="1:9" x14ac:dyDescent="0.3">
@@ -12100,7 +12097,7 @@
         <v>5</v>
       </c>
       <c r="H380" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="381" spans="1:9" x14ac:dyDescent="0.3">
@@ -12230,7 +12227,7 @@
         <v>11</v>
       </c>
       <c r="H385" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="386" spans="1:9" x14ac:dyDescent="0.3">
@@ -12256,7 +12253,7 @@
         <v>5</v>
       </c>
       <c r="H386" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="387" spans="1:9" x14ac:dyDescent="0.3">
@@ -12308,7 +12305,7 @@
         <v>5</v>
       </c>
       <c r="H388" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="389" spans="1:9" x14ac:dyDescent="0.3">
@@ -12334,7 +12331,7 @@
         <v>3</v>
       </c>
       <c r="H389" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="390" spans="1:9" x14ac:dyDescent="0.3">
@@ -12360,7 +12357,7 @@
         <v>11</v>
       </c>
       <c r="H390" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="391" spans="1:9" x14ac:dyDescent="0.3">
@@ -12386,10 +12383,10 @@
         <v>11</v>
       </c>
       <c r="H391" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I391" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="392" spans="1:9" x14ac:dyDescent="0.3">
@@ -12415,7 +12412,7 @@
         <v>3</v>
       </c>
       <c r="H392" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="393" spans="1:9" x14ac:dyDescent="0.3">
@@ -12493,7 +12490,7 @@
         <v>11</v>
       </c>
       <c r="H395" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="396" spans="1:9" x14ac:dyDescent="0.3">
@@ -12519,7 +12516,7 @@
         <v>5</v>
       </c>
       <c r="H396" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="397" spans="1:9" x14ac:dyDescent="0.3">
@@ -12571,7 +12568,7 @@
         <v>11</v>
       </c>
       <c r="H398" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="399" spans="1:9" x14ac:dyDescent="0.3">
@@ -12597,7 +12594,7 @@
         <v>11</v>
       </c>
       <c r="H399" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="400" spans="1:9" x14ac:dyDescent="0.3">
@@ -12623,7 +12620,7 @@
         <v>5</v>
       </c>
       <c r="H400" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="401" spans="1:9" x14ac:dyDescent="0.3">
@@ -12649,7 +12646,7 @@
         <v>5</v>
       </c>
       <c r="H401" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="402" spans="1:9" x14ac:dyDescent="0.3">
@@ -12805,7 +12802,7 @@
         <v>5</v>
       </c>
       <c r="H407" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="408" spans="1:9" x14ac:dyDescent="0.3">
@@ -12857,7 +12854,7 @@
         <v>5</v>
       </c>
       <c r="H409" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="410" spans="1:9" x14ac:dyDescent="0.3">
@@ -12883,10 +12880,10 @@
         <v>5</v>
       </c>
       <c r="H410" t="s">
+        <v>460</v>
+      </c>
+      <c r="I410" t="s">
         <v>461</v>
-      </c>
-      <c r="I410" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="411" spans="1:9" x14ac:dyDescent="0.3">
@@ -12964,7 +12961,7 @@
         <v>5</v>
       </c>
       <c r="H413" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="414" spans="1:9" x14ac:dyDescent="0.3">
@@ -13198,10 +13195,10 @@
         <v>5</v>
       </c>
       <c r="H422" t="s">
+        <v>463</v>
+      </c>
+      <c r="I422" t="s">
         <v>464</v>
-      </c>
-      <c r="I422" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="423" spans="1:9" x14ac:dyDescent="0.3">
@@ -13227,7 +13224,7 @@
         <v>5</v>
       </c>
       <c r="H423" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="424" spans="1:9" x14ac:dyDescent="0.3">
@@ -13308,7 +13305,7 @@
         <v>5</v>
       </c>
       <c r="I426" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="427" spans="1:9" x14ac:dyDescent="0.3">
@@ -13412,7 +13409,7 @@
         <v>11</v>
       </c>
       <c r="H430" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="431" spans="1:9" x14ac:dyDescent="0.3">
@@ -13464,7 +13461,7 @@
         <v>3</v>
       </c>
       <c r="H432" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="433" spans="1:9" x14ac:dyDescent="0.3">
@@ -13516,7 +13513,7 @@
         <v>3</v>
       </c>
       <c r="H434" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="435" spans="1:9" x14ac:dyDescent="0.3">
@@ -13594,10 +13591,10 @@
         <v>11</v>
       </c>
       <c r="H437" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I437" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="438" spans="1:9" x14ac:dyDescent="0.3">
@@ -13623,10 +13620,10 @@
         <v>11</v>
       </c>
       <c r="H438" t="s">
+        <v>470</v>
+      </c>
+      <c r="I438" t="s">
         <v>471</v>
-      </c>
-      <c r="I438" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="439" spans="1:9" x14ac:dyDescent="0.3">
@@ -13652,7 +13649,7 @@
         <v>11</v>
       </c>
       <c r="H439" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="440" spans="1:9" x14ac:dyDescent="0.3">
@@ -13681,7 +13678,7 @@
         <v>5</v>
       </c>
       <c r="I440" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="441" spans="1:9" x14ac:dyDescent="0.3">
@@ -13733,7 +13730,7 @@
         <v>5</v>
       </c>
       <c r="I442" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="443" spans="1:9" x14ac:dyDescent="0.3">
@@ -13837,7 +13834,7 @@
         <v>3</v>
       </c>
       <c r="H446" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="447" spans="1:9" x14ac:dyDescent="0.3">
@@ -13863,7 +13860,7 @@
         <v>3</v>
       </c>
       <c r="H447" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="448" spans="1:9" x14ac:dyDescent="0.3">
@@ -13889,7 +13886,7 @@
         <v>3</v>
       </c>
       <c r="H448" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="449" spans="1:9" x14ac:dyDescent="0.3">
@@ -13918,7 +13915,7 @@
         <v>5</v>
       </c>
       <c r="I449" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="450" spans="1:9" x14ac:dyDescent="0.3">
@@ -13944,7 +13941,7 @@
         <v>11</v>
       </c>
       <c r="H450" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="451" spans="1:9" x14ac:dyDescent="0.3">
@@ -13973,7 +13970,7 @@
         <v>5</v>
       </c>
       <c r="I451" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="452" spans="1:9" x14ac:dyDescent="0.3">
@@ -14285,7 +14282,7 @@
         <v>11</v>
       </c>
       <c r="H463" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="464" spans="1:9" x14ac:dyDescent="0.3">
@@ -14363,10 +14360,10 @@
         <v>11</v>
       </c>
       <c r="H466" t="s">
+        <v>479</v>
+      </c>
+      <c r="I466" t="s">
         <v>480</v>
-      </c>
-      <c r="I466" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="467" spans="1:9" x14ac:dyDescent="0.3">
@@ -14418,10 +14415,10 @@
         <v>11</v>
       </c>
       <c r="H468" t="s">
+        <v>481</v>
+      </c>
+      <c r="I468" t="s">
         <v>482</v>
-      </c>
-      <c r="I468" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="469" spans="1:9" x14ac:dyDescent="0.3">
@@ -14733,7 +14730,7 @@
         <v>11</v>
       </c>
       <c r="H480" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="481" spans="1:9" x14ac:dyDescent="0.3">
@@ -14759,7 +14756,7 @@
         <v>11</v>
       </c>
       <c r="H481" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="482" spans="1:9" x14ac:dyDescent="0.3">
@@ -14863,7 +14860,7 @@
         <v>5</v>
       </c>
       <c r="H485" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="486" spans="1:9" x14ac:dyDescent="0.3">
@@ -14993,10 +14990,10 @@
         <v>3</v>
       </c>
       <c r="H490" t="s">
+        <v>486</v>
+      </c>
+      <c r="I490" t="s">
         <v>487</v>
-      </c>
-      <c r="I490" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="491" spans="1:9" x14ac:dyDescent="0.3">
@@ -15412,7 +15409,7 @@
         <v>5</v>
       </c>
       <c r="H506" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="507" spans="1:9" x14ac:dyDescent="0.3">
@@ -15441,7 +15438,7 @@
         <v>5</v>
       </c>
       <c r="I507" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="508" spans="1:9" x14ac:dyDescent="0.3">
@@ -15571,7 +15568,7 @@
         <v>3</v>
       </c>
       <c r="H512" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="513" spans="1:8" x14ac:dyDescent="0.3">
@@ -15649,7 +15646,7 @@
         <v>11</v>
       </c>
       <c r="H515" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="516" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added arginine annotations, needs rescuing
Missed GBT somehow???
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F15B97-49A4-4A62-B6C9-4EB873567BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE714AA-14C1-4542-B5CE-F7CD237AC5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5012" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5298" uniqueCount="603">
   <si>
     <t>Amm</t>
   </si>
@@ -1555,6 +1555,285 @@
   </si>
   <si>
     <t>FT1441</t>
+  </si>
+  <si>
+    <t>FT0036</t>
+  </si>
+  <si>
+    <t>FT0180</t>
+  </si>
+  <si>
+    <t>FT0184</t>
+  </si>
+  <si>
+    <t>FT0428</t>
+  </si>
+  <si>
+    <t>FT0427</t>
+  </si>
+  <si>
+    <t>FT0854</t>
+  </si>
+  <si>
+    <t>FT1013</t>
+  </si>
+  <si>
+    <t>FT1081</t>
+  </si>
+  <si>
+    <t>FT1181</t>
+  </si>
+  <si>
+    <t>FT1180</t>
+  </si>
+  <si>
+    <t>FT1197</t>
+  </si>
+  <si>
+    <t>Rescue?</t>
+  </si>
+  <si>
+    <t>FT1380</t>
+  </si>
+  <si>
+    <t>FT1383</t>
+  </si>
+  <si>
+    <t>Why is this in the pooled samples??</t>
+  </si>
+  <si>
+    <t>FT1468</t>
+  </si>
+  <si>
+    <t>FT1473</t>
+  </si>
+  <si>
+    <t>Mixed with Leu</t>
+  </si>
+  <si>
+    <t>FT1498</t>
+  </si>
+  <si>
+    <t>Rescue but looks gross</t>
+  </si>
+  <si>
+    <t>FT1515</t>
+  </si>
+  <si>
+    <t>FT1552</t>
+  </si>
+  <si>
+    <t>FT1568</t>
+  </si>
+  <si>
+    <t>FT1601</t>
+  </si>
+  <si>
+    <t>FT1600</t>
+  </si>
+  <si>
+    <t>FT1841</t>
+  </si>
+  <si>
+    <t>FT1868</t>
+  </si>
+  <si>
+    <t>FT1908</t>
+  </si>
+  <si>
+    <t>FT1909</t>
+  </si>
+  <si>
+    <t>Check RT</t>
+  </si>
+  <si>
+    <t>FT1929</t>
+  </si>
+  <si>
+    <t>FT1950</t>
+  </si>
+  <si>
+    <t>FT1990</t>
+  </si>
+  <si>
+    <t>FT2027</t>
+  </si>
+  <si>
+    <t>Second peak nearby confusing?</t>
+  </si>
+  <si>
+    <t>Could be rescued</t>
+  </si>
+  <si>
+    <t>FT2104</t>
+  </si>
+  <si>
+    <t>FT2208</t>
+  </si>
+  <si>
+    <t>Others nearby, check grouping</t>
+  </si>
+  <si>
+    <t>FT2219</t>
+  </si>
+  <si>
+    <t>FT2257</t>
+  </si>
+  <si>
+    <t>Probably but multiple peaks</t>
+  </si>
+  <si>
+    <t>FT2256</t>
+  </si>
+  <si>
+    <t>FT2261</t>
+  </si>
+  <si>
+    <t>FT2262</t>
+  </si>
+  <si>
+    <t>FT2263</t>
+  </si>
+  <si>
+    <t>FT2372</t>
+  </si>
+  <si>
+    <t>FT2540</t>
+  </si>
+  <si>
+    <t>FT2542</t>
+  </si>
+  <si>
+    <t>FT2550</t>
+  </si>
+  <si>
+    <t>FT2586</t>
+  </si>
+  <si>
+    <t>FT2590</t>
+  </si>
+  <si>
+    <t>FT2607</t>
+  </si>
+  <si>
+    <t>FT2690</t>
+  </si>
+  <si>
+    <t>FT2717</t>
+  </si>
+  <si>
+    <t>FT2718</t>
+  </si>
+  <si>
+    <t>FT2771</t>
+  </si>
+  <si>
+    <t>FT2966</t>
+  </si>
+  <si>
+    <t>FT3273</t>
+  </si>
+  <si>
+    <t>FT3534</t>
+  </si>
+  <si>
+    <t>FT3557</t>
+  </si>
+  <si>
+    <t>FT3630</t>
+  </si>
+  <si>
+    <t>FT3691</t>
+  </si>
+  <si>
+    <t>FT3775</t>
+  </si>
+  <si>
+    <t>FT3776</t>
+  </si>
+  <si>
+    <t>FT3922</t>
+  </si>
+  <si>
+    <t>FT3943</t>
+  </si>
+  <si>
+    <t>FT3942</t>
+  </si>
+  <si>
+    <t>FT3966</t>
+  </si>
+  <si>
+    <t>FT4056</t>
+  </si>
+  <si>
+    <t>FT4258</t>
+  </si>
+  <si>
+    <t>FT4367</t>
+  </si>
+  <si>
+    <t>Second peak at 10 min could also be?</t>
+  </si>
+  <si>
+    <t>FT0846</t>
+  </si>
+  <si>
+    <t>Doesn't really match mixes</t>
+  </si>
+  <si>
+    <t>FT0904</t>
+  </si>
+  <si>
+    <t>Peak looks awful, rescue?</t>
+  </si>
+  <si>
+    <t>FT1038</t>
+  </si>
+  <si>
+    <t>Awful</t>
+  </si>
+  <si>
+    <t>FT1103</t>
+  </si>
+  <si>
+    <t>FT1200</t>
+  </si>
+  <si>
+    <t>FT1226</t>
+  </si>
+  <si>
+    <t>FT1266</t>
+  </si>
+  <si>
+    <t>Maybe 1335</t>
+  </si>
+  <si>
+    <t>FT1474</t>
+  </si>
+  <si>
+    <t>FT1559</t>
+  </si>
+  <si>
+    <t>FT2152</t>
+  </si>
+  <si>
+    <t>FT2655</t>
+  </si>
+  <si>
+    <t>FT2660</t>
+  </si>
+  <si>
+    <t>FT2799</t>
+  </si>
+  <si>
+    <t>RT doesn't match standards</t>
+  </si>
+  <si>
+    <t>FT3135</t>
+  </si>
+  <si>
+    <t>FT3136</t>
   </si>
 </sst>
 </file>
@@ -1874,8 +2153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1084"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
-      <selection activeCell="H274" sqref="H274"/>
+    <sheetView tabSelected="1" topLeftCell="A1062" workbookViewId="0">
+      <selection activeCell="J1076" sqref="J1076"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22306,7 +22585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="801" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="801" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A801" t="s">
         <v>245</v>
       </c>
@@ -22329,7 +22608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="802" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="802" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A802" t="s">
         <v>245</v>
       </c>
@@ -22352,7 +22631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="803" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="803" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A803" t="s">
         <v>245</v>
       </c>
@@ -22375,7 +22654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="804" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="804" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A804" t="s">
         <v>245</v>
       </c>
@@ -22398,7 +22677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="805" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="805" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A805" t="s">
         <v>245</v>
       </c>
@@ -22421,7 +22700,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="806" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="806" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A806" t="s">
         <v>245</v>
       </c>
@@ -22444,7 +22723,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="807" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="807" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A807" t="s">
         <v>245</v>
       </c>
@@ -22467,7 +22746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="808" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="808" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A808" t="s">
         <v>245</v>
       </c>
@@ -22490,7 +22769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="809" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="809" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A809" t="s">
         <v>245</v>
       </c>
@@ -22513,7 +22792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="810" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="810" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A810" t="s">
         <v>245</v>
       </c>
@@ -22536,7 +22815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="811" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="811" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A811" t="s">
         <v>245</v>
       </c>
@@ -22559,7 +22838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="812" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="812" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A812" t="s">
         <v>245</v>
       </c>
@@ -22582,7 +22861,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="813" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="813" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A813" t="s">
         <v>245</v>
       </c>
@@ -22605,7 +22884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="814" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="814" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A814" t="s">
         <v>245</v>
       </c>
@@ -22628,7 +22907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="815" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="815" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A815" t="s">
         <v>246</v>
       </c>
@@ -22650,8 +22929,11 @@
       <c r="G815" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="816" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H815" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="816" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A816" t="s">
         <v>246</v>
       </c>
@@ -22673,8 +22955,11 @@
       <c r="G816" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="817" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H816" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="817" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A817" t="s">
         <v>246</v>
       </c>
@@ -22696,8 +22981,11 @@
       <c r="G817" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="818" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H817" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="818" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A818" t="s">
         <v>246</v>
       </c>
@@ -22719,8 +23007,11 @@
       <c r="G818" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="819" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H818" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="819" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A819" t="s">
         <v>246</v>
       </c>
@@ -22742,8 +23033,11 @@
       <c r="G819" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="820" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H819" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="820" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A820" t="s">
         <v>246</v>
       </c>
@@ -22765,8 +23059,11 @@
       <c r="G820" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="821" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H820" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="821" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A821" t="s">
         <v>246</v>
       </c>
@@ -22788,8 +23085,11 @@
       <c r="G821" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="822" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H821" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="822" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A822" t="s">
         <v>246</v>
       </c>
@@ -22811,8 +23111,11 @@
       <c r="G822" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="823" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H822" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="823" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A823" t="s">
         <v>246</v>
       </c>
@@ -22834,8 +23137,11 @@
       <c r="G823" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="824" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H823" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="824" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A824" t="s">
         <v>246</v>
       </c>
@@ -22857,8 +23163,11 @@
       <c r="G824" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="825" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H824" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="825" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A825" t="s">
         <v>246</v>
       </c>
@@ -22880,8 +23189,11 @@
       <c r="G825" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="826" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H825" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="826" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A826" t="s">
         <v>246</v>
       </c>
@@ -22903,8 +23215,11 @@
       <c r="G826" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="827" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H826" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="827" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A827" t="s">
         <v>246</v>
       </c>
@@ -22926,8 +23241,11 @@
       <c r="G827" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="828" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H827" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="828" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A828" t="s">
         <v>246</v>
       </c>
@@ -22949,8 +23267,11 @@
       <c r="G828" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="829" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H828" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="829" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A829" t="s">
         <v>246</v>
       </c>
@@ -22972,8 +23293,11 @@
       <c r="G829" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="830" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I829" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="830" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A830" t="s">
         <v>246</v>
       </c>
@@ -22995,8 +23319,11 @@
       <c r="G830" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="831" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H830" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="831" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A831" t="s">
         <v>246</v>
       </c>
@@ -23018,8 +23345,11 @@
       <c r="G831" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="832" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H831" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="832" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A832" t="s">
         <v>246</v>
       </c>
@@ -23041,8 +23371,11 @@
       <c r="G832" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="833" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H832" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="833" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A833" t="s">
         <v>246</v>
       </c>
@@ -23064,8 +23397,11 @@
       <c r="G833" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="834" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H833" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="834" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A834" t="s">
         <v>246</v>
       </c>
@@ -23087,8 +23423,11 @@
       <c r="G834" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="835" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I834" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="835" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A835" t="s">
         <v>246</v>
       </c>
@@ -23110,8 +23449,11 @@
       <c r="G835" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="836" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H835" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="836" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A836" t="s">
         <v>246</v>
       </c>
@@ -23133,8 +23475,11 @@
       <c r="G836" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="837" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H836" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="837" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A837" t="s">
         <v>246</v>
       </c>
@@ -23156,8 +23501,11 @@
       <c r="G837" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="838" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H837" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="838" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A838" t="s">
         <v>246</v>
       </c>
@@ -23179,8 +23527,11 @@
       <c r="G838" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="839" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H838" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="839" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A839" t="s">
         <v>246</v>
       </c>
@@ -23202,8 +23553,11 @@
       <c r="G839" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="840" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H839" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="840" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A840" t="s">
         <v>246</v>
       </c>
@@ -23225,8 +23579,11 @@
       <c r="G840" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="841" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H840" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="841" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A841" t="s">
         <v>246</v>
       </c>
@@ -23248,8 +23605,11 @@
       <c r="G841" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="842" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H841" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="842" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A842" t="s">
         <v>246</v>
       </c>
@@ -23271,8 +23631,11 @@
       <c r="G842" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="843" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H842" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="843" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A843" t="s">
         <v>246</v>
       </c>
@@ -23294,8 +23657,11 @@
       <c r="G843" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="844" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I843" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="844" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A844" t="s">
         <v>246</v>
       </c>
@@ -23317,8 +23683,11 @@
       <c r="G844" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="845" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H844" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="845" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A845" t="s">
         <v>246</v>
       </c>
@@ -23340,8 +23709,11 @@
       <c r="G845" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="846" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H845" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="846" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A846" t="s">
         <v>246</v>
       </c>
@@ -23363,8 +23735,14 @@
       <c r="G846" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="847" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H846" t="s">
+        <v>523</v>
+      </c>
+      <c r="I846" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="847" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A847" t="s">
         <v>246</v>
       </c>
@@ -23386,8 +23764,11 @@
       <c r="G847" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="848" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I847" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="848" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A848" t="s">
         <v>246</v>
       </c>
@@ -23409,8 +23790,11 @@
       <c r="G848" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="849" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I848" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="849" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A849" t="s">
         <v>246</v>
       </c>
@@ -23432,8 +23816,11 @@
       <c r="G849" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="850" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H849" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="850" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A850" t="s">
         <v>246</v>
       </c>
@@ -23455,8 +23842,11 @@
       <c r="G850" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="851" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H850" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="851" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A851" t="s">
         <v>246</v>
       </c>
@@ -23478,8 +23868,11 @@
       <c r="G851" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="852" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H851" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="852" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A852" t="s">
         <v>246</v>
       </c>
@@ -23501,8 +23894,14 @@
       <c r="G852" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="853" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H852" t="s">
+        <v>470</v>
+      </c>
+      <c r="I852" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="853" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A853" t="s">
         <v>246</v>
       </c>
@@ -23524,8 +23923,11 @@
       <c r="G853" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="854" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I853" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="854" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A854" t="s">
         <v>246</v>
       </c>
@@ -23547,8 +23949,11 @@
       <c r="G854" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="855" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H854" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="855" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A855" t="s">
         <v>246</v>
       </c>
@@ -23570,8 +23975,11 @@
       <c r="G855" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="856" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I855" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="856" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A856" t="s">
         <v>246</v>
       </c>
@@ -23593,8 +24001,11 @@
       <c r="G856" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="857" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H856" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="857" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A857" t="s">
         <v>246</v>
       </c>
@@ -23616,8 +24027,11 @@
       <c r="G857" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="858" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I857" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="858" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A858" t="s">
         <v>246</v>
       </c>
@@ -23639,8 +24053,11 @@
       <c r="G858" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="859" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H858" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="859" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A859" t="s">
         <v>246</v>
       </c>
@@ -23662,8 +24079,11 @@
       <c r="G859" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="860" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H859" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="860" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A860" t="s">
         <v>246</v>
       </c>
@@ -23685,8 +24105,11 @@
       <c r="G860" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="861" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H860" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="861" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A861" t="s">
         <v>246</v>
       </c>
@@ -23708,8 +24131,11 @@
       <c r="G861" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="862" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H861" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="862" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A862" t="s">
         <v>246</v>
       </c>
@@ -23731,8 +24157,11 @@
       <c r="G862" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="863" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H862" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="863" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A863" t="s">
         <v>246</v>
       </c>
@@ -23754,8 +24183,11 @@
       <c r="G863" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="864" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H863" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="864" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A864" t="s">
         <v>246</v>
       </c>
@@ -23777,8 +24209,11 @@
       <c r="G864" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="865" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H864" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="865" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A865" t="s">
         <v>246</v>
       </c>
@@ -23800,8 +24235,11 @@
       <c r="G865" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="866" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H865" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="866" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A866" t="s">
         <v>246</v>
       </c>
@@ -23823,8 +24261,11 @@
       <c r="G866" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="867" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H866" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="867" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A867" t="s">
         <v>246</v>
       </c>
@@ -23846,8 +24287,11 @@
       <c r="G867" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="868" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H867" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="868" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A868" t="s">
         <v>246</v>
       </c>
@@ -23869,8 +24313,11 @@
       <c r="G868" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="869" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H868" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="869" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A869" t="s">
         <v>246</v>
       </c>
@@ -23892,8 +24339,11 @@
       <c r="G869" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="870" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H869" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="870" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A870" t="s">
         <v>246</v>
       </c>
@@ -23915,8 +24365,11 @@
       <c r="G870" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="871" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H870" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="871" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A871" t="s">
         <v>246</v>
       </c>
@@ -23938,8 +24391,14 @@
       <c r="G871" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="872" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H871" t="s">
+        <v>538</v>
+      </c>
+      <c r="I871" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="872" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A872" t="s">
         <v>246</v>
       </c>
@@ -23961,8 +24420,11 @@
       <c r="G872" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="873" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H872" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="873" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A873" t="s">
         <v>246</v>
       </c>
@@ -23984,8 +24446,11 @@
       <c r="G873" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="874" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I873" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="874" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A874" t="s">
         <v>246</v>
       </c>
@@ -24007,8 +24472,11 @@
       <c r="G874" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="875" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H874" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="875" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A875" t="s">
         <v>246</v>
       </c>
@@ -24030,8 +24498,11 @@
       <c r="G875" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="876" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H875" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="876" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A876" t="s">
         <v>246</v>
       </c>
@@ -24053,8 +24524,11 @@
       <c r="G876" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="877" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I876" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="877" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A877" t="s">
         <v>246</v>
       </c>
@@ -24076,8 +24550,11 @@
       <c r="G877" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="878" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H877" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="878" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A878" t="s">
         <v>246</v>
       </c>
@@ -24099,8 +24576,11 @@
       <c r="G878" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="879" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H878" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="879" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A879" t="s">
         <v>246</v>
       </c>
@@ -24122,8 +24602,11 @@
       <c r="G879" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="880" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H879" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="880" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A880" t="s">
         <v>246</v>
       </c>
@@ -24145,8 +24628,11 @@
       <c r="G880" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="881" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H880" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="881" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A881" t="s">
         <v>246</v>
       </c>
@@ -24168,8 +24654,11 @@
       <c r="G881" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="882" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H881" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="882" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A882" t="s">
         <v>246</v>
       </c>
@@ -24191,8 +24680,11 @@
       <c r="G882" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="883" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H882" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="883" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A883" t="s">
         <v>246</v>
       </c>
@@ -24214,8 +24706,14 @@
       <c r="G883" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="884" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H883" t="s">
+        <v>543</v>
+      </c>
+      <c r="I883" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="884" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A884" t="s">
         <v>246</v>
       </c>
@@ -24237,8 +24735,14 @@
       <c r="G884" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="885" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H884" t="s">
+        <v>5</v>
+      </c>
+      <c r="I884" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="885" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A885" t="s">
         <v>246</v>
       </c>
@@ -24260,8 +24764,11 @@
       <c r="G885" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="886" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H885" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="886" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A886" t="s">
         <v>246</v>
       </c>
@@ -24283,8 +24790,11 @@
       <c r="G886" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="887" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H886" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="887" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A887" t="s">
         <v>246</v>
       </c>
@@ -24306,8 +24816,14 @@
       <c r="G887" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="888" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H887" t="s">
+        <v>547</v>
+      </c>
+      <c r="I887" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="888" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A888" t="s">
         <v>246</v>
       </c>
@@ -24329,8 +24845,11 @@
       <c r="G888" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="889" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H888" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="889" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A889" t="s">
         <v>246</v>
       </c>
@@ -24352,8 +24871,11 @@
       <c r="G889" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="890" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H889" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="890" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A890" t="s">
         <v>246</v>
       </c>
@@ -24375,8 +24897,14 @@
       <c r="G890" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="891" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H890" t="s">
+        <v>550</v>
+      </c>
+      <c r="I890" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="891" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A891" t="s">
         <v>246</v>
       </c>
@@ -24398,8 +24926,11 @@
       <c r="G891" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="892" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H891" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="892" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A892" t="s">
         <v>246</v>
       </c>
@@ -24421,8 +24952,11 @@
       <c r="G892" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="893" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H892" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="893" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A893" t="s">
         <v>246</v>
       </c>
@@ -24444,8 +24978,11 @@
       <c r="G893" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="894" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H893" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="894" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A894" t="s">
         <v>246</v>
       </c>
@@ -24467,8 +25004,11 @@
       <c r="G894" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="895" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H894" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="895" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A895" t="s">
         <v>246</v>
       </c>
@@ -24490,8 +25030,11 @@
       <c r="G895" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="896" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H895" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="896" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A896" t="s">
         <v>246</v>
       </c>
@@ -24513,8 +25056,11 @@
       <c r="G896" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="897" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H896" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="897" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A897" t="s">
         <v>246</v>
       </c>
@@ -24536,8 +25082,11 @@
       <c r="G897" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="898" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H897" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="898" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A898" t="s">
         <v>246</v>
       </c>
@@ -24559,8 +25108,11 @@
       <c r="G898" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="899" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H898" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="899" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A899" t="s">
         <v>246</v>
       </c>
@@ -24582,8 +25134,11 @@
       <c r="G899" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="900" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I899" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="900" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A900" t="s">
         <v>246</v>
       </c>
@@ -24605,8 +25160,11 @@
       <c r="G900" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="901" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H900" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="901" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A901" t="s">
         <v>246</v>
       </c>
@@ -24628,8 +25186,11 @@
       <c r="G901" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="902" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H901" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="902" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A902" t="s">
         <v>246</v>
       </c>
@@ -24651,8 +25212,11 @@
       <c r="G902" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="903" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H902" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="903" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A903" t="s">
         <v>246</v>
       </c>
@@ -24674,8 +25238,11 @@
       <c r="G903" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="904" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H903" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="904" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A904" t="s">
         <v>246</v>
       </c>
@@ -24697,8 +25264,11 @@
       <c r="G904" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="905" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H904" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="905" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A905" t="s">
         <v>246</v>
       </c>
@@ -24720,8 +25290,11 @@
       <c r="G905" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="906" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H905" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="906" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A906" t="s">
         <v>246</v>
       </c>
@@ -24743,8 +25316,11 @@
       <c r="G906" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="907" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H906" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="907" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A907" t="s">
         <v>246</v>
       </c>
@@ -24766,8 +25342,11 @@
       <c r="G907" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="908" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H907" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="908" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A908" t="s">
         <v>246</v>
       </c>
@@ -24789,8 +25368,11 @@
       <c r="G908" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="909" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H908" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="909" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A909" t="s">
         <v>246</v>
       </c>
@@ -24812,8 +25394,11 @@
       <c r="G909" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="910" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H909" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="910" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A910" t="s">
         <v>246</v>
       </c>
@@ -24835,8 +25420,11 @@
       <c r="G910" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="911" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H910" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="911" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A911" t="s">
         <v>246</v>
       </c>
@@ -24858,8 +25446,11 @@
       <c r="G911" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="912" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H911" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="912" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A912" t="s">
         <v>246</v>
       </c>
@@ -24881,8 +25472,11 @@
       <c r="G912" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="913" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H912" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="913" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A913" t="s">
         <v>246</v>
       </c>
@@ -24904,8 +25498,14 @@
       <c r="G913" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="914" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H913" t="s">
+        <v>5</v>
+      </c>
+      <c r="I913" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="914" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A914" t="s">
         <v>246</v>
       </c>
@@ -24927,8 +25527,11 @@
       <c r="G914" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="915" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H914" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="915" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A915" t="s">
         <v>246</v>
       </c>
@@ -24950,8 +25553,11 @@
       <c r="G915" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="916" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H915" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="916" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A916" t="s">
         <v>246</v>
       </c>
@@ -24973,8 +25579,14 @@
       <c r="G916" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="917" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H916" t="s">
+        <v>5</v>
+      </c>
+      <c r="I916" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="917" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A917" t="s">
         <v>246</v>
       </c>
@@ -24996,8 +25608,11 @@
       <c r="G917" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="918" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H917" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="918" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A918" t="s">
         <v>246</v>
       </c>
@@ -25019,8 +25634,11 @@
       <c r="G918" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="919" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H918" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="919" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A919" t="s">
         <v>246</v>
       </c>
@@ -25042,8 +25660,11 @@
       <c r="G919" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="920" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H919" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="920" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A920" t="s">
         <v>246</v>
       </c>
@@ -25065,8 +25686,11 @@
       <c r="G920" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="921" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H920" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="921" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A921" t="s">
         <v>246</v>
       </c>
@@ -25088,8 +25712,11 @@
       <c r="G921" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="922" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H921" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="922" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A922" t="s">
         <v>246</v>
       </c>
@@ -25111,8 +25738,11 @@
       <c r="G922" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="923" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H922" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="923" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A923" t="s">
         <v>246</v>
       </c>
@@ -25134,8 +25764,11 @@
       <c r="G923" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="924" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H923" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="924" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A924" t="s">
         <v>246</v>
       </c>
@@ -25157,8 +25790,11 @@
       <c r="G924" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="925" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H924" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="925" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A925" t="s">
         <v>246</v>
       </c>
@@ -25180,8 +25816,11 @@
       <c r="G925" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="926" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H925" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="926" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A926" t="s">
         <v>246</v>
       </c>
@@ -25203,8 +25842,11 @@
       <c r="G926" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="927" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H926" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="927" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A927" t="s">
         <v>246</v>
       </c>
@@ -25226,8 +25868,11 @@
       <c r="G927" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="928" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H927" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="928" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A928" t="s">
         <v>246</v>
       </c>
@@ -25249,8 +25894,11 @@
       <c r="G928" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="929" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H928" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="929" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A929" t="s">
         <v>246</v>
       </c>
@@ -25272,8 +25920,11 @@
       <c r="G929" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="930" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H929" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="930" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A930" t="s">
         <v>246</v>
       </c>
@@ -25295,8 +25946,11 @@
       <c r="G930" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="931" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H930" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="931" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A931" t="s">
         <v>246</v>
       </c>
@@ -25318,8 +25972,11 @@
       <c r="G931" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="932" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H931" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="932" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A932" t="s">
         <v>246</v>
       </c>
@@ -25341,8 +25998,11 @@
       <c r="G932" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="933" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H932" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="933" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A933" t="s">
         <v>246</v>
       </c>
@@ -25364,8 +26024,11 @@
       <c r="G933" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="934" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H933" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="934" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A934" t="s">
         <v>246</v>
       </c>
@@ -25387,8 +26050,11 @@
       <c r="G934" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="935" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I934" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="935" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A935" t="s">
         <v>246</v>
       </c>
@@ -25410,8 +26076,11 @@
       <c r="G935" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="936" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H935" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="936" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A936" t="s">
         <v>246</v>
       </c>
@@ -25433,8 +26102,11 @@
       <c r="G936" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="937" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H936" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="937" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A937" t="s">
         <v>246</v>
       </c>
@@ -25456,8 +26128,11 @@
       <c r="G937" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="938" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H937" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="938" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A938" t="s">
         <v>246</v>
       </c>
@@ -25479,8 +26154,11 @@
       <c r="G938" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="939" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H938" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="939" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A939" t="s">
         <v>246</v>
       </c>
@@ -25502,8 +26180,11 @@
       <c r="G939" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="940" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H939" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="940" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A940" t="s">
         <v>246</v>
       </c>
@@ -25525,8 +26206,11 @@
       <c r="G940" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="941" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H940" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="941" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A941" t="s">
         <v>246</v>
       </c>
@@ -25548,8 +26232,11 @@
       <c r="G941" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="942" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I941" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="942" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A942" t="s">
         <v>246</v>
       </c>
@@ -25571,8 +26258,11 @@
       <c r="G942" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="943" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H942" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="943" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A943" t="s">
         <v>246</v>
       </c>
@@ -25594,8 +26284,11 @@
       <c r="G943" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="944" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H943" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="944" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A944" t="s">
         <v>246</v>
       </c>
@@ -25617,8 +26310,11 @@
       <c r="G944" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="945" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H944" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="945" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A945" t="s">
         <v>246</v>
       </c>
@@ -25640,8 +26336,11 @@
       <c r="G945" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="946" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H945" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="946" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A946" t="s">
         <v>246</v>
       </c>
@@ -25663,8 +26362,11 @@
       <c r="G946" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="947" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H946" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="947" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A947" t="s">
         <v>246</v>
       </c>
@@ -25686,8 +26388,11 @@
       <c r="G947" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="948" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H947" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="948" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A948" t="s">
         <v>246</v>
       </c>
@@ -25709,8 +26414,11 @@
       <c r="G948" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="949" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H948" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="949" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A949" t="s">
         <v>246</v>
       </c>
@@ -25732,8 +26440,11 @@
       <c r="G949" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="950" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H949" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="950" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A950" t="s">
         <v>246</v>
       </c>
@@ -25755,8 +26466,11 @@
       <c r="G950" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="951" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H950" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="951" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A951" t="s">
         <v>246</v>
       </c>
@@ -25778,8 +26492,11 @@
       <c r="G951" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="952" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H951" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="952" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A952" t="s">
         <v>246</v>
       </c>
@@ -25801,8 +26518,11 @@
       <c r="G952" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="953" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H952" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="953" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A953" t="s">
         <v>246</v>
       </c>
@@ -25824,8 +26544,11 @@
       <c r="G953" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="954" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H953" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="954" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A954" t="s">
         <v>246</v>
       </c>
@@ -25847,8 +26570,11 @@
       <c r="G954" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="955" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H954" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="955" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A955" t="s">
         <v>246</v>
       </c>
@@ -25870,8 +26596,11 @@
       <c r="G955" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="956" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H955" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="956" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A956" t="s">
         <v>246</v>
       </c>
@@ -25893,8 +26622,14 @@
       <c r="G956" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="957" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H956" t="s">
+        <v>581</v>
+      </c>
+      <c r="I956" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="957" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A957" t="s">
         <v>246</v>
       </c>
@@ -25916,8 +26651,11 @@
       <c r="G957" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="958" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H957" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="958" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A958" t="s">
         <v>246</v>
       </c>
@@ -25939,8 +26677,11 @@
       <c r="G958" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="959" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H958" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="959" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A959" t="s">
         <v>246</v>
       </c>
@@ -25962,8 +26703,11 @@
       <c r="G959" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="960" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H959" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="960" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A960" t="s">
         <v>246</v>
       </c>
@@ -25985,8 +26729,11 @@
       <c r="G960" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="961" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H960" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="961" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A961" t="s">
         <v>246</v>
       </c>
@@ -26008,8 +26755,11 @@
       <c r="G961" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="962" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H961" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="962" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A962" t="s">
         <v>246</v>
       </c>
@@ -26031,8 +26781,11 @@
       <c r="G962" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="963" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H962" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="963" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A963" t="s">
         <v>246</v>
       </c>
@@ -26054,8 +26807,11 @@
       <c r="G963" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="964" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H963" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="964" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A964" t="s">
         <v>246</v>
       </c>
@@ -26077,8 +26833,11 @@
       <c r="G964" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="965" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H964" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="965" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A965" t="s">
         <v>246</v>
       </c>
@@ -26100,8 +26859,11 @@
       <c r="G965" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="966" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H965" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="966" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A966" t="s">
         <v>246</v>
       </c>
@@ -26123,8 +26885,11 @@
       <c r="G966" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="967" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H966" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="967" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A967" t="s">
         <v>246</v>
       </c>
@@ -26146,8 +26911,11 @@
       <c r="G967" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="968" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H967" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="968" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A968" t="s">
         <v>246</v>
       </c>
@@ -26169,8 +26937,11 @@
       <c r="G968" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="969" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H968" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="969" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A969" t="s">
         <v>246</v>
       </c>
@@ -26192,8 +26963,11 @@
       <c r="G969" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="970" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H969" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="970" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A970" t="s">
         <v>246</v>
       </c>
@@ -26215,8 +26989,11 @@
       <c r="G970" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="971" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H970" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="971" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A971" t="s">
         <v>246</v>
       </c>
@@ -26238,8 +27015,11 @@
       <c r="G971" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="972" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H971" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="972" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A972" t="s">
         <v>246</v>
       </c>
@@ -26261,8 +27041,11 @@
       <c r="G972" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="973" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H972" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="973" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A973" t="s">
         <v>246</v>
       </c>
@@ -26284,8 +27067,11 @@
       <c r="G973" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="974" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I973" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="974" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A974" t="s">
         <v>246</v>
       </c>
@@ -26307,8 +27093,11 @@
       <c r="G974" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="975" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H974" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="975" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A975" t="s">
         <v>246</v>
       </c>
@@ -26330,8 +27119,14 @@
       <c r="G975" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="976" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H975" t="s">
+        <v>583</v>
+      </c>
+      <c r="I975" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="976" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A976" t="s">
         <v>246</v>
       </c>
@@ -26353,8 +27148,11 @@
       <c r="G976" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="977" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H976" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="977" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A977" t="s">
         <v>246</v>
       </c>
@@ -26376,8 +27174,11 @@
       <c r="G977" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="978" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H977" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="978" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A978" t="s">
         <v>246</v>
       </c>
@@ -26399,8 +27200,11 @@
       <c r="G978" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="979" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H978" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="979" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A979" t="s">
         <v>246</v>
       </c>
@@ -26422,8 +27226,11 @@
       <c r="G979" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="980" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H979" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="980" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A980" t="s">
         <v>246</v>
       </c>
@@ -26445,8 +27252,11 @@
       <c r="G980" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="981" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I980" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="981" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A981" t="s">
         <v>246</v>
       </c>
@@ -26468,8 +27278,11 @@
       <c r="G981" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="982" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I981" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="982" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A982" t="s">
         <v>246</v>
       </c>
@@ -26491,8 +27304,11 @@
       <c r="G982" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="983" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H982" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="983" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A983" t="s">
         <v>246</v>
       </c>
@@ -26514,8 +27330,14 @@
       <c r="G983" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="984" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H983" t="s">
+        <v>5</v>
+      </c>
+      <c r="I983" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="984" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A984" t="s">
         <v>246</v>
       </c>
@@ -26537,8 +27359,11 @@
       <c r="G984" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="985" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H984" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="985" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A985" t="s">
         <v>246</v>
       </c>
@@ -26560,8 +27385,11 @@
       <c r="G985" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="986" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H985" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="986" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A986" t="s">
         <v>246</v>
       </c>
@@ -26583,8 +27411,11 @@
       <c r="G986" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="987" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H986" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="987" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A987" t="s">
         <v>246</v>
       </c>
@@ -26606,8 +27437,11 @@
       <c r="G987" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="988" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H987" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="988" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A988" t="s">
         <v>246</v>
       </c>
@@ -26629,8 +27463,11 @@
       <c r="G988" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="989" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H988" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="989" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A989" t="s">
         <v>246</v>
       </c>
@@ -26652,8 +27489,11 @@
       <c r="G989" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="990" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H989" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="990" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A990" t="s">
         <v>246</v>
       </c>
@@ -26675,8 +27515,11 @@
       <c r="G990" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="991" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H990" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="991" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A991" t="s">
         <v>246</v>
       </c>
@@ -26698,8 +27541,11 @@
       <c r="G991" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="992" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H991" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="992" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A992" t="s">
         <v>246</v>
       </c>
@@ -26721,8 +27567,11 @@
       <c r="G992" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="993" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H992" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="993" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A993" t="s">
         <v>246</v>
       </c>
@@ -26744,8 +27593,11 @@
       <c r="G993" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="994" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H993" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="994" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A994" t="s">
         <v>246</v>
       </c>
@@ -26767,8 +27619,14 @@
       <c r="G994" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="995" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H994" t="s">
+        <v>5</v>
+      </c>
+      <c r="I994" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="995" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A995" t="s">
         <v>246</v>
       </c>
@@ -26790,8 +27648,11 @@
       <c r="G995" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="996" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H995" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="996" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A996" t="s">
         <v>246</v>
       </c>
@@ -26813,8 +27674,11 @@
       <c r="G996" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="997" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H996" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="997" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A997" t="s">
         <v>246</v>
       </c>
@@ -26836,8 +27700,14 @@
       <c r="G997" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="998" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H997" t="s">
+        <v>5</v>
+      </c>
+      <c r="I997" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="998" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A998" t="s">
         <v>246</v>
       </c>
@@ -26859,8 +27729,11 @@
       <c r="G998" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="999" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H998" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="999" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A999" t="s">
         <v>246</v>
       </c>
@@ -26882,8 +27755,11 @@
       <c r="G999" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1000" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H999" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1000" t="s">
         <v>246</v>
       </c>
@@ -26905,8 +27781,11 @@
       <c r="G1000" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1001" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1000" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1001" t="s">
         <v>246</v>
       </c>
@@ -26928,8 +27807,14 @@
       <c r="G1001" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1002" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1001" t="s">
+        <v>594</v>
+      </c>
+      <c r="I1001" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1002" t="s">
         <v>246</v>
       </c>
@@ -26951,8 +27836,11 @@
       <c r="G1002" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1003" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1002" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1003" t="s">
         <v>246</v>
       </c>
@@ -26974,8 +27862,11 @@
       <c r="G1003" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1004" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1003" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1004" t="s">
         <v>246</v>
       </c>
@@ -26997,8 +27888,11 @@
       <c r="G1004" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1005" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1004" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1005" t="s">
         <v>246</v>
       </c>
@@ -27020,8 +27914,11 @@
       <c r="G1005" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1006" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1005" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1006" t="s">
         <v>246</v>
       </c>
@@ -27043,8 +27940,11 @@
       <c r="G1006" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1007" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1006" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1007" t="s">
         <v>246</v>
       </c>
@@ -27066,8 +27966,11 @@
       <c r="G1007" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1008" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1007" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1008" t="s">
         <v>246</v>
       </c>
@@ -27089,8 +27992,11 @@
       <c r="G1008" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1009" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1008" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1009" t="s">
         <v>246</v>
       </c>
@@ -27112,8 +28018,11 @@
       <c r="G1009" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1010" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1009" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1010" t="s">
         <v>246</v>
       </c>
@@ -27135,8 +28044,11 @@
       <c r="G1010" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1011" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1010" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1011" t="s">
         <v>246</v>
       </c>
@@ -27158,8 +28070,11 @@
       <c r="G1011" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1012" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1011" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1012" t="s">
         <v>246</v>
       </c>
@@ -27181,8 +28096,11 @@
       <c r="G1012" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1013" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1012" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1013" t="s">
         <v>246</v>
       </c>
@@ -27204,8 +28122,11 @@
       <c r="G1013" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1014" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1013" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1014" t="s">
         <v>246</v>
       </c>
@@ -27227,8 +28148,11 @@
       <c r="G1014" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="1015" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1014" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1015" t="s">
         <v>246</v>
       </c>
@@ -27250,8 +28174,11 @@
       <c r="G1015" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="1016" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1015" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1016" t="s">
         <v>246</v>
       </c>
@@ -27273,8 +28200,11 @@
       <c r="G1016" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1017" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1016" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1017" t="s">
         <v>246</v>
       </c>
@@ -27296,8 +28226,11 @@
       <c r="G1017" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1018" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1017" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1018" t="s">
         <v>246</v>
       </c>
@@ -27319,8 +28252,11 @@
       <c r="G1018" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1019" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1018" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1019" t="s">
         <v>246</v>
       </c>
@@ -27342,8 +28278,11 @@
       <c r="G1019" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1020" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1019" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1020" t="s">
         <v>246</v>
       </c>
@@ -27365,8 +28304,11 @@
       <c r="G1020" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1021" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1020" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1021" t="s">
         <v>246</v>
       </c>
@@ -27388,8 +28330,11 @@
       <c r="G1021" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="1022" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1021" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1022" t="s">
         <v>246</v>
       </c>
@@ -27411,8 +28356,11 @@
       <c r="G1022" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1023" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1022" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1023" t="s">
         <v>246</v>
       </c>
@@ -27434,8 +28382,11 @@
       <c r="G1023" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1024" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1023" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1024" t="s">
         <v>246</v>
       </c>
@@ -27457,8 +28408,11 @@
       <c r="G1024" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1025" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1024" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1025" t="s">
         <v>246</v>
       </c>
@@ -27480,8 +28434,11 @@
       <c r="G1025" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1026" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1025" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1026" t="s">
         <v>246</v>
       </c>
@@ -27503,8 +28460,11 @@
       <c r="G1026" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1027" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1026" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1027" t="s">
         <v>246</v>
       </c>
@@ -27526,8 +28486,11 @@
       <c r="G1027" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1028" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1027" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1028" t="s">
         <v>246</v>
       </c>
@@ -27549,8 +28512,11 @@
       <c r="G1028" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="1029" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1028" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1029" t="s">
         <v>246</v>
       </c>
@@ -27572,8 +28538,11 @@
       <c r="G1029" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1030" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1029" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1030" t="s">
         <v>246</v>
       </c>
@@ -27595,8 +28564,11 @@
       <c r="G1030" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1031" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1030" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1031" t="s">
         <v>246</v>
       </c>
@@ -27618,8 +28590,11 @@
       <c r="G1031" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1032" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1031" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1032" t="s">
         <v>246</v>
       </c>
@@ -27641,8 +28616,11 @@
       <c r="G1032" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1033" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1032" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1033" t="s">
         <v>246</v>
       </c>
@@ -27664,8 +28642,11 @@
       <c r="G1033" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1034" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1033" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1034" t="s">
         <v>246</v>
       </c>
@@ -27687,8 +28668,11 @@
       <c r="G1034" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1035" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1034" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1035" t="s">
         <v>246</v>
       </c>
@@ -27710,8 +28694,11 @@
       <c r="G1035" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1036" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1035" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1036" t="s">
         <v>246</v>
       </c>
@@ -27733,8 +28720,11 @@
       <c r="G1036" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1037" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1036" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1037" t="s">
         <v>246</v>
       </c>
@@ -27756,8 +28746,11 @@
       <c r="G1037" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1038" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1037" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1038" t="s">
         <v>246</v>
       </c>
@@ -27779,8 +28772,11 @@
       <c r="G1038" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1039" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1038" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1039" t="s">
         <v>246</v>
       </c>
@@ -27802,8 +28798,11 @@
       <c r="G1039" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1040" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1039" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1040" t="s">
         <v>246</v>
       </c>
@@ -27825,8 +28824,11 @@
       <c r="G1040" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1041" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1040" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1041" t="s">
         <v>246</v>
       </c>
@@ -27848,8 +28850,11 @@
       <c r="G1041" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1042" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1041" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1042" t="s">
         <v>246</v>
       </c>
@@ -27871,8 +28876,11 @@
       <c r="G1042" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1043" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1042" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1043" t="s">
         <v>246</v>
       </c>
@@ -27894,8 +28902,11 @@
       <c r="G1043" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="1044" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1043" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1044" t="s">
         <v>246</v>
       </c>
@@ -27917,8 +28928,11 @@
       <c r="G1044" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1045" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1044" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1045" t="s">
         <v>246</v>
       </c>
@@ -27940,8 +28954,11 @@
       <c r="G1045" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1046" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1045" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1046" t="s">
         <v>246</v>
       </c>
@@ -27963,8 +28980,11 @@
       <c r="G1046" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1047" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1046" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1047" t="s">
         <v>246</v>
       </c>
@@ -27986,8 +29006,11 @@
       <c r="G1047" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1048" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1047" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1048" t="s">
         <v>246</v>
       </c>
@@ -28009,8 +29032,11 @@
       <c r="G1048" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1049" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1048" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1049" t="s">
         <v>246</v>
       </c>
@@ -28032,8 +29058,11 @@
       <c r="G1049" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="1050" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1049" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1050" t="s">
         <v>246</v>
       </c>
@@ -28055,8 +29084,14 @@
       <c r="G1050" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1051" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1050" t="s">
+        <v>599</v>
+      </c>
+      <c r="I1050" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1051" t="s">
         <v>246</v>
       </c>
@@ -28078,8 +29113,11 @@
       <c r="G1051" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1052" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1051" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1052" t="s">
         <v>246</v>
       </c>
@@ -28101,8 +29139,11 @@
       <c r="G1052" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1053" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1052" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1053" t="s">
         <v>246</v>
       </c>
@@ -28124,8 +29165,11 @@
       <c r="G1053" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1054" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1053" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1054" t="s">
         <v>246</v>
       </c>
@@ -28147,8 +29191,11 @@
       <c r="G1054" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1055" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1054" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1055" t="s">
         <v>246</v>
       </c>
@@ -28170,8 +29217,11 @@
       <c r="G1055" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1056" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1055" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1056" t="s">
         <v>246</v>
       </c>
@@ -28193,8 +29243,11 @@
       <c r="G1056" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1057" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1056" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1057" t="s">
         <v>246</v>
       </c>
@@ -28216,8 +29269,11 @@
       <c r="G1057" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1058" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1057" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1058" t="s">
         <v>246</v>
       </c>
@@ -28239,8 +29295,11 @@
       <c r="G1058" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1059" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1058" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1059" t="s">
         <v>246</v>
       </c>
@@ -28262,8 +29321,11 @@
       <c r="G1059" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1060" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1059" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1060" t="s">
         <v>246</v>
       </c>
@@ -28285,8 +29347,11 @@
       <c r="G1060" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1061" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1060" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1061" t="s">
         <v>246</v>
       </c>
@@ -28308,8 +29373,11 @@
       <c r="G1061" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1062" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1061" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1062" t="s">
         <v>246</v>
       </c>
@@ -28331,8 +29399,11 @@
       <c r="G1062" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1063" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1062" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1063" t="s">
         <v>246</v>
       </c>
@@ -28354,8 +29425,11 @@
       <c r="G1063" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1064" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1063" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1064" t="s">
         <v>246</v>
       </c>
@@ -28377,8 +29451,11 @@
       <c r="G1064" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="1065" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1064" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1065" t="s">
         <v>246</v>
       </c>
@@ -28400,8 +29477,11 @@
       <c r="G1065" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1066" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1065" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1066" t="s">
         <v>246</v>
       </c>
@@ -28423,8 +29503,11 @@
       <c r="G1066" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="1067" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1066" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1067" t="s">
         <v>246</v>
       </c>
@@ -28446,8 +29529,11 @@
       <c r="G1067" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1068" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1067" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1068" t="s">
         <v>246</v>
       </c>
@@ -28469,8 +29555,11 @@
       <c r="G1068" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1069" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1068" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1069" t="s">
         <v>246</v>
       </c>
@@ -28492,8 +29581,11 @@
       <c r="G1069" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1070" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1069" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1070" t="s">
         <v>246</v>
       </c>
@@ -28515,8 +29607,11 @@
       <c r="G1070" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1071" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1070" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1071" t="s">
         <v>246</v>
       </c>
@@ -28538,8 +29633,11 @@
       <c r="G1071" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1072" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1071" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1072" t="s">
         <v>246</v>
       </c>
@@ -28561,8 +29659,11 @@
       <c r="G1072" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="1073" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1072" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1073" t="s">
         <v>246</v>
       </c>
@@ -28584,8 +29685,11 @@
       <c r="G1073" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1074" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1073" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1074" t="s">
         <v>246</v>
       </c>
@@ -28607,8 +29711,11 @@
       <c r="G1074" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1075" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1074" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1075" t="s">
         <v>246</v>
       </c>
@@ -28630,8 +29737,11 @@
       <c r="G1075" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1076" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1075" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1076" t="s">
         <v>246</v>
       </c>
@@ -28653,8 +29763,11 @@
       <c r="G1076" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="1077" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1076" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1077" t="s">
         <v>246</v>
       </c>
@@ -28676,8 +29789,11 @@
       <c r="G1077" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1078" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1077" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1078" t="s">
         <v>246</v>
       </c>
@@ -28699,8 +29815,11 @@
       <c r="G1078" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1079" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1078" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1079" t="s">
         <v>246</v>
       </c>
@@ -28722,8 +29841,11 @@
       <c r="G1079" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1080" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1079" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1080" t="s">
         <v>246</v>
       </c>
@@ -28745,8 +29867,11 @@
       <c r="G1080" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1081" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1080" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1081" t="s">
         <v>246</v>
       </c>
@@ -28768,8 +29893,11 @@
       <c r="G1081" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1082" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1081" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1082" t="s">
         <v>246</v>
       </c>
@@ -28791,8 +29919,11 @@
       <c r="G1082" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1083" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1082" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1083" t="s">
         <v>246</v>
       </c>
@@ -28814,8 +29945,11 @@
       <c r="G1083" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="1084" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1083" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1084" t="s">
         <v>246</v>
       </c>
@@ -28836,6 +29970,9 @@
       </c>
       <c r="G1084" t="s">
         <v>3</v>
+      </c>
+      <c r="H1084" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished rescuing Arginine targets
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE714AA-14C1-4542-B5CE-F7CD237AC5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80924479-22B2-4E09-B2AB-A72EC573ABB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5298" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5313" uniqueCount="625">
   <si>
     <t>Amm</t>
   </si>
@@ -1590,9 +1590,6 @@
     <t>FT1197</t>
   </si>
   <si>
-    <t>Rescue?</t>
-  </si>
-  <si>
     <t>FT1380</t>
   </si>
   <si>
@@ -1614,9 +1611,6 @@
     <t>FT1498</t>
   </si>
   <si>
-    <t>Rescue but looks gross</t>
-  </si>
-  <si>
     <t>FT1515</t>
   </si>
   <si>
@@ -1834,6 +1828,78 @@
   </si>
   <si>
     <t>FT3136</t>
+  </si>
+  <si>
+    <t>FT0945</t>
+  </si>
+  <si>
+    <t>Saved</t>
+  </si>
+  <si>
+    <t>FT1138</t>
+  </si>
+  <si>
+    <t>FT1346</t>
+  </si>
+  <si>
+    <t>Isn't a great peak, check grouping</t>
+  </si>
+  <si>
+    <t>FT1413</t>
+  </si>
+  <si>
+    <t>Not saved</t>
+  </si>
+  <si>
+    <t>FT1476</t>
+  </si>
+  <si>
+    <t>FT1505</t>
+  </si>
+  <si>
+    <t>Saved but looks gross</t>
+  </si>
+  <si>
+    <t>FT1533</t>
+  </si>
+  <si>
+    <t>FT1935</t>
+  </si>
+  <si>
+    <t>FT1945</t>
+  </si>
+  <si>
+    <t>FT2029</t>
+  </si>
+  <si>
+    <t>FT2425</t>
+  </si>
+  <si>
+    <t>FT2774</t>
+  </si>
+  <si>
+    <t>not great but saved anywa</t>
+  </si>
+  <si>
+    <t>FT2999</t>
+  </si>
+  <si>
+    <t>FT3668</t>
+  </si>
+  <si>
+    <t>FT3801</t>
+  </si>
+  <si>
+    <t>FT0790</t>
+  </si>
+  <si>
+    <t>FT1022</t>
+  </si>
+  <si>
+    <t>FT1031</t>
+  </si>
+  <si>
+    <t>FT1387</t>
   </si>
 </sst>
 </file>
@@ -2153,8 +2219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1084"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1062" workbookViewId="0">
-      <selection activeCell="J1076" sqref="J1076"/>
+    <sheetView tabSelected="1" topLeftCell="A982" workbookViewId="0">
+      <selection activeCell="H998" sqref="H998"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23293,8 +23359,11 @@
       <c r="G829" t="s">
         <v>11</v>
       </c>
+      <c r="H829" t="s">
+        <v>601</v>
+      </c>
       <c r="I829" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="830" spans="1:9" x14ac:dyDescent="0.3">
@@ -23423,8 +23492,11 @@
       <c r="G834" t="s">
         <v>3</v>
       </c>
+      <c r="H834" t="s">
+        <v>603</v>
+      </c>
       <c r="I834" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="835" spans="1:9" x14ac:dyDescent="0.3">
@@ -23657,8 +23729,11 @@
       <c r="G843" t="s">
         <v>11</v>
       </c>
+      <c r="H843" t="s">
+        <v>604</v>
+      </c>
       <c r="I843" t="s">
-        <v>521</v>
+        <v>605</v>
       </c>
     </row>
     <row r="844" spans="1:9" x14ac:dyDescent="0.3">
@@ -23710,7 +23785,7 @@
         <v>11</v>
       </c>
       <c r="H845" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="846" spans="1:9" x14ac:dyDescent="0.3">
@@ -23736,10 +23811,10 @@
         <v>11</v>
       </c>
       <c r="H846" t="s">
+        <v>522</v>
+      </c>
+      <c r="I846" t="s">
         <v>523</v>
-      </c>
-      <c r="I846" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="847" spans="1:9" x14ac:dyDescent="0.3">
@@ -23764,8 +23839,11 @@
       <c r="G847" t="s">
         <v>3</v>
       </c>
+      <c r="H847" t="s">
+        <v>606</v>
+      </c>
       <c r="I847" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="848" spans="1:9" x14ac:dyDescent="0.3">
@@ -23790,8 +23868,11 @@
       <c r="G848" t="s">
         <v>3</v>
       </c>
+      <c r="H848" t="s">
+        <v>5</v>
+      </c>
       <c r="I848" t="s">
-        <v>521</v>
+        <v>607</v>
       </c>
     </row>
     <row r="849" spans="1:9" x14ac:dyDescent="0.3">
@@ -23817,7 +23898,7 @@
         <v>3</v>
       </c>
       <c r="H849" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="850" spans="1:9" x14ac:dyDescent="0.3">
@@ -23843,7 +23924,7 @@
         <v>3</v>
       </c>
       <c r="H850" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="851" spans="1:9" x14ac:dyDescent="0.3">
@@ -23898,7 +23979,7 @@
         <v>470</v>
       </c>
       <c r="I852" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="853" spans="1:9" x14ac:dyDescent="0.3">
@@ -23923,8 +24004,11 @@
       <c r="G853" t="s">
         <v>11</v>
       </c>
+      <c r="H853" t="s">
+        <v>608</v>
+      </c>
       <c r="I853" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="854" spans="1:9" x14ac:dyDescent="0.3">
@@ -23950,7 +24034,7 @@
         <v>3</v>
       </c>
       <c r="H854" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="855" spans="1:9" x14ac:dyDescent="0.3">
@@ -23975,8 +24059,11 @@
       <c r="G855" t="s">
         <v>3</v>
       </c>
+      <c r="H855" t="s">
+        <v>609</v>
+      </c>
       <c r="I855" t="s">
-        <v>529</v>
+        <v>610</v>
       </c>
     </row>
     <row r="856" spans="1:9" x14ac:dyDescent="0.3">
@@ -24002,7 +24089,7 @@
         <v>3</v>
       </c>
       <c r="H856" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="857" spans="1:9" x14ac:dyDescent="0.3">
@@ -24027,8 +24114,11 @@
       <c r="G857" t="s">
         <v>11</v>
       </c>
+      <c r="H857" t="s">
+        <v>611</v>
+      </c>
       <c r="I857" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="858" spans="1:9" x14ac:dyDescent="0.3">
@@ -24106,7 +24196,7 @@
         <v>3</v>
       </c>
       <c r="H860" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="861" spans="1:9" x14ac:dyDescent="0.3">
@@ -24158,7 +24248,7 @@
         <v>11</v>
       </c>
       <c r="H862" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="863" spans="1:9" x14ac:dyDescent="0.3">
@@ -24184,7 +24274,7 @@
         <v>11</v>
       </c>
       <c r="H863" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="864" spans="1:9" x14ac:dyDescent="0.3">
@@ -24210,7 +24300,7 @@
         <v>3</v>
       </c>
       <c r="H864" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="865" spans="1:9" x14ac:dyDescent="0.3">
@@ -24314,7 +24404,7 @@
         <v>11</v>
       </c>
       <c r="H868" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="869" spans="1:9" x14ac:dyDescent="0.3">
@@ -24340,7 +24430,7 @@
         <v>3</v>
       </c>
       <c r="H869" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="870" spans="1:9" x14ac:dyDescent="0.3">
@@ -24366,7 +24456,7 @@
         <v>3</v>
       </c>
       <c r="H870" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="871" spans="1:9" x14ac:dyDescent="0.3">
@@ -24392,10 +24482,10 @@
         <v>11</v>
       </c>
       <c r="H871" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I871" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="872" spans="1:9" x14ac:dyDescent="0.3">
@@ -24421,7 +24511,7 @@
         <v>3</v>
       </c>
       <c r="H872" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="873" spans="1:9" x14ac:dyDescent="0.3">
@@ -24446,8 +24536,11 @@
       <c r="G873" t="s">
         <v>3</v>
       </c>
+      <c r="H873" t="s">
+        <v>612</v>
+      </c>
       <c r="I873" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="874" spans="1:9" x14ac:dyDescent="0.3">
@@ -24524,8 +24617,8 @@
       <c r="G876" t="s">
         <v>3</v>
       </c>
-      <c r="I876" t="s">
-        <v>392</v>
+      <c r="H876" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="877" spans="1:9" x14ac:dyDescent="0.3">
@@ -24551,7 +24644,7 @@
         <v>11</v>
       </c>
       <c r="H877" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="878" spans="1:9" x14ac:dyDescent="0.3">
@@ -24577,7 +24670,7 @@
         <v>3</v>
       </c>
       <c r="H878" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="879" spans="1:9" x14ac:dyDescent="0.3">
@@ -24707,10 +24800,10 @@
         <v>11</v>
       </c>
       <c r="H883" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I883" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="884" spans="1:9" x14ac:dyDescent="0.3">
@@ -24736,10 +24829,10 @@
         <v>11</v>
       </c>
       <c r="H884" t="s">
-        <v>5</v>
+        <v>614</v>
       </c>
       <c r="I884" t="s">
-        <v>545</v>
+        <v>602</v>
       </c>
     </row>
     <row r="885" spans="1:9" x14ac:dyDescent="0.3">
@@ -24791,7 +24884,7 @@
         <v>3</v>
       </c>
       <c r="H886" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="887" spans="1:9" x14ac:dyDescent="0.3">
@@ -24817,10 +24910,10 @@
         <v>11</v>
       </c>
       <c r="H887" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="I887" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="888" spans="1:9" x14ac:dyDescent="0.3">
@@ -24846,7 +24939,7 @@
         <v>11</v>
       </c>
       <c r="H888" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="889" spans="1:9" x14ac:dyDescent="0.3">
@@ -24898,10 +24991,10 @@
         <v>5</v>
       </c>
       <c r="H890" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I890" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="891" spans="1:9" x14ac:dyDescent="0.3">
@@ -24927,7 +25020,7 @@
         <v>5</v>
       </c>
       <c r="H891" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="892" spans="1:9" x14ac:dyDescent="0.3">
@@ -24953,7 +25046,7 @@
         <v>5</v>
       </c>
       <c r="H892" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="893" spans="1:9" x14ac:dyDescent="0.3">
@@ -24979,7 +25072,7 @@
         <v>5</v>
       </c>
       <c r="H893" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="894" spans="1:9" x14ac:dyDescent="0.3">
@@ -25005,7 +25098,7 @@
         <v>3</v>
       </c>
       <c r="H894" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="895" spans="1:9" x14ac:dyDescent="0.3">
@@ -25057,7 +25150,7 @@
         <v>3</v>
       </c>
       <c r="H896" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="897" spans="1:9" x14ac:dyDescent="0.3">
@@ -25134,8 +25227,11 @@
       <c r="G899" t="s">
         <v>3</v>
       </c>
+      <c r="H899" t="s">
+        <v>615</v>
+      </c>
       <c r="I899" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="900" spans="1:9" x14ac:dyDescent="0.3">
@@ -25187,7 +25283,7 @@
         <v>5</v>
       </c>
       <c r="H901" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="902" spans="1:9" x14ac:dyDescent="0.3">
@@ -25213,7 +25309,7 @@
         <v>3</v>
       </c>
       <c r="H902" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="903" spans="1:9" x14ac:dyDescent="0.3">
@@ -25265,7 +25361,7 @@
         <v>3</v>
       </c>
       <c r="H904" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="905" spans="1:9" x14ac:dyDescent="0.3">
@@ -25291,7 +25387,7 @@
         <v>11</v>
       </c>
       <c r="H905" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="906" spans="1:9" x14ac:dyDescent="0.3">
@@ -25343,7 +25439,7 @@
         <v>11</v>
       </c>
       <c r="H907" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="908" spans="1:9" x14ac:dyDescent="0.3">
@@ -25369,7 +25465,7 @@
         <v>3</v>
       </c>
       <c r="H908" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="909" spans="1:9" x14ac:dyDescent="0.3">
@@ -25395,7 +25491,7 @@
         <v>3</v>
       </c>
       <c r="H909" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="910" spans="1:9" x14ac:dyDescent="0.3">
@@ -25421,7 +25517,7 @@
         <v>3</v>
       </c>
       <c r="H910" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="911" spans="1:9" x14ac:dyDescent="0.3">
@@ -25447,7 +25543,7 @@
         <v>3</v>
       </c>
       <c r="H911" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="912" spans="1:9" x14ac:dyDescent="0.3">
@@ -25473,7 +25569,7 @@
         <v>3</v>
       </c>
       <c r="H912" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="913" spans="1:9" x14ac:dyDescent="0.3">
@@ -25499,10 +25595,10 @@
         <v>11</v>
       </c>
       <c r="H913" t="s">
-        <v>5</v>
+        <v>616</v>
       </c>
       <c r="I913" t="s">
-        <v>545</v>
+        <v>617</v>
       </c>
     </row>
     <row r="914" spans="1:9" x14ac:dyDescent="0.3">
@@ -25554,7 +25650,7 @@
         <v>3</v>
       </c>
       <c r="H915" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="916" spans="1:9" x14ac:dyDescent="0.3">
@@ -25580,10 +25676,10 @@
         <v>11</v>
       </c>
       <c r="H916" t="s">
-        <v>5</v>
+        <v>618</v>
       </c>
       <c r="I916" t="s">
-        <v>545</v>
+        <v>602</v>
       </c>
     </row>
     <row r="917" spans="1:9" x14ac:dyDescent="0.3">
@@ -25765,7 +25861,7 @@
         <v>5</v>
       </c>
       <c r="H923" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="924" spans="1:9" x14ac:dyDescent="0.3">
@@ -25895,7 +25991,7 @@
         <v>11</v>
       </c>
       <c r="H928" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="929" spans="1:9" x14ac:dyDescent="0.3">
@@ -25921,7 +26017,7 @@
         <v>5</v>
       </c>
       <c r="H929" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="930" spans="1:9" x14ac:dyDescent="0.3">
@@ -26025,7 +26121,7 @@
         <v>11</v>
       </c>
       <c r="H933" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="934" spans="1:9" x14ac:dyDescent="0.3">
@@ -26050,8 +26146,11 @@
       <c r="G934" t="s">
         <v>11</v>
       </c>
+      <c r="H934" t="s">
+        <v>619</v>
+      </c>
       <c r="I934" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="935" spans="1:9" x14ac:dyDescent="0.3">
@@ -26077,7 +26176,7 @@
         <v>3</v>
       </c>
       <c r="H935" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="936" spans="1:9" x14ac:dyDescent="0.3">
@@ -26155,7 +26254,7 @@
         <v>11</v>
       </c>
       <c r="H938" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="939" spans="1:9" x14ac:dyDescent="0.3">
@@ -26181,7 +26280,7 @@
         <v>5</v>
       </c>
       <c r="H939" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="940" spans="1:9" x14ac:dyDescent="0.3">
@@ -26232,8 +26331,11 @@
       <c r="G941" t="s">
         <v>11</v>
       </c>
+      <c r="H941" t="s">
+        <v>620</v>
+      </c>
       <c r="I941" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="942" spans="1:9" x14ac:dyDescent="0.3">
@@ -26259,7 +26361,7 @@
         <v>11</v>
       </c>
       <c r="H942" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="943" spans="1:9" x14ac:dyDescent="0.3">
@@ -26285,7 +26387,7 @@
         <v>5</v>
       </c>
       <c r="H943" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="944" spans="1:9" x14ac:dyDescent="0.3">
@@ -26311,7 +26413,7 @@
         <v>5</v>
       </c>
       <c r="H944" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="945" spans="1:9" x14ac:dyDescent="0.3">
@@ -26337,7 +26439,7 @@
         <v>5</v>
       </c>
       <c r="H945" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="946" spans="1:9" x14ac:dyDescent="0.3">
@@ -26467,7 +26569,7 @@
         <v>5</v>
       </c>
       <c r="H950" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="951" spans="1:9" x14ac:dyDescent="0.3">
@@ -26519,7 +26621,7 @@
         <v>5</v>
       </c>
       <c r="H952" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="953" spans="1:9" x14ac:dyDescent="0.3">
@@ -26623,10 +26725,10 @@
         <v>5</v>
       </c>
       <c r="H956" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="I956" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="957" spans="1:9" x14ac:dyDescent="0.3">
@@ -27067,8 +27169,11 @@
       <c r="G973" t="s">
         <v>11</v>
       </c>
+      <c r="H973" t="s">
+        <v>621</v>
+      </c>
       <c r="I973" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="974" spans="1:9" x14ac:dyDescent="0.3">
@@ -27120,10 +27225,10 @@
         <v>3</v>
       </c>
       <c r="H975" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="I975" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="976" spans="1:9" x14ac:dyDescent="0.3">
@@ -27175,7 +27280,7 @@
         <v>3</v>
       </c>
       <c r="H977" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="978" spans="1:9" x14ac:dyDescent="0.3">
@@ -27252,8 +27357,11 @@
       <c r="G980" t="s">
         <v>11</v>
       </c>
+      <c r="H980" t="s">
+        <v>622</v>
+      </c>
       <c r="I980" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="981" spans="1:9" x14ac:dyDescent="0.3">
@@ -27278,8 +27386,11 @@
       <c r="G981" t="s">
         <v>11</v>
       </c>
+      <c r="H981" t="s">
+        <v>623</v>
+      </c>
       <c r="I981" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="982" spans="1:9" x14ac:dyDescent="0.3">
@@ -27305,7 +27416,7 @@
         <v>11</v>
       </c>
       <c r="H982" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="983" spans="1:9" x14ac:dyDescent="0.3">
@@ -27334,7 +27445,7 @@
         <v>5</v>
       </c>
       <c r="I983" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="984" spans="1:9" x14ac:dyDescent="0.3">
@@ -27386,7 +27497,7 @@
         <v>5</v>
       </c>
       <c r="H985" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="986" spans="1:9" x14ac:dyDescent="0.3">
@@ -27490,7 +27601,7 @@
         <v>3</v>
       </c>
       <c r="H989" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="990" spans="1:9" x14ac:dyDescent="0.3">
@@ -27516,7 +27627,7 @@
         <v>3</v>
       </c>
       <c r="H990" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="991" spans="1:9" x14ac:dyDescent="0.3">
@@ -27594,7 +27705,7 @@
         <v>11</v>
       </c>
       <c r="H993" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="994" spans="1:9" x14ac:dyDescent="0.3">
@@ -27623,7 +27734,7 @@
         <v>5</v>
       </c>
       <c r="I994" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="995" spans="1:9" x14ac:dyDescent="0.3">
@@ -27701,10 +27812,10 @@
         <v>11</v>
       </c>
       <c r="H997" t="s">
-        <v>5</v>
+        <v>624</v>
       </c>
       <c r="I997" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="998" spans="1:9" x14ac:dyDescent="0.3">
@@ -27808,7 +27919,7 @@
         <v>3</v>
       </c>
       <c r="H1001" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="I1001" t="s">
         <v>464</v>
@@ -27941,7 +28052,7 @@
         <v>11</v>
       </c>
       <c r="H1006" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="1007" spans="1:9" x14ac:dyDescent="0.3">
@@ -28669,7 +28780,7 @@
         <v>11</v>
       </c>
       <c r="H1034" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="1035" spans="1:8" x14ac:dyDescent="0.3">
@@ -28851,7 +28962,7 @@
         <v>3</v>
       </c>
       <c r="H1041" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="1042" spans="1:9" x14ac:dyDescent="0.3">
@@ -28929,7 +29040,7 @@
         <v>11</v>
       </c>
       <c r="H1044" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="1045" spans="1:9" x14ac:dyDescent="0.3">
@@ -29085,10 +29196,10 @@
         <v>11</v>
       </c>
       <c r="H1050" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="I1050" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="1051" spans="1:9" x14ac:dyDescent="0.3">
@@ -29218,7 +29329,7 @@
         <v>3</v>
       </c>
       <c r="H1055" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="1056" spans="1:9" x14ac:dyDescent="0.3">
@@ -29296,7 +29407,7 @@
         <v>11</v>
       </c>
       <c r="H1058" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="1059" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Finished rescuing Arg both pos and neg
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80924479-22B2-4E09-B2AB-A72EC573ABB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4B05F8-3B70-49CA-9954-ACA2CB64239F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2220,7 +2220,7 @@
   <dimension ref="A1:I1084"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A982" workbookViewId="0">
-      <selection activeCell="H998" sqref="H998"/>
+      <selection activeCell="D991" sqref="D991"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Annotated GMP, needs rescuing
But surprisingly few!
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4B05F8-3B70-49CA-9954-ACA2CB64239F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF0FE8E-5B33-4393-BEBC-3C655B3702A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5313" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5597" uniqueCount="726">
   <si>
     <t>Amm</t>
   </si>
@@ -1900,6 +1900,309 @@
   </si>
   <si>
     <t>FT1387</t>
+  </si>
+  <si>
+    <t>FT0035</t>
+  </si>
+  <si>
+    <t>High background</t>
+  </si>
+  <si>
+    <t>FT0183</t>
+  </si>
+  <si>
+    <t>Peak looks kinda gross</t>
+  </si>
+  <si>
+    <t>FT0188</t>
+  </si>
+  <si>
+    <t>FT0408</t>
+  </si>
+  <si>
+    <t>FT0406</t>
+  </si>
+  <si>
+    <t>FT0407</t>
+  </si>
+  <si>
+    <t>Too spread out to trust integrations</t>
+  </si>
+  <si>
+    <t>FT0839</t>
+  </si>
+  <si>
+    <t>FT0933</t>
+  </si>
+  <si>
+    <t>FT1009</t>
+  </si>
+  <si>
+    <t>FT1071</t>
+  </si>
+  <si>
+    <t>FT1129</t>
+  </si>
+  <si>
+    <t>FT1209</t>
+  </si>
+  <si>
+    <t>Not sure which one this is</t>
+  </si>
+  <si>
+    <t>FT1223</t>
+  </si>
+  <si>
+    <t>FT1342</t>
+  </si>
+  <si>
+    <t>Rescue but looks gross</t>
+  </si>
+  <si>
+    <t>FT1434</t>
+  </si>
+  <si>
+    <t>FT1456</t>
+  </si>
+  <si>
+    <t>FT1460</t>
+  </si>
+  <si>
+    <t>FT1511</t>
+  </si>
+  <si>
+    <t>FT1579</t>
+  </si>
+  <si>
+    <t>FT1597</t>
+  </si>
+  <si>
+    <t>FT1613</t>
+  </si>
+  <si>
+    <t>FT1632</t>
+  </si>
+  <si>
+    <t>FT1650</t>
+  </si>
+  <si>
+    <t>FT1649</t>
+  </si>
+  <si>
+    <t>FT1699</t>
+  </si>
+  <si>
+    <t>FT1698</t>
+  </si>
+  <si>
+    <t>FT1725</t>
+  </si>
+  <si>
+    <t>FT1952</t>
+  </si>
+  <si>
+    <t>FT1987</t>
+  </si>
+  <si>
+    <t>FT2069</t>
+  </si>
+  <si>
+    <t>FT2070</t>
+  </si>
+  <si>
+    <t>FT2091</t>
+  </si>
+  <si>
+    <t>FT2096</t>
+  </si>
+  <si>
+    <t>FT2114</t>
+  </si>
+  <si>
+    <t>FT2165</t>
+  </si>
+  <si>
+    <t>FT2221</t>
+  </si>
+  <si>
+    <t>FT2220</t>
+  </si>
+  <si>
+    <t>FT2291</t>
+  </si>
+  <si>
+    <t>FT2428</t>
+  </si>
+  <si>
+    <t>FT2448</t>
+  </si>
+  <si>
+    <t>FT2484</t>
+  </si>
+  <si>
+    <t>FT2489</t>
+  </si>
+  <si>
+    <t>FT2491</t>
+  </si>
+  <si>
+    <t>FT2490</t>
+  </si>
+  <si>
+    <t>FT2636</t>
+  </si>
+  <si>
+    <t>Peak doesn't match RT</t>
+  </si>
+  <si>
+    <t>FT2698</t>
+  </si>
+  <si>
+    <t>FT2808</t>
+  </si>
+  <si>
+    <t>FT2809</t>
+  </si>
+  <si>
+    <t>FT2825</t>
+  </si>
+  <si>
+    <t>FT2874</t>
+  </si>
+  <si>
+    <t>FT2877</t>
+  </si>
+  <si>
+    <t>FT2995</t>
+  </si>
+  <si>
+    <t>FT3031</t>
+  </si>
+  <si>
+    <t>FT3092</t>
+  </si>
+  <si>
+    <t>FT3371</t>
+  </si>
+  <si>
+    <t>FT3821</t>
+  </si>
+  <si>
+    <t>FT3851</t>
+  </si>
+  <si>
+    <t>FT4169</t>
+  </si>
+  <si>
+    <t>FT4205</t>
+  </si>
+  <si>
+    <t>FT4212</t>
+  </si>
+  <si>
+    <t>Peak is at wront RT</t>
+  </si>
+  <si>
+    <t>FT4314</t>
+  </si>
+  <si>
+    <t>FT4397</t>
+  </si>
+  <si>
+    <t>FT4527</t>
+  </si>
+  <si>
+    <t>FT4528</t>
+  </si>
+  <si>
+    <t>FT4556</t>
+  </si>
+  <si>
+    <t>FT4677</t>
+  </si>
+  <si>
+    <t>FT4704</t>
+  </si>
+  <si>
+    <t>FT4703</t>
+  </si>
+  <si>
+    <t>FT4721</t>
+  </si>
+  <si>
+    <t>FT4839</t>
+  </si>
+  <si>
+    <t>FT5072</t>
+  </si>
+  <si>
+    <t>FT5191</t>
+  </si>
+  <si>
+    <t>Second peak at 10.5 also interesting</t>
+  </si>
+  <si>
+    <t>FT1089</t>
+  </si>
+  <si>
+    <t>FT0202</t>
+  </si>
+  <si>
+    <t>FT1010</t>
+  </si>
+  <si>
+    <t>FT1164</t>
+  </si>
+  <si>
+    <t>FT1172, FT1174</t>
+  </si>
+  <si>
+    <t>Split across two feats</t>
+  </si>
+  <si>
+    <t>FT1250</t>
+  </si>
+  <si>
+    <t>FT1370</t>
+  </si>
+  <si>
+    <t>FT1400</t>
+  </si>
+  <si>
+    <t>FT1445</t>
+  </si>
+  <si>
+    <t>FT1532</t>
+  </si>
+  <si>
+    <t>FT1702</t>
+  </si>
+  <si>
+    <t>FT1799</t>
+  </si>
+  <si>
+    <t>FT2156</t>
+  </si>
+  <si>
+    <t>FT2336</t>
+  </si>
+  <si>
+    <t>FT3077</t>
+  </si>
+  <si>
+    <t>FT3080</t>
+  </si>
+  <si>
+    <t>FT3090</t>
+  </si>
+  <si>
+    <t>FT3236</t>
+  </si>
+  <si>
+    <t>FT3575</t>
+  </si>
+  <si>
+    <t>FT3574</t>
   </si>
 </sst>
 </file>
@@ -2219,8 +2522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1084"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A982" workbookViewId="0">
-      <selection activeCell="D991" sqref="D991"/>
+    <sheetView tabSelected="1" topLeftCell="A792" workbookViewId="0">
+      <selection activeCell="J811" sqref="J811"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16763,7 +17066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="545" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A545" t="s">
         <v>245</v>
       </c>
@@ -16785,8 +17088,11 @@
       <c r="G545" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="546" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H545" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="546" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A546" t="s">
         <v>245</v>
       </c>
@@ -16808,8 +17114,11 @@
       <c r="G546" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="547" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H546" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="547" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
         <v>245</v>
       </c>
@@ -16831,8 +17140,14 @@
       <c r="G547" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="548" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H547" t="s">
+        <v>625</v>
+      </c>
+      <c r="I547" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="548" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A548" t="s">
         <v>245</v>
       </c>
@@ -16854,8 +17169,11 @@
       <c r="G548" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="549" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H548" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="549" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A549" t="s">
         <v>245</v>
       </c>
@@ -16877,8 +17195,14 @@
       <c r="G549" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="550" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H549" t="s">
+        <v>627</v>
+      </c>
+      <c r="I549" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="550" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A550" t="s">
         <v>245</v>
       </c>
@@ -16900,8 +17224,11 @@
       <c r="G550" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="551" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H550" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="551" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A551" t="s">
         <v>245</v>
       </c>
@@ -16923,8 +17250,11 @@
       <c r="G551" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="552" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H551" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="552" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A552" t="s">
         <v>245</v>
       </c>
@@ -16946,8 +17276,11 @@
       <c r="G552" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="553" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H552" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="553" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A553" t="s">
         <v>245</v>
       </c>
@@ -16969,8 +17302,11 @@
       <c r="G553" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="554" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H553" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="554" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A554" t="s">
         <v>245</v>
       </c>
@@ -16992,8 +17328,11 @@
       <c r="G554" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="555" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H554" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="555" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A555" t="s">
         <v>245</v>
       </c>
@@ -17015,8 +17354,11 @@
       <c r="G555" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="556" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H555" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="556" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A556" t="s">
         <v>245</v>
       </c>
@@ -17038,8 +17380,14 @@
       <c r="G556" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="557" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H556" t="s">
+        <v>5</v>
+      </c>
+      <c r="I556" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="557" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A557" t="s">
         <v>245</v>
       </c>
@@ -17061,8 +17409,11 @@
       <c r="G557" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="558" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H557" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="558" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A558" t="s">
         <v>245</v>
       </c>
@@ -17084,8 +17435,11 @@
       <c r="G558" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="559" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H558" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="559" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A559" t="s">
         <v>245</v>
       </c>
@@ -17107,8 +17461,11 @@
       <c r="G559" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="560" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H559" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="560" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A560" t="s">
         <v>245</v>
       </c>
@@ -17130,8 +17487,11 @@
       <c r="G560" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="561" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H560" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="561" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A561" t="s">
         <v>245</v>
       </c>
@@ -17153,8 +17513,11 @@
       <c r="G561" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="562" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H561" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="562" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A562" t="s">
         <v>245</v>
       </c>
@@ -17176,8 +17539,11 @@
       <c r="G562" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="563" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H562" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="563" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A563" t="s">
         <v>245</v>
       </c>
@@ -17199,8 +17565,11 @@
       <c r="G563" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="564" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H563" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="564" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A564" t="s">
         <v>245</v>
       </c>
@@ -17222,8 +17591,11 @@
       <c r="G564" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="565" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H564" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="565" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A565" t="s">
         <v>245</v>
       </c>
@@ -17245,8 +17617,11 @@
       <c r="G565" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="566" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H565" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="566" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A566" t="s">
         <v>245</v>
       </c>
@@ -17268,8 +17643,14 @@
       <c r="G566" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="567" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H566" t="s">
+        <v>639</v>
+      </c>
+      <c r="I566" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="567" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A567" t="s">
         <v>245</v>
       </c>
@@ -17291,8 +17672,11 @@
       <c r="G567" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="568" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H567" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="568" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A568" t="s">
         <v>245</v>
       </c>
@@ -17314,8 +17698,11 @@
       <c r="G568" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="569" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H568" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="569" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A569" t="s">
         <v>245</v>
       </c>
@@ -17337,8 +17724,11 @@
       <c r="G569" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="570" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H569" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="570" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A570" t="s">
         <v>245</v>
       </c>
@@ -17360,8 +17750,11 @@
       <c r="G570" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="571" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H570" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="571" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A571" t="s">
         <v>245</v>
       </c>
@@ -17383,8 +17776,11 @@
       <c r="G571" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="572" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H571" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="572" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A572" t="s">
         <v>245</v>
       </c>
@@ -17406,8 +17802,11 @@
       <c r="G572" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="573" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H572" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="573" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A573" t="s">
         <v>245</v>
       </c>
@@ -17429,8 +17828,11 @@
       <c r="G573" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="574" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I573" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="574" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A574" t="s">
         <v>245</v>
       </c>
@@ -17452,8 +17854,11 @@
       <c r="G574" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="575" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H574" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="575" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A575" t="s">
         <v>245</v>
       </c>
@@ -17475,8 +17880,11 @@
       <c r="G575" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="576" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H575" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="576" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A576" t="s">
         <v>245</v>
       </c>
@@ -17498,8 +17906,11 @@
       <c r="G576" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="577" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H576" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="577" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
         <v>245</v>
       </c>
@@ -17521,8 +17932,14 @@
       <c r="G577" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="578" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H577" t="s">
+        <v>647</v>
+      </c>
+      <c r="I577" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="578" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
         <v>245</v>
       </c>
@@ -17544,8 +17961,11 @@
       <c r="G578" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="579" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H578" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="579" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A579" t="s">
         <v>245</v>
       </c>
@@ -17567,8 +17987,11 @@
       <c r="G579" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="580" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H579" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="580" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
         <v>245</v>
       </c>
@@ -17590,8 +18013,11 @@
       <c r="G580" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="581" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H580" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="581" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
         <v>245</v>
       </c>
@@ -17613,8 +18039,11 @@
       <c r="G581" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="582" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I581" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="582" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
         <v>245</v>
       </c>
@@ -17636,8 +18065,11 @@
       <c r="G582" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="583" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I582" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="583" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
         <v>245</v>
       </c>
@@ -17659,8 +18091,11 @@
       <c r="G583" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="584" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H583" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="584" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
         <v>245</v>
       </c>
@@ -17682,8 +18117,14 @@
       <c r="G584" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="585" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H584" t="s">
+        <v>649</v>
+      </c>
+      <c r="I584" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="585" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
         <v>245</v>
       </c>
@@ -17705,8 +18146,11 @@
       <c r="G585" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="586" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I585" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="586" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
         <v>245</v>
       </c>
@@ -17728,8 +18172,11 @@
       <c r="G586" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="587" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H586" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="587" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
         <v>245</v>
       </c>
@@ -17751,8 +18198,11 @@
       <c r="G587" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="588" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H587" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="588" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
         <v>245</v>
       </c>
@@ -17774,8 +18224,11 @@
       <c r="G588" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="589" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H588" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="589" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
         <v>245</v>
       </c>
@@ -17797,8 +18250,11 @@
       <c r="G589" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="590" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H589" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="590" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A590" t="s">
         <v>245</v>
       </c>
@@ -17820,8 +18276,11 @@
       <c r="G590" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="591" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H590" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="591" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A591" t="s">
         <v>245</v>
       </c>
@@ -17843,8 +18302,11 @@
       <c r="G591" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="592" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H591" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="592" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A592" t="s">
         <v>245</v>
       </c>
@@ -17866,8 +18328,11 @@
       <c r="G592" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="593" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H592" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="593" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A593" t="s">
         <v>245</v>
       </c>
@@ -17889,8 +18354,11 @@
       <c r="G593" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="594" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H593" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="594" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A594" t="s">
         <v>245</v>
       </c>
@@ -17912,8 +18380,11 @@
       <c r="G594" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="595" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H594" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="595" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A595" t="s">
         <v>245</v>
       </c>
@@ -17935,8 +18406,11 @@
       <c r="G595" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="596" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H595" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="596" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A596" t="s">
         <v>245</v>
       </c>
@@ -17958,8 +18432,11 @@
       <c r="G596" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="597" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H596" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="597" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A597" t="s">
         <v>245</v>
       </c>
@@ -17981,8 +18458,11 @@
       <c r="G597" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="598" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H597" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="598" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A598" t="s">
         <v>245</v>
       </c>
@@ -18004,8 +18484,11 @@
       <c r="G598" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="599" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H598" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="599" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A599" t="s">
         <v>245</v>
       </c>
@@ -18027,8 +18510,11 @@
       <c r="G599" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="600" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H599" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="600" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A600" t="s">
         <v>245</v>
       </c>
@@ -18050,8 +18536,11 @@
       <c r="G600" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="601" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H600" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="601" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A601" t="s">
         <v>245</v>
       </c>
@@ -18073,8 +18562,11 @@
       <c r="G601" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="602" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H601" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="602" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A602" t="s">
         <v>245</v>
       </c>
@@ -18096,8 +18588,11 @@
       <c r="G602" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="603" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H602" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="603" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A603" t="s">
         <v>245</v>
       </c>
@@ -18119,8 +18614,11 @@
       <c r="G603" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="604" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H603" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="604" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A604" t="s">
         <v>245</v>
       </c>
@@ -18142,8 +18640,11 @@
       <c r="G604" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="605" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H604" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="605" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A605" t="s">
         <v>245</v>
       </c>
@@ -18165,8 +18666,11 @@
       <c r="G605" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="606" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H605" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="606" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A606" t="s">
         <v>245</v>
       </c>
@@ -18188,8 +18692,11 @@
       <c r="G606" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="607" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H606" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="607" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A607" t="s">
         <v>245</v>
       </c>
@@ -18211,8 +18718,11 @@
       <c r="G607" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="608" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H607" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="608" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A608" t="s">
         <v>245</v>
       </c>
@@ -18234,8 +18744,11 @@
       <c r="G608" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="609" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H608" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="609" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A609" t="s">
         <v>245</v>
       </c>
@@ -18257,8 +18770,11 @@
       <c r="G609" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="610" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H609" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="610" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A610" t="s">
         <v>245</v>
       </c>
@@ -18280,8 +18796,11 @@
       <c r="G610" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="611" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H610" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="611" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A611" t="s">
         <v>245</v>
       </c>
@@ -18303,8 +18822,11 @@
       <c r="G611" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="612" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H611" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="612" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A612" t="s">
         <v>245</v>
       </c>
@@ -18326,8 +18848,11 @@
       <c r="G612" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="613" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H612" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="613" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A613" t="s">
         <v>245</v>
       </c>
@@ -18349,8 +18874,11 @@
       <c r="G613" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="614" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H613" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="614" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A614" t="s">
         <v>245</v>
       </c>
@@ -18372,8 +18900,11 @@
       <c r="G614" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="615" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H614" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="615" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A615" t="s">
         <v>245</v>
       </c>
@@ -18395,8 +18926,11 @@
       <c r="G615" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="616" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H615" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="616" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A616" t="s">
         <v>245</v>
       </c>
@@ -18418,8 +18952,11 @@
       <c r="G616" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="617" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H616" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="617" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A617" t="s">
         <v>245</v>
       </c>
@@ -18441,8 +18978,14 @@
       <c r="G617" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="618" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H617" t="s">
+        <v>668</v>
+      </c>
+      <c r="I617" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="618" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A618" t="s">
         <v>245</v>
       </c>
@@ -18464,8 +19007,11 @@
       <c r="G618" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="619" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H618" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="619" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A619" t="s">
         <v>245</v>
       </c>
@@ -18487,8 +19033,11 @@
       <c r="G619" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="620" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H619" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="620" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A620" t="s">
         <v>245</v>
       </c>
@@ -18510,8 +19059,14 @@
       <c r="G620" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="621" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H620" t="s">
+        <v>670</v>
+      </c>
+      <c r="I620" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="621" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A621" t="s">
         <v>245</v>
       </c>
@@ -18533,8 +19088,11 @@
       <c r="G621" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="622" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H621" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="622" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A622" t="s">
         <v>245</v>
       </c>
@@ -18556,8 +19114,11 @@
       <c r="G622" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="623" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H622" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="623" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A623" t="s">
         <v>245</v>
       </c>
@@ -18579,8 +19140,11 @@
       <c r="G623" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="624" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H623" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="624" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A624" t="s">
         <v>245</v>
       </c>
@@ -18602,8 +19166,11 @@
       <c r="G624" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="625" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H624" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="625" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A625" t="s">
         <v>245</v>
       </c>
@@ -18625,8 +19192,11 @@
       <c r="G625" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="626" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H625" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="626" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A626" t="s">
         <v>245</v>
       </c>
@@ -18648,8 +19218,11 @@
       <c r="G626" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="627" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H626" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="627" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A627" t="s">
         <v>245</v>
       </c>
@@ -18671,8 +19244,14 @@
       <c r="G627" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="628" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H627" t="s">
+        <v>5</v>
+      </c>
+      <c r="I627" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="628" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A628" t="s">
         <v>245</v>
       </c>
@@ -18694,8 +19273,11 @@
       <c r="G628" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="629" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H628" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="629" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A629" t="s">
         <v>245</v>
       </c>
@@ -18717,8 +19299,11 @@
       <c r="G629" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="630" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H629" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="630" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A630" t="s">
         <v>245</v>
       </c>
@@ -18740,8 +19325,11 @@
       <c r="G630" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="631" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H630" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="631" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A631" t="s">
         <v>245</v>
       </c>
@@ -18763,8 +19351,11 @@
       <c r="G631" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="632" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H631" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="632" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A632" t="s">
         <v>245</v>
       </c>
@@ -18786,8 +19377,11 @@
       <c r="G632" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="633" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H632" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="633" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A633" t="s">
         <v>245</v>
       </c>
@@ -18809,8 +19403,11 @@
       <c r="G633" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="634" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H633" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="634" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A634" t="s">
         <v>245</v>
       </c>
@@ -18832,8 +19429,11 @@
       <c r="G634" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="635" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H634" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="635" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A635" t="s">
         <v>245</v>
       </c>
@@ -18855,8 +19455,11 @@
       <c r="G635" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="636" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H635" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="636" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A636" t="s">
         <v>245</v>
       </c>
@@ -18878,8 +19481,11 @@
       <c r="G636" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="637" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H636" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="637" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A637" t="s">
         <v>245</v>
       </c>
@@ -18901,8 +19507,11 @@
       <c r="G637" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="638" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H637" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="638" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A638" t="s">
         <v>245</v>
       </c>
@@ -18924,8 +19533,11 @@
       <c r="G638" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="639" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H638" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="639" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A639" t="s">
         <v>245</v>
       </c>
@@ -18947,8 +19559,11 @@
       <c r="G639" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="640" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H639" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="640" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A640" t="s">
         <v>245</v>
       </c>
@@ -18970,8 +19585,11 @@
       <c r="G640" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="641" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I640" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="641" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A641" t="s">
         <v>245</v>
       </c>
@@ -18993,8 +19611,11 @@
       <c r="G641" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="642" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H641" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="642" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A642" t="s">
         <v>245</v>
       </c>
@@ -19016,8 +19637,11 @@
       <c r="G642" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="643" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H642" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="643" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A643" t="s">
         <v>245</v>
       </c>
@@ -19039,8 +19663,11 @@
       <c r="G643" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="644" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H643" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="644" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A644" t="s">
         <v>245</v>
       </c>
@@ -19062,8 +19689,11 @@
       <c r="G644" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="645" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H644" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="645" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A645" t="s">
         <v>245</v>
       </c>
@@ -19085,8 +19715,11 @@
       <c r="G645" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="646" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H645" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="646" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A646" t="s">
         <v>245</v>
       </c>
@@ -19108,8 +19741,11 @@
       <c r="G646" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="647" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H646" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="647" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A647" t="s">
         <v>245</v>
       </c>
@@ -19131,8 +19767,11 @@
       <c r="G647" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="648" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H647" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="648" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A648" t="s">
         <v>245</v>
       </c>
@@ -19154,8 +19793,11 @@
       <c r="G648" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="649" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H648" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="649" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A649" t="s">
         <v>245</v>
       </c>
@@ -19177,8 +19819,11 @@
       <c r="G649" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="650" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H649" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="650" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A650" t="s">
         <v>245</v>
       </c>
@@ -19200,8 +19845,11 @@
       <c r="G650" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="651" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H650" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="651" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A651" t="s">
         <v>245</v>
       </c>
@@ -19223,8 +19871,11 @@
       <c r="G651" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="652" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H651" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="652" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A652" t="s">
         <v>245</v>
       </c>
@@ -19246,8 +19897,11 @@
       <c r="G652" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="653" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H652" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="653" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A653" t="s">
         <v>245</v>
       </c>
@@ -19269,8 +19923,11 @@
       <c r="G653" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="654" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H653" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="654" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A654" t="s">
         <v>245</v>
       </c>
@@ -19292,8 +19949,11 @@
       <c r="G654" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="655" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H654" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="655" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A655" t="s">
         <v>245</v>
       </c>
@@ -19315,8 +19975,11 @@
       <c r="G655" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="656" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H655" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="656" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A656" t="s">
         <v>245</v>
       </c>
@@ -19338,8 +20001,11 @@
       <c r="G656" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="657" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H656" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="657" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A657" t="s">
         <v>245</v>
       </c>
@@ -19361,8 +20027,11 @@
       <c r="G657" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="658" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H657" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="658" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A658" t="s">
         <v>245</v>
       </c>
@@ -19384,8 +20053,11 @@
       <c r="G658" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="659" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H658" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="659" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A659" t="s">
         <v>245</v>
       </c>
@@ -19407,8 +20079,11 @@
       <c r="G659" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="660" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H659" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="660" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A660" t="s">
         <v>245</v>
       </c>
@@ -19430,8 +20105,11 @@
       <c r="G660" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="661" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H660" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="661" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A661" t="s">
         <v>245</v>
       </c>
@@ -19453,8 +20131,11 @@
       <c r="G661" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="662" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H661" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="662" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A662" t="s">
         <v>245</v>
       </c>
@@ -19476,8 +20157,14 @@
       <c r="G662" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="663" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H662" t="s">
+        <v>5</v>
+      </c>
+      <c r="I662" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="663" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A663" t="s">
         <v>245</v>
       </c>
@@ -19499,8 +20186,11 @@
       <c r="G663" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="664" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H663" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="664" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A664" t="s">
         <v>245</v>
       </c>
@@ -19522,8 +20212,11 @@
       <c r="G664" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="665" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H664" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="665" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A665" t="s">
         <v>245</v>
       </c>
@@ -19545,8 +20238,11 @@
       <c r="G665" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="666" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H665" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="666" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A666" t="s">
         <v>245</v>
       </c>
@@ -19568,8 +20264,11 @@
       <c r="G666" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="667" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H666" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="667" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A667" t="s">
         <v>245</v>
       </c>
@@ -19591,8 +20290,11 @@
       <c r="G667" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="668" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H667" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="668" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A668" t="s">
         <v>245</v>
       </c>
@@ -19614,8 +20316,11 @@
       <c r="G668" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="669" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H668" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="669" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A669" t="s">
         <v>245</v>
       </c>
@@ -19637,8 +20342,11 @@
       <c r="G669" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="670" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H669" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="670" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A670" t="s">
         <v>245</v>
       </c>
@@ -19660,8 +20368,11 @@
       <c r="G670" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="671" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H670" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="671" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A671" t="s">
         <v>245</v>
       </c>
@@ -19683,8 +20394,11 @@
       <c r="G671" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="672" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H671" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="672" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A672" t="s">
         <v>245</v>
       </c>
@@ -19706,8 +20420,11 @@
       <c r="G672" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="673" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H672" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="673" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A673" t="s">
         <v>245</v>
       </c>
@@ -19729,8 +20446,11 @@
       <c r="G673" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="674" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H673" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="674" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A674" t="s">
         <v>245</v>
       </c>
@@ -19752,8 +20472,11 @@
       <c r="G674" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="675" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H674" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="675" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A675" t="s">
         <v>245</v>
       </c>
@@ -19775,8 +20498,11 @@
       <c r="G675" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="676" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H675" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="676" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A676" t="s">
         <v>245</v>
       </c>
@@ -19798,8 +20524,11 @@
       <c r="G676" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="677" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H676" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="677" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A677" t="s">
         <v>245</v>
       </c>
@@ -19821,8 +20550,11 @@
       <c r="G677" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="678" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H677" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="678" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A678" t="s">
         <v>245</v>
       </c>
@@ -19844,8 +20576,11 @@
       <c r="G678" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="679" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H678" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="679" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A679" t="s">
         <v>245</v>
       </c>
@@ -19867,8 +20602,11 @@
       <c r="G679" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="680" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H679" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="680" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A680" t="s">
         <v>245</v>
       </c>
@@ -19890,8 +20628,11 @@
       <c r="G680" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="681" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H680" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="681" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A681" t="s">
         <v>245</v>
       </c>
@@ -19913,8 +20654,11 @@
       <c r="G681" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="682" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H681" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="682" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A682" t="s">
         <v>245</v>
       </c>
@@ -19936,8 +20680,11 @@
       <c r="G682" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="683" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H682" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="683" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A683" t="s">
         <v>245</v>
       </c>
@@ -19959,8 +20706,11 @@
       <c r="G683" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="684" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H683" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="684" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A684" t="s">
         <v>245</v>
       </c>
@@ -19982,8 +20732,11 @@
       <c r="G684" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="685" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H684" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="685" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A685" t="s">
         <v>245</v>
       </c>
@@ -20005,8 +20758,11 @@
       <c r="G685" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="686" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H685" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="686" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A686" t="s">
         <v>245</v>
       </c>
@@ -20028,8 +20784,14 @@
       <c r="G686" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="687" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H686" t="s">
+        <v>703</v>
+      </c>
+      <c r="I686" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="687" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A687" t="s">
         <v>245</v>
       </c>
@@ -20051,8 +20813,11 @@
       <c r="G687" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="688" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H687" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="688" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A688" t="s">
         <v>245</v>
       </c>
@@ -20074,8 +20839,11 @@
       <c r="G688" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="689" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H688" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="689" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A689" t="s">
         <v>245</v>
       </c>
@@ -20097,8 +20865,11 @@
       <c r="G689" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="690" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H689" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="690" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A690" t="s">
         <v>245</v>
       </c>
@@ -20120,8 +20891,11 @@
       <c r="G690" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="691" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H690" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="691" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A691" t="s">
         <v>245</v>
       </c>
@@ -20143,8 +20917,11 @@
       <c r="G691" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="692" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H691" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="692" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A692" t="s">
         <v>245</v>
       </c>
@@ -20166,8 +20943,11 @@
       <c r="G692" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="693" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H692" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="693" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A693" t="s">
         <v>245</v>
       </c>
@@ -20189,8 +20969,11 @@
       <c r="G693" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="694" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H693" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="694" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A694" t="s">
         <v>245</v>
       </c>
@@ -20212,8 +20995,11 @@
       <c r="G694" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="695" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H694" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="695" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A695" t="s">
         <v>245</v>
       </c>
@@ -20235,8 +21021,11 @@
       <c r="G695" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="696" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H695" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="696" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A696" t="s">
         <v>245</v>
       </c>
@@ -20258,8 +21047,11 @@
       <c r="G696" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="697" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H696" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="697" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A697" t="s">
         <v>245</v>
       </c>
@@ -20281,8 +21073,11 @@
       <c r="G697" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="698" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H697" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="698" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A698" t="s">
         <v>245</v>
       </c>
@@ -20304,8 +21099,11 @@
       <c r="G698" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="699" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H698" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="699" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A699" t="s">
         <v>245</v>
       </c>
@@ -20327,8 +21125,11 @@
       <c r="G699" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="700" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H699" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="700" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A700" t="s">
         <v>245</v>
       </c>
@@ -20350,8 +21151,11 @@
       <c r="G700" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="701" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H700" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="701" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A701" t="s">
         <v>245</v>
       </c>
@@ -20373,8 +21177,11 @@
       <c r="G701" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="702" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H701" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="702" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A702" t="s">
         <v>245</v>
       </c>
@@ -20396,8 +21203,11 @@
       <c r="G702" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="703" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H702" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="703" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A703" t="s">
         <v>245</v>
       </c>
@@ -20419,8 +21229,11 @@
       <c r="G703" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="704" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I703" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="704" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A704" t="s">
         <v>245</v>
       </c>
@@ -20442,8 +21255,11 @@
       <c r="G704" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="705" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H704" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="705" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A705" t="s">
         <v>245</v>
       </c>
@@ -20465,8 +21281,14 @@
       <c r="G705" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="706" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H705" t="s">
+        <v>5</v>
+      </c>
+      <c r="I705" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="706" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A706" t="s">
         <v>245</v>
       </c>
@@ -20488,8 +21310,11 @@
       <c r="G706" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="707" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H706" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="707" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A707" t="s">
         <v>245</v>
       </c>
@@ -20511,8 +21336,11 @@
       <c r="G707" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="708" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H707" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="708" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A708" t="s">
         <v>245</v>
       </c>
@@ -20534,8 +21362,11 @@
       <c r="G708" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="709" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H708" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="709" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A709" t="s">
         <v>245</v>
       </c>
@@ -20557,8 +21388,11 @@
       <c r="G709" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="710" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H709" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="710" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A710" t="s">
         <v>245</v>
       </c>
@@ -20580,8 +21414,11 @@
       <c r="G710" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="711" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H710" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="711" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A711" t="s">
         <v>245</v>
       </c>
@@ -20603,8 +21440,14 @@
       <c r="G711" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="712" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H711" t="s">
+        <v>709</v>
+      </c>
+      <c r="I711" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="712" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A712" t="s">
         <v>245</v>
       </c>
@@ -20626,8 +21469,11 @@
       <c r="G712" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="713" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H712" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="713" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A713" t="s">
         <v>245</v>
       </c>
@@ -20649,8 +21495,11 @@
       <c r="G713" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="714" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H713" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="714" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A714" t="s">
         <v>245</v>
       </c>
@@ -20672,8 +21521,11 @@
       <c r="G714" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="715" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H714" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="715" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A715" t="s">
         <v>245</v>
       </c>
@@ -20695,8 +21547,11 @@
       <c r="G715" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="716" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H715" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="716" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A716" t="s">
         <v>245</v>
       </c>
@@ -20718,8 +21573,11 @@
       <c r="G716" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="717" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H716" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="717" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A717" t="s">
         <v>245</v>
       </c>
@@ -20741,8 +21599,11 @@
       <c r="G717" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="718" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H717" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="718" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A718" t="s">
         <v>245</v>
       </c>
@@ -20764,8 +21625,11 @@
       <c r="G718" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="719" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H718" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="719" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A719" t="s">
         <v>245</v>
       </c>
@@ -20787,8 +21651,11 @@
       <c r="G719" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="720" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H719" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="720" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A720" t="s">
         <v>245</v>
       </c>
@@ -20810,8 +21677,11 @@
       <c r="G720" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="721" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H720" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="721" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A721" t="s">
         <v>245</v>
       </c>
@@ -20833,8 +21703,11 @@
       <c r="G721" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="722" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H721" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="722" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A722" t="s">
         <v>245</v>
       </c>
@@ -20856,8 +21729,11 @@
       <c r="G722" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="723" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H722" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="723" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A723" t="s">
         <v>245</v>
       </c>
@@ -20879,8 +21755,11 @@
       <c r="G723" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="724" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H723" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="724" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A724" t="s">
         <v>245</v>
       </c>
@@ -20902,8 +21781,11 @@
       <c r="G724" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="725" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H724" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="725" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A725" t="s">
         <v>245</v>
       </c>
@@ -20925,8 +21807,11 @@
       <c r="G725" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="726" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H725" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="726" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A726" t="s">
         <v>245</v>
       </c>
@@ -20948,8 +21833,11 @@
       <c r="G726" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="727" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H726" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="727" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A727" t="s">
         <v>245</v>
       </c>
@@ -20971,8 +21859,11 @@
       <c r="G727" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="728" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H727" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="728" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A728" t="s">
         <v>245</v>
       </c>
@@ -20994,8 +21885,11 @@
       <c r="G728" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="729" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H728" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="729" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A729" t="s">
         <v>245</v>
       </c>
@@ -21017,8 +21911,11 @@
       <c r="G729" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="730" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H729" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="730" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A730" t="s">
         <v>245</v>
       </c>
@@ -21040,8 +21937,11 @@
       <c r="G730" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="731" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H730" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="731" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A731" t="s">
         <v>245</v>
       </c>
@@ -21063,8 +21963,11 @@
       <c r="G731" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="732" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H731" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="732" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A732" t="s">
         <v>245</v>
       </c>
@@ -21086,8 +21989,11 @@
       <c r="G732" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="733" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H732" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="733" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A733" t="s">
         <v>245</v>
       </c>
@@ -21109,8 +22015,11 @@
       <c r="G733" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="734" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H733" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="734" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A734" t="s">
         <v>245</v>
       </c>
@@ -21132,8 +22041,11 @@
       <c r="G734" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="735" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H734" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="735" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A735" t="s">
         <v>245</v>
       </c>
@@ -21155,8 +22067,11 @@
       <c r="G735" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="736" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H735" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="736" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A736" t="s">
         <v>245</v>
       </c>
@@ -21178,8 +22093,11 @@
       <c r="G736" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="737" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H736" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="737" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A737" t="s">
         <v>245</v>
       </c>
@@ -21201,8 +22119,11 @@
       <c r="G737" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="738" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H737" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="738" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A738" t="s">
         <v>245</v>
       </c>
@@ -21224,8 +22145,11 @@
       <c r="G738" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="739" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H738" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="739" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A739" t="s">
         <v>245</v>
       </c>
@@ -21247,8 +22171,11 @@
       <c r="G739" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="740" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H739" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="740" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A740" t="s">
         <v>245</v>
       </c>
@@ -21270,8 +22197,11 @@
       <c r="G740" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="741" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H740" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="741" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A741" t="s">
         <v>245</v>
       </c>
@@ -21293,8 +22223,11 @@
       <c r="G741" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="742" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H741" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="742" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A742" t="s">
         <v>245</v>
       </c>
@@ -21316,8 +22249,11 @@
       <c r="G742" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="743" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H742" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="743" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A743" t="s">
         <v>245</v>
       </c>
@@ -21339,8 +22275,11 @@
       <c r="G743" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="744" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H743" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="744" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A744" t="s">
         <v>245</v>
       </c>
@@ -21362,8 +22301,11 @@
       <c r="G744" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="745" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H744" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="745" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A745" t="s">
         <v>245</v>
       </c>
@@ -21385,8 +22327,11 @@
       <c r="G745" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="746" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H745" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="746" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A746" t="s">
         <v>245</v>
       </c>
@@ -21408,8 +22353,11 @@
       <c r="G746" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="747" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H746" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="747" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A747" t="s">
         <v>245</v>
       </c>
@@ -21431,8 +22379,11 @@
       <c r="G747" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="748" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H747" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="748" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A748" t="s">
         <v>245</v>
       </c>
@@ -21454,8 +22405,11 @@
       <c r="G748" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="749" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H748" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="749" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A749" t="s">
         <v>245</v>
       </c>
@@ -21477,8 +22431,11 @@
       <c r="G749" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="750" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H749" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="750" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A750" t="s">
         <v>245</v>
       </c>
@@ -21500,8 +22457,11 @@
       <c r="G750" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="751" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H750" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="751" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A751" t="s">
         <v>245</v>
       </c>
@@ -21523,8 +22483,11 @@
       <c r="G751" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="752" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H751" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="752" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A752" t="s">
         <v>245</v>
       </c>
@@ -21546,8 +22509,11 @@
       <c r="G752" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="753" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H752" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="753" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A753" t="s">
         <v>245</v>
       </c>
@@ -21569,8 +22535,11 @@
       <c r="G753" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="754" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H753" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="754" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A754" t="s">
         <v>245</v>
       </c>
@@ -21592,8 +22561,11 @@
       <c r="G754" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="755" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H754" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="755" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A755" t="s">
         <v>245</v>
       </c>
@@ -21615,8 +22587,11 @@
       <c r="G755" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="756" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H755" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="756" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A756" t="s">
         <v>245</v>
       </c>
@@ -21638,8 +22613,11 @@
       <c r="G756" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="757" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H756" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="757" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A757" t="s">
         <v>245</v>
       </c>
@@ -21661,8 +22639,11 @@
       <c r="G757" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="758" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H757" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="758" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A758" t="s">
         <v>245</v>
       </c>
@@ -21684,8 +22665,11 @@
       <c r="G758" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="759" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H758" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="759" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A759" t="s">
         <v>245</v>
       </c>
@@ -21707,8 +22691,11 @@
       <c r="G759" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="760" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H759" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="760" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A760" t="s">
         <v>245</v>
       </c>
@@ -21730,8 +22717,11 @@
       <c r="G760" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="761" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H760" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="761" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A761" t="s">
         <v>245</v>
       </c>
@@ -21753,8 +22743,11 @@
       <c r="G761" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="762" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H761" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="762" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A762" t="s">
         <v>245</v>
       </c>
@@ -21776,8 +22769,11 @@
       <c r="G762" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="763" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H762" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="763" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A763" t="s">
         <v>245</v>
       </c>
@@ -21799,8 +22795,11 @@
       <c r="G763" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="764" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H763" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="764" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A764" t="s">
         <v>245</v>
       </c>
@@ -21822,8 +22821,11 @@
       <c r="G764" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="765" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H764" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="765" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A765" t="s">
         <v>245</v>
       </c>
@@ -21845,8 +22847,11 @@
       <c r="G765" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="766" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H765" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="766" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A766" t="s">
         <v>245</v>
       </c>
@@ -21868,8 +22873,11 @@
       <c r="G766" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="767" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H766" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="767" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A767" t="s">
         <v>245</v>
       </c>
@@ -21891,8 +22899,11 @@
       <c r="G767" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="768" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H767" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="768" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A768" t="s">
         <v>245</v>
       </c>
@@ -21914,8 +22925,11 @@
       <c r="G768" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="769" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H768" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="769" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A769" t="s">
         <v>245</v>
       </c>
@@ -21937,8 +22951,11 @@
       <c r="G769" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="770" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H769" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="770" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A770" t="s">
         <v>245</v>
       </c>
@@ -21960,8 +22977,11 @@
       <c r="G770" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="771" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H770" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="771" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A771" t="s">
         <v>245</v>
       </c>
@@ -21983,8 +23003,11 @@
       <c r="G771" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="772" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H771" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="772" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A772" t="s">
         <v>245</v>
       </c>
@@ -22006,8 +23029,11 @@
       <c r="G772" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="773" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H772" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="773" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A773" t="s">
         <v>245</v>
       </c>
@@ -22029,8 +23055,11 @@
       <c r="G773" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="774" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H773" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="774" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A774" t="s">
         <v>245</v>
       </c>
@@ -22052,8 +23081,11 @@
       <c r="G774" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="775" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H774" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="775" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A775" t="s">
         <v>245</v>
       </c>
@@ -22075,8 +23107,11 @@
       <c r="G775" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="776" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H775" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="776" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A776" t="s">
         <v>245</v>
       </c>
@@ -22098,8 +23133,11 @@
       <c r="G776" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="777" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H776" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="777" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A777" t="s">
         <v>245</v>
       </c>
@@ -22121,8 +23159,11 @@
       <c r="G777" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="778" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H777" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="778" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A778" t="s">
         <v>245</v>
       </c>
@@ -22144,8 +23185,14 @@
       <c r="G778" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="779" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H778" t="s">
+        <v>5</v>
+      </c>
+      <c r="I778" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="779" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A779" t="s">
         <v>245</v>
       </c>
@@ -22167,8 +23214,11 @@
       <c r="G779" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="780" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H779" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="780" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A780" t="s">
         <v>245</v>
       </c>
@@ -22190,8 +23240,11 @@
       <c r="G780" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="781" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H780" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="781" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A781" t="s">
         <v>245</v>
       </c>
@@ -22213,8 +23266,11 @@
       <c r="G781" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="782" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H781" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="782" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A782" t="s">
         <v>245</v>
       </c>
@@ -22236,8 +23292,11 @@
       <c r="G782" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="783" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H782" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="783" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A783" t="s">
         <v>245</v>
       </c>
@@ -22259,8 +23318,11 @@
       <c r="G783" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="784" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H783" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="784" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A784" t="s">
         <v>245</v>
       </c>
@@ -22282,8 +23344,11 @@
       <c r="G784" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="785" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H784" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="785" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A785" t="s">
         <v>245</v>
       </c>
@@ -22305,8 +23370,11 @@
       <c r="G785" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="786" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H785" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="786" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A786" t="s">
         <v>245</v>
       </c>
@@ -22328,8 +23396,11 @@
       <c r="G786" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="787" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H786" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="787" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A787" t="s">
         <v>245</v>
       </c>
@@ -22351,8 +23422,11 @@
       <c r="G787" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="788" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H787" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="788" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A788" t="s">
         <v>245</v>
       </c>
@@ -22374,8 +23448,11 @@
       <c r="G788" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="789" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H788" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="789" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A789" t="s">
         <v>245</v>
       </c>
@@ -22397,8 +23474,11 @@
       <c r="G789" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="790" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H789" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="790" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A790" t="s">
         <v>245</v>
       </c>
@@ -22420,8 +23500,11 @@
       <c r="G790" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="791" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H790" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="791" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A791" t="s">
         <v>245</v>
       </c>
@@ -22443,8 +23526,11 @@
       <c r="G791" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="792" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H791" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="792" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A792" t="s">
         <v>245</v>
       </c>
@@ -22466,8 +23552,11 @@
       <c r="G792" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="793" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H792" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="793" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A793" t="s">
         <v>245</v>
       </c>
@@ -22489,8 +23578,11 @@
       <c r="G793" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="794" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H793" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="794" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A794" t="s">
         <v>245</v>
       </c>
@@ -22512,8 +23604,11 @@
       <c r="G794" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="795" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H794" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="795" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A795" t="s">
         <v>245</v>
       </c>
@@ -22535,8 +23630,11 @@
       <c r="G795" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="796" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H795" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="796" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A796" t="s">
         <v>245</v>
       </c>
@@ -22558,8 +23656,11 @@
       <c r="G796" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="797" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H796" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="797" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A797" t="s">
         <v>245</v>
       </c>
@@ -22581,8 +23682,11 @@
       <c r="G797" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="798" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H797" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="798" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A798" t="s">
         <v>245</v>
       </c>
@@ -22604,8 +23708,11 @@
       <c r="G798" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="799" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H798" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="799" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A799" t="s">
         <v>245</v>
       </c>
@@ -22627,8 +23734,11 @@
       <c r="G799" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="800" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H799" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="800" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A800" t="s">
         <v>245</v>
       </c>
@@ -22649,6 +23759,9 @@
       </c>
       <c r="G800" t="s">
         <v>11</v>
+      </c>
+      <c r="H800" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="801" spans="1:8" x14ac:dyDescent="0.3">
@@ -22673,6 +23786,9 @@
       <c r="G801" t="s">
         <v>11</v>
       </c>
+      <c r="H801" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="802" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A802" t="s">
@@ -22696,6 +23812,9 @@
       <c r="G802" t="s">
         <v>5</v>
       </c>
+      <c r="H802" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="803" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A803" t="s">
@@ -22719,6 +23838,9 @@
       <c r="G803" t="s">
         <v>11</v>
       </c>
+      <c r="H803" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="804" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A804" t="s">
@@ -22742,6 +23864,9 @@
       <c r="G804" t="s">
         <v>11</v>
       </c>
+      <c r="H804" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="805" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A805" t="s">
@@ -22765,6 +23890,9 @@
       <c r="G805" t="s">
         <v>11</v>
       </c>
+      <c r="H805" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="806" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A806" t="s">
@@ -22788,6 +23916,9 @@
       <c r="G806" t="s">
         <v>11</v>
       </c>
+      <c r="H806" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="807" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A807" t="s">
@@ -22811,6 +23942,9 @@
       <c r="G807" t="s">
         <v>3</v>
       </c>
+      <c r="H807" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="808" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A808" t="s">
@@ -22834,6 +23968,9 @@
       <c r="G808" t="s">
         <v>3</v>
       </c>
+      <c r="H808" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="809" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A809" t="s">
@@ -22857,6 +23994,9 @@
       <c r="G809" t="s">
         <v>3</v>
       </c>
+      <c r="H809" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="810" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A810" t="s">
@@ -22880,6 +24020,9 @@
       <c r="G810" t="s">
         <v>3</v>
       </c>
+      <c r="H810" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="811" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A811" t="s">
@@ -22903,6 +24046,9 @@
       <c r="G811" t="s">
         <v>3</v>
       </c>
+      <c r="H811" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="812" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A812" t="s">
@@ -22926,6 +24072,9 @@
       <c r="G812" t="s">
         <v>3</v>
       </c>
+      <c r="H812" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="813" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A813" t="s">
@@ -22949,6 +24098,9 @@
       <c r="G813" t="s">
         <v>3</v>
       </c>
+      <c r="H813" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="814" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A814" t="s">
@@ -22971,6 +24123,9 @@
       </c>
       <c r="G814" t="s">
         <v>3</v>
+      </c>
+      <c r="H814" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="815" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Saved GMP samples, done annotating
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF0FE8E-5B33-4393-BEBC-3C655B3702A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2FA9AF-14F6-45B1-80D8-38CDAB38E27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5597" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5603" uniqueCount="731">
   <si>
     <t>Amm</t>
   </si>
@@ -1956,9 +1956,6 @@
     <t>FT1342</t>
   </si>
   <si>
-    <t>Rescue but looks gross</t>
-  </si>
-  <si>
     <t>FT1434</t>
   </si>
   <si>
@@ -2203,6 +2200,24 @@
   </si>
   <si>
     <t>FT3574</t>
+  </si>
+  <si>
+    <t>FT1422</t>
+  </si>
+  <si>
+    <t>FT1580</t>
+  </si>
+  <si>
+    <t>FT1585</t>
+  </si>
+  <si>
+    <t>FT1603</t>
+  </si>
+  <si>
+    <t>FT3030</t>
+  </si>
+  <si>
+    <t>FT0865</t>
   </si>
 </sst>
 </file>
@@ -2522,8 +2537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1084"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A792" workbookViewId="0">
-      <selection activeCell="J811" sqref="J811"/>
+    <sheetView tabSelected="1" topLeftCell="A764" workbookViewId="0">
+      <selection activeCell="I704" sqref="I704"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17828,8 +17843,11 @@
       <c r="G573" t="s">
         <v>11</v>
       </c>
+      <c r="H573" t="s">
+        <v>725</v>
+      </c>
       <c r="I573" t="s">
-        <v>643</v>
+        <v>610</v>
       </c>
     </row>
     <row r="574" spans="1:9" x14ac:dyDescent="0.3">
@@ -17855,7 +17873,7 @@
         <v>11</v>
       </c>
       <c r="H574" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="575" spans="1:9" x14ac:dyDescent="0.3">
@@ -17881,7 +17899,7 @@
         <v>11</v>
       </c>
       <c r="H575" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="576" spans="1:9" x14ac:dyDescent="0.3">
@@ -17907,7 +17925,7 @@
         <v>11</v>
       </c>
       <c r="H576" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="577" spans="1:9" x14ac:dyDescent="0.3">
@@ -17933,7 +17951,7 @@
         <v>3</v>
       </c>
       <c r="H577" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I577" t="s">
         <v>480</v>
@@ -18039,8 +18057,11 @@
       <c r="G581" t="s">
         <v>3</v>
       </c>
+      <c r="H581" t="s">
+        <v>726</v>
+      </c>
       <c r="I581" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="582" spans="1:9" x14ac:dyDescent="0.3">
@@ -18065,8 +18086,11 @@
       <c r="G582" t="s">
         <v>3</v>
       </c>
+      <c r="H582" t="s">
+        <v>727</v>
+      </c>
       <c r="I582" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="583" spans="1:9" x14ac:dyDescent="0.3">
@@ -18092,7 +18116,7 @@
         <v>11</v>
       </c>
       <c r="H583" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="584" spans="1:9" x14ac:dyDescent="0.3">
@@ -18118,7 +18142,7 @@
         <v>3</v>
       </c>
       <c r="H584" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="I584" t="s">
         <v>400</v>
@@ -18146,8 +18170,11 @@
       <c r="G585" t="s">
         <v>3</v>
       </c>
+      <c r="H585" t="s">
+        <v>728</v>
+      </c>
       <c r="I585" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="586" spans="1:9" x14ac:dyDescent="0.3">
@@ -18173,7 +18200,7 @@
         <v>3</v>
       </c>
       <c r="H586" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="587" spans="1:9" x14ac:dyDescent="0.3">
@@ -18199,7 +18226,7 @@
         <v>11</v>
       </c>
       <c r="H587" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="588" spans="1:9" x14ac:dyDescent="0.3">
@@ -18251,7 +18278,7 @@
         <v>11</v>
       </c>
       <c r="H589" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="590" spans="1:9" x14ac:dyDescent="0.3">
@@ -18277,7 +18304,7 @@
         <v>3</v>
       </c>
       <c r="H590" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="591" spans="1:9" x14ac:dyDescent="0.3">
@@ -18355,7 +18382,7 @@
         <v>11</v>
       </c>
       <c r="H593" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="594" spans="1:8" x14ac:dyDescent="0.3">
@@ -18381,7 +18408,7 @@
         <v>3</v>
       </c>
       <c r="H594" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="595" spans="1:8" x14ac:dyDescent="0.3">
@@ -18407,7 +18434,7 @@
         <v>11</v>
       </c>
       <c r="H595" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="596" spans="1:8" x14ac:dyDescent="0.3">
@@ -18485,7 +18512,7 @@
         <v>11</v>
       </c>
       <c r="H598" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="599" spans="1:8" x14ac:dyDescent="0.3">
@@ -18511,7 +18538,7 @@
         <v>3</v>
       </c>
       <c r="H599" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="600" spans="1:8" x14ac:dyDescent="0.3">
@@ -18537,7 +18564,7 @@
         <v>3</v>
       </c>
       <c r="H600" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="601" spans="1:8" x14ac:dyDescent="0.3">
@@ -18563,7 +18590,7 @@
         <v>11</v>
       </c>
       <c r="H601" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="602" spans="1:8" x14ac:dyDescent="0.3">
@@ -18589,7 +18616,7 @@
         <v>3</v>
       </c>
       <c r="H602" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="603" spans="1:8" x14ac:dyDescent="0.3">
@@ -18615,7 +18642,7 @@
         <v>3</v>
       </c>
       <c r="H603" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="604" spans="1:8" x14ac:dyDescent="0.3">
@@ -18719,7 +18746,7 @@
         <v>11</v>
       </c>
       <c r="H607" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="608" spans="1:8" x14ac:dyDescent="0.3">
@@ -18745,7 +18772,7 @@
         <v>3</v>
       </c>
       <c r="H608" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="609" spans="1:9" x14ac:dyDescent="0.3">
@@ -18875,7 +18902,7 @@
         <v>11</v>
       </c>
       <c r="H613" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="614" spans="1:9" x14ac:dyDescent="0.3">
@@ -18901,7 +18928,7 @@
         <v>11</v>
       </c>
       <c r="H614" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="615" spans="1:9" x14ac:dyDescent="0.3">
@@ -18953,7 +18980,7 @@
         <v>3</v>
       </c>
       <c r="H616" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="617" spans="1:9" x14ac:dyDescent="0.3">
@@ -18979,7 +19006,7 @@
         <v>11</v>
       </c>
       <c r="H617" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I617" t="s">
         <v>471</v>
@@ -19008,7 +19035,7 @@
         <v>11</v>
       </c>
       <c r="H618" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="619" spans="1:9" x14ac:dyDescent="0.3">
@@ -19060,7 +19087,7 @@
         <v>5</v>
       </c>
       <c r="H620" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I620" t="s">
         <v>480</v>
@@ -19115,7 +19142,7 @@
         <v>5</v>
       </c>
       <c r="H622" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="623" spans="1:9" x14ac:dyDescent="0.3">
@@ -19141,7 +19168,7 @@
         <v>5</v>
       </c>
       <c r="H623" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="624" spans="1:9" x14ac:dyDescent="0.3">
@@ -19167,7 +19194,7 @@
         <v>3</v>
       </c>
       <c r="H624" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="625" spans="1:9" x14ac:dyDescent="0.3">
@@ -19219,7 +19246,7 @@
         <v>3</v>
       </c>
       <c r="H626" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="627" spans="1:9" x14ac:dyDescent="0.3">
@@ -19248,7 +19275,7 @@
         <v>5</v>
       </c>
       <c r="I627" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="628" spans="1:9" x14ac:dyDescent="0.3">
@@ -19300,7 +19327,7 @@
         <v>3</v>
       </c>
       <c r="H629" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="630" spans="1:9" x14ac:dyDescent="0.3">
@@ -19352,7 +19379,7 @@
         <v>5</v>
       </c>
       <c r="H631" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="632" spans="1:9" x14ac:dyDescent="0.3">
@@ -19378,7 +19405,7 @@
         <v>3</v>
       </c>
       <c r="H632" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="633" spans="1:9" x14ac:dyDescent="0.3">
@@ -19430,7 +19457,7 @@
         <v>3</v>
       </c>
       <c r="H634" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="635" spans="1:9" x14ac:dyDescent="0.3">
@@ -19456,7 +19483,7 @@
         <v>11</v>
       </c>
       <c r="H635" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="636" spans="1:9" x14ac:dyDescent="0.3">
@@ -19508,7 +19535,7 @@
         <v>11</v>
       </c>
       <c r="H637" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="638" spans="1:9" x14ac:dyDescent="0.3">
@@ -19560,7 +19587,7 @@
         <v>3</v>
       </c>
       <c r="H639" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="640" spans="1:9" x14ac:dyDescent="0.3">
@@ -19585,8 +19612,11 @@
       <c r="G640" t="s">
         <v>3</v>
       </c>
+      <c r="H640" t="s">
+        <v>729</v>
+      </c>
       <c r="I640" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="641" spans="1:8" x14ac:dyDescent="0.3">
@@ -19612,7 +19642,7 @@
         <v>3</v>
       </c>
       <c r="H641" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="642" spans="1:8" x14ac:dyDescent="0.3">
@@ -19638,7 +19668,7 @@
         <v>3</v>
       </c>
       <c r="H642" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="643" spans="1:8" x14ac:dyDescent="0.3">
@@ -19716,7 +19746,7 @@
         <v>3</v>
       </c>
       <c r="H645" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="646" spans="1:8" x14ac:dyDescent="0.3">
@@ -19924,7 +19954,7 @@
         <v>5</v>
       </c>
       <c r="H653" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="654" spans="1:8" x14ac:dyDescent="0.3">
@@ -19950,7 +19980,7 @@
         <v>3</v>
       </c>
       <c r="H654" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="655" spans="1:8" x14ac:dyDescent="0.3">
@@ -20054,7 +20084,7 @@
         <v>11</v>
       </c>
       <c r="H658" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="659" spans="1:9" x14ac:dyDescent="0.3">
@@ -20080,7 +20110,7 @@
         <v>5</v>
       </c>
       <c r="H659" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="660" spans="1:9" x14ac:dyDescent="0.3">
@@ -20106,7 +20136,7 @@
         <v>5</v>
       </c>
       <c r="H660" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="661" spans="1:9" x14ac:dyDescent="0.3">
@@ -20161,7 +20191,7 @@
         <v>5</v>
       </c>
       <c r="I662" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="663" spans="1:9" x14ac:dyDescent="0.3">
@@ -20187,7 +20217,7 @@
         <v>11</v>
       </c>
       <c r="H663" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="664" spans="1:9" x14ac:dyDescent="0.3">
@@ -20239,7 +20269,7 @@
         <v>3</v>
       </c>
       <c r="H665" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="666" spans="1:9" x14ac:dyDescent="0.3">
@@ -20317,7 +20347,7 @@
         <v>11</v>
       </c>
       <c r="H668" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="669" spans="1:9" x14ac:dyDescent="0.3">
@@ -20343,7 +20373,7 @@
         <v>5</v>
       </c>
       <c r="H669" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="670" spans="1:9" x14ac:dyDescent="0.3">
@@ -20395,7 +20425,7 @@
         <v>11</v>
       </c>
       <c r="H671" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="672" spans="1:9" x14ac:dyDescent="0.3">
@@ -20421,7 +20451,7 @@
         <v>11</v>
       </c>
       <c r="H672" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="673" spans="1:9" x14ac:dyDescent="0.3">
@@ -20447,7 +20477,7 @@
         <v>5</v>
       </c>
       <c r="H673" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="674" spans="1:9" x14ac:dyDescent="0.3">
@@ -20473,7 +20503,7 @@
         <v>5</v>
       </c>
       <c r="H674" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="675" spans="1:9" x14ac:dyDescent="0.3">
@@ -20499,7 +20529,7 @@
         <v>5</v>
       </c>
       <c r="H675" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="676" spans="1:9" x14ac:dyDescent="0.3">
@@ -20629,7 +20659,7 @@
         <v>5</v>
       </c>
       <c r="H680" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="681" spans="1:9" x14ac:dyDescent="0.3">
@@ -20681,7 +20711,7 @@
         <v>5</v>
       </c>
       <c r="H682" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="683" spans="1:9" x14ac:dyDescent="0.3">
@@ -20785,10 +20815,10 @@
         <v>5</v>
       </c>
       <c r="H686" t="s">
+        <v>702</v>
+      </c>
+      <c r="I686" t="s">
         <v>703</v>
-      </c>
-      <c r="I686" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="687" spans="1:9" x14ac:dyDescent="0.3">
@@ -21022,7 +21052,7 @@
         <v>5</v>
       </c>
       <c r="H695" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="696" spans="1:9" x14ac:dyDescent="0.3">
@@ -21048,7 +21078,7 @@
         <v>5</v>
       </c>
       <c r="H696" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="697" spans="1:9" x14ac:dyDescent="0.3">
@@ -21229,8 +21259,11 @@
       <c r="G703" t="s">
         <v>11</v>
       </c>
+      <c r="H703" t="s">
+        <v>730</v>
+      </c>
       <c r="I703" t="s">
-        <v>392</v>
+        <v>602</v>
       </c>
     </row>
     <row r="704" spans="1:9" x14ac:dyDescent="0.3">
@@ -21285,7 +21318,7 @@
         <v>5</v>
       </c>
       <c r="I705" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="706" spans="1:9" x14ac:dyDescent="0.3">
@@ -21337,7 +21370,7 @@
         <v>3</v>
       </c>
       <c r="H707" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="708" spans="1:9" x14ac:dyDescent="0.3">
@@ -21415,7 +21448,7 @@
         <v>11</v>
       </c>
       <c r="H710" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="711" spans="1:9" x14ac:dyDescent="0.3">
@@ -21441,10 +21474,10 @@
         <v>11</v>
       </c>
       <c r="H711" t="s">
+        <v>708</v>
+      </c>
+      <c r="I711" t="s">
         <v>709</v>
-      </c>
-      <c r="I711" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="712" spans="1:9" x14ac:dyDescent="0.3">
@@ -21496,7 +21529,7 @@
         <v>3</v>
       </c>
       <c r="H713" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="714" spans="1:9" x14ac:dyDescent="0.3">
@@ -21652,7 +21685,7 @@
         <v>3</v>
       </c>
       <c r="H719" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="720" spans="1:9" x14ac:dyDescent="0.3">
@@ -21678,7 +21711,7 @@
         <v>3</v>
       </c>
       <c r="H720" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="721" spans="1:8" x14ac:dyDescent="0.3">
@@ -21756,7 +21789,7 @@
         <v>11</v>
       </c>
       <c r="H723" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="724" spans="1:8" x14ac:dyDescent="0.3">
@@ -21782,7 +21815,7 @@
         <v>3</v>
       </c>
       <c r="H724" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="725" spans="1:8" x14ac:dyDescent="0.3">
@@ -21964,7 +21997,7 @@
         <v>3</v>
       </c>
       <c r="H731" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="732" spans="1:8" x14ac:dyDescent="0.3">
@@ -22094,7 +22127,7 @@
         <v>11</v>
       </c>
       <c r="H736" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="737" spans="1:8" x14ac:dyDescent="0.3">
@@ -22536,7 +22569,7 @@
         <v>11</v>
       </c>
       <c r="H753" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="754" spans="1:8" x14ac:dyDescent="0.3">
@@ -22666,7 +22699,7 @@
         <v>5</v>
       </c>
       <c r="H758" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="759" spans="1:8" x14ac:dyDescent="0.3">
@@ -23004,7 +23037,7 @@
         <v>3</v>
       </c>
       <c r="H771" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="772" spans="1:9" x14ac:dyDescent="0.3">
@@ -23030,7 +23063,7 @@
         <v>11</v>
       </c>
       <c r="H772" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="773" spans="1:9" x14ac:dyDescent="0.3">
@@ -23082,7 +23115,7 @@
         <v>11</v>
       </c>
       <c r="H774" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="775" spans="1:9" x14ac:dyDescent="0.3">
@@ -23189,7 +23222,7 @@
         <v>5</v>
       </c>
       <c r="I778" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="779" spans="1:9" x14ac:dyDescent="0.3">
@@ -23215,7 +23248,7 @@
         <v>5</v>
       </c>
       <c r="H779" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="780" spans="1:9" x14ac:dyDescent="0.3">
@@ -23371,7 +23404,7 @@
         <v>3</v>
       </c>
       <c r="H785" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="786" spans="1:8" x14ac:dyDescent="0.3">
@@ -23449,7 +23482,7 @@
         <v>11</v>
       </c>
       <c r="H788" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="789" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixing some erroneous annotations
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CFD22E-17CC-4D50-B505-C04B80D36F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C240168C-B4CA-41E8-B650-2A10640E88ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5654" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5655" uniqueCount="738">
   <si>
     <t>Amm</t>
   </si>
@@ -1554,6 +1554,9 @@
     <t>FT2058</t>
   </si>
   <si>
+    <t>FT1441</t>
+  </si>
+  <si>
     <t>FT0036</t>
   </si>
   <si>
@@ -2136,9 +2139,6 @@
     <t>Second peak at 10.5 also interesting</t>
   </si>
   <si>
-    <t>FT1089</t>
-  </si>
-  <si>
     <t>FT0202</t>
   </si>
   <si>
@@ -2236,6 +2236,9 @@
   </si>
   <si>
     <t>Not present???</t>
+  </si>
+  <si>
+    <t>FT0189</t>
   </si>
 </sst>
 </file>
@@ -2561,8 +2564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1093"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1086" workbookViewId="0">
-      <selection activeCell="C1094" sqref="C1094"/>
+    <sheetView tabSelected="1" topLeftCell="A686" workbookViewId="0">
+      <selection activeCell="H700" sqref="H700"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9944,7 +9947,7 @@
         <v>5</v>
       </c>
       <c r="H274" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.3">
@@ -13426,7 +13429,10 @@
         <v>5</v>
       </c>
       <c r="H404" t="s">
-        <v>457</v>
+        <v>5</v>
+      </c>
+      <c r="I404" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="405" spans="1:9" x14ac:dyDescent="0.3">
@@ -13452,7 +13458,7 @@
         <v>5</v>
       </c>
       <c r="H405" t="s">
-        <v>5</v>
+        <v>457</v>
       </c>
     </row>
     <row r="406" spans="1:9" x14ac:dyDescent="0.3">
@@ -17267,10 +17273,10 @@
         <v>3</v>
       </c>
       <c r="H550" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="I550" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="551" spans="1:9" x14ac:dyDescent="0.3">
@@ -17322,10 +17328,10 @@
         <v>3</v>
       </c>
       <c r="H552" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="I552" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="553" spans="1:9" x14ac:dyDescent="0.3">
@@ -17351,7 +17357,7 @@
         <v>3</v>
       </c>
       <c r="H553" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="554" spans="1:9" x14ac:dyDescent="0.3">
@@ -17377,7 +17383,7 @@
         <v>11</v>
       </c>
       <c r="H554" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="555" spans="1:9" x14ac:dyDescent="0.3">
@@ -17403,7 +17409,7 @@
         <v>3</v>
       </c>
       <c r="H555" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="556" spans="1:9" x14ac:dyDescent="0.3">
@@ -17429,7 +17435,7 @@
         <v>11</v>
       </c>
       <c r="H556" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="557" spans="1:9" x14ac:dyDescent="0.3">
@@ -17510,7 +17516,7 @@
         <v>5</v>
       </c>
       <c r="I559" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="560" spans="1:9" x14ac:dyDescent="0.3">
@@ -17536,7 +17542,7 @@
         <v>3</v>
       </c>
       <c r="H560" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="561" spans="1:9" x14ac:dyDescent="0.3">
@@ -17588,7 +17594,7 @@
         <v>11</v>
       </c>
       <c r="H562" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="563" spans="1:9" x14ac:dyDescent="0.3">
@@ -17614,7 +17620,7 @@
         <v>3</v>
       </c>
       <c r="H563" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="564" spans="1:9" x14ac:dyDescent="0.3">
@@ -17666,7 +17672,7 @@
         <v>3</v>
       </c>
       <c r="H565" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="566" spans="1:9" x14ac:dyDescent="0.3">
@@ -17718,7 +17724,7 @@
         <v>3</v>
       </c>
       <c r="H567" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="568" spans="1:9" x14ac:dyDescent="0.3">
@@ -17770,10 +17776,10 @@
         <v>3</v>
       </c>
       <c r="H569" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="I569" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="570" spans="1:9" x14ac:dyDescent="0.3">
@@ -17799,7 +17805,7 @@
         <v>3</v>
       </c>
       <c r="H570" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="571" spans="1:9" x14ac:dyDescent="0.3">
@@ -17825,7 +17831,7 @@
         <v>11</v>
       </c>
       <c r="H571" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="572" spans="1:9" x14ac:dyDescent="0.3">
@@ -17903,7 +17909,7 @@
         <v>11</v>
       </c>
       <c r="H574" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="575" spans="1:9" x14ac:dyDescent="0.3">
@@ -17958,7 +17964,7 @@
         <v>724</v>
       </c>
       <c r="I576" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="577" spans="1:9" x14ac:dyDescent="0.3">
@@ -17984,7 +17990,7 @@
         <v>11</v>
       </c>
       <c r="H577" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.3">
@@ -18010,7 +18016,7 @@
         <v>11</v>
       </c>
       <c r="H578" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.3">
@@ -18036,7 +18042,7 @@
         <v>11</v>
       </c>
       <c r="H579" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="580" spans="1:9" x14ac:dyDescent="0.3">
@@ -18062,7 +18068,7 @@
         <v>3</v>
       </c>
       <c r="H580" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="I580" t="s">
         <v>480</v>
@@ -18172,7 +18178,7 @@
         <v>725</v>
       </c>
       <c r="I584" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="585" spans="1:9" x14ac:dyDescent="0.3">
@@ -18201,7 +18207,7 @@
         <v>726</v>
       </c>
       <c r="I585" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="586" spans="1:9" x14ac:dyDescent="0.3">
@@ -18227,7 +18233,7 @@
         <v>11</v>
       </c>
       <c r="H586" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="587" spans="1:9" x14ac:dyDescent="0.3">
@@ -18253,7 +18259,7 @@
         <v>3</v>
       </c>
       <c r="H587" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="I587" t="s">
         <v>400</v>
@@ -18285,7 +18291,7 @@
         <v>727</v>
       </c>
       <c r="I588" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="589" spans="1:9" x14ac:dyDescent="0.3">
@@ -18311,7 +18317,7 @@
         <v>3</v>
       </c>
       <c r="H589" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="590" spans="1:9" x14ac:dyDescent="0.3">
@@ -18337,7 +18343,7 @@
         <v>11</v>
       </c>
       <c r="H590" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="591" spans="1:9" x14ac:dyDescent="0.3">
@@ -18389,7 +18395,7 @@
         <v>11</v>
       </c>
       <c r="H592" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="593" spans="1:8" x14ac:dyDescent="0.3">
@@ -18415,7 +18421,7 @@
         <v>3</v>
       </c>
       <c r="H593" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="594" spans="1:8" x14ac:dyDescent="0.3">
@@ -18493,7 +18499,7 @@
         <v>11</v>
       </c>
       <c r="H596" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="597" spans="1:8" x14ac:dyDescent="0.3">
@@ -18519,7 +18525,7 @@
         <v>3</v>
       </c>
       <c r="H597" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="598" spans="1:8" x14ac:dyDescent="0.3">
@@ -18545,7 +18551,7 @@
         <v>11</v>
       </c>
       <c r="H598" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="599" spans="1:8" x14ac:dyDescent="0.3">
@@ -18623,7 +18629,7 @@
         <v>11</v>
       </c>
       <c r="H601" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="602" spans="1:8" x14ac:dyDescent="0.3">
@@ -18649,7 +18655,7 @@
         <v>3</v>
       </c>
       <c r="H602" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="603" spans="1:8" x14ac:dyDescent="0.3">
@@ -18675,7 +18681,7 @@
         <v>3</v>
       </c>
       <c r="H603" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="604" spans="1:8" x14ac:dyDescent="0.3">
@@ -18701,7 +18707,7 @@
         <v>11</v>
       </c>
       <c r="H604" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="605" spans="1:8" x14ac:dyDescent="0.3">
@@ -18727,7 +18733,7 @@
         <v>3</v>
       </c>
       <c r="H605" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="606" spans="1:8" x14ac:dyDescent="0.3">
@@ -18753,7 +18759,7 @@
         <v>3</v>
       </c>
       <c r="H606" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="607" spans="1:8" x14ac:dyDescent="0.3">
@@ -18857,7 +18863,7 @@
         <v>11</v>
       </c>
       <c r="H610" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="611" spans="1:9" x14ac:dyDescent="0.3">
@@ -18883,7 +18889,7 @@
         <v>3</v>
       </c>
       <c r="H611" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="612" spans="1:9" x14ac:dyDescent="0.3">
@@ -19013,7 +19019,7 @@
         <v>11</v>
       </c>
       <c r="H616" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="617" spans="1:9" x14ac:dyDescent="0.3">
@@ -19039,7 +19045,7 @@
         <v>11</v>
       </c>
       <c r="H617" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="618" spans="1:9" x14ac:dyDescent="0.3">
@@ -19091,7 +19097,7 @@
         <v>3</v>
       </c>
       <c r="H619" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="620" spans="1:9" x14ac:dyDescent="0.3">
@@ -19117,7 +19123,7 @@
         <v>11</v>
       </c>
       <c r="H620" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="I620" t="s">
         <v>471</v>
@@ -19146,7 +19152,7 @@
         <v>11</v>
       </c>
       <c r="H621" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="622" spans="1:9" x14ac:dyDescent="0.3">
@@ -19198,7 +19204,7 @@
         <v>5</v>
       </c>
       <c r="H623" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="I623" t="s">
         <v>480</v>
@@ -19253,7 +19259,7 @@
         <v>5</v>
       </c>
       <c r="H625" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="626" spans="1:9" x14ac:dyDescent="0.3">
@@ -19279,7 +19285,7 @@
         <v>5</v>
       </c>
       <c r="H626" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="627" spans="1:9" x14ac:dyDescent="0.3">
@@ -19305,7 +19311,7 @@
         <v>3</v>
       </c>
       <c r="H627" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="628" spans="1:9" x14ac:dyDescent="0.3">
@@ -19357,7 +19363,7 @@
         <v>3</v>
       </c>
       <c r="H629" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="630" spans="1:9" x14ac:dyDescent="0.3">
@@ -19386,7 +19392,7 @@
         <v>5</v>
       </c>
       <c r="I630" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="631" spans="1:9" x14ac:dyDescent="0.3">
@@ -19438,7 +19444,7 @@
         <v>3</v>
       </c>
       <c r="H632" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="633" spans="1:9" x14ac:dyDescent="0.3">
@@ -19490,7 +19496,7 @@
         <v>5</v>
       </c>
       <c r="H634" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="635" spans="1:9" x14ac:dyDescent="0.3">
@@ -19516,7 +19522,7 @@
         <v>3</v>
       </c>
       <c r="H635" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="636" spans="1:9" x14ac:dyDescent="0.3">
@@ -19568,7 +19574,7 @@
         <v>3</v>
       </c>
       <c r="H637" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="638" spans="1:9" x14ac:dyDescent="0.3">
@@ -19594,7 +19600,7 @@
         <v>11</v>
       </c>
       <c r="H638" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="639" spans="1:9" x14ac:dyDescent="0.3">
@@ -19646,7 +19652,7 @@
         <v>11</v>
       </c>
       <c r="H640" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="641" spans="1:9" x14ac:dyDescent="0.3">
@@ -19698,7 +19704,7 @@
         <v>3</v>
       </c>
       <c r="H642" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="643" spans="1:9" x14ac:dyDescent="0.3">
@@ -19727,7 +19733,7 @@
         <v>728</v>
       </c>
       <c r="I643" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="644" spans="1:9" x14ac:dyDescent="0.3">
@@ -19753,7 +19759,7 @@
         <v>3</v>
       </c>
       <c r="H644" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="645" spans="1:9" x14ac:dyDescent="0.3">
@@ -19779,7 +19785,7 @@
         <v>3</v>
       </c>
       <c r="H645" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="646" spans="1:9" x14ac:dyDescent="0.3">
@@ -19857,7 +19863,7 @@
         <v>3</v>
       </c>
       <c r="H648" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="649" spans="1:9" x14ac:dyDescent="0.3">
@@ -20065,7 +20071,7 @@
         <v>5</v>
       </c>
       <c r="H656" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="657" spans="1:9" x14ac:dyDescent="0.3">
@@ -20091,7 +20097,7 @@
         <v>3</v>
       </c>
       <c r="H657" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="658" spans="1:9" x14ac:dyDescent="0.3">
@@ -20195,7 +20201,7 @@
         <v>11</v>
       </c>
       <c r="H661" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="662" spans="1:9" x14ac:dyDescent="0.3">
@@ -20221,7 +20227,7 @@
         <v>5</v>
       </c>
       <c r="H662" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="663" spans="1:9" x14ac:dyDescent="0.3">
@@ -20247,7 +20253,7 @@
         <v>5</v>
       </c>
       <c r="H663" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="664" spans="1:9" x14ac:dyDescent="0.3">
@@ -20302,7 +20308,7 @@
         <v>5</v>
       </c>
       <c r="I665" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="666" spans="1:9" x14ac:dyDescent="0.3">
@@ -20328,7 +20334,7 @@
         <v>11</v>
       </c>
       <c r="H666" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="667" spans="1:9" x14ac:dyDescent="0.3">
@@ -20354,7 +20360,7 @@
         <v>11</v>
       </c>
       <c r="H667" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="668" spans="1:9" x14ac:dyDescent="0.3">
@@ -20380,7 +20386,7 @@
         <v>3</v>
       </c>
       <c r="H668" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="669" spans="1:9" x14ac:dyDescent="0.3">
@@ -20458,7 +20464,7 @@
         <v>11</v>
       </c>
       <c r="H671" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="672" spans="1:9" x14ac:dyDescent="0.3">
@@ -20484,7 +20490,7 @@
         <v>5</v>
       </c>
       <c r="H672" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="673" spans="1:8" x14ac:dyDescent="0.3">
@@ -20536,7 +20542,7 @@
         <v>11</v>
       </c>
       <c r="H674" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="675" spans="1:8" x14ac:dyDescent="0.3">
@@ -20562,7 +20568,7 @@
         <v>11</v>
       </c>
       <c r="H675" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="676" spans="1:8" x14ac:dyDescent="0.3">
@@ -20588,7 +20594,7 @@
         <v>5</v>
       </c>
       <c r="H676" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="677" spans="1:8" x14ac:dyDescent="0.3">
@@ -20614,7 +20620,7 @@
         <v>5</v>
       </c>
       <c r="H677" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="678" spans="1:8" x14ac:dyDescent="0.3">
@@ -20640,7 +20646,7 @@
         <v>5</v>
       </c>
       <c r="H678" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="679" spans="1:8" x14ac:dyDescent="0.3">
@@ -20770,7 +20776,7 @@
         <v>5</v>
       </c>
       <c r="H683" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="684" spans="1:8" x14ac:dyDescent="0.3">
@@ -20822,7 +20828,7 @@
         <v>5</v>
       </c>
       <c r="H685" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="686" spans="1:8" x14ac:dyDescent="0.3">
@@ -20926,10 +20932,10 @@
         <v>5</v>
       </c>
       <c r="H689" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="I689" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="690" spans="1:9" x14ac:dyDescent="0.3">
@@ -21218,7 +21224,7 @@
         <v>5</v>
       </c>
       <c r="H700" t="s">
-        <v>703</v>
+        <v>737</v>
       </c>
     </row>
     <row r="701" spans="1:9" x14ac:dyDescent="0.3">
@@ -21429,7 +21435,7 @@
         <v>729</v>
       </c>
       <c r="I708" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="709" spans="1:9" x14ac:dyDescent="0.3">
@@ -21484,7 +21490,7 @@
         <v>5</v>
       </c>
       <c r="I710" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="711" spans="1:9" x14ac:dyDescent="0.3">
@@ -21669,7 +21675,7 @@
         <v>11</v>
       </c>
       <c r="H717" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="718" spans="1:9" x14ac:dyDescent="0.3">
@@ -23388,7 +23394,7 @@
         <v>5</v>
       </c>
       <c r="I783" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="784" spans="1:9" x14ac:dyDescent="0.3">
@@ -24428,7 +24434,7 @@
         <v>3</v>
       </c>
       <c r="H823" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="824" spans="1:8" x14ac:dyDescent="0.3">
@@ -24480,7 +24486,7 @@
         <v>3</v>
       </c>
       <c r="H825" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="826" spans="1:8" x14ac:dyDescent="0.3">
@@ -24506,7 +24512,7 @@
         <v>3</v>
       </c>
       <c r="H826" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="827" spans="1:8" x14ac:dyDescent="0.3">
@@ -24558,7 +24564,7 @@
         <v>3</v>
       </c>
       <c r="H828" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="829" spans="1:8" x14ac:dyDescent="0.3">
@@ -24584,7 +24590,7 @@
         <v>11</v>
       </c>
       <c r="H829" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="830" spans="1:8" x14ac:dyDescent="0.3">
@@ -24688,7 +24694,7 @@
         <v>3</v>
       </c>
       <c r="H833" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="834" spans="1:9" x14ac:dyDescent="0.3">
@@ -24740,10 +24746,10 @@
         <v>11</v>
       </c>
       <c r="H835" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="I835" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="836" spans="1:9" x14ac:dyDescent="0.3">
@@ -24769,7 +24775,7 @@
         <v>3</v>
       </c>
       <c r="H836" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="837" spans="1:9" x14ac:dyDescent="0.3">
@@ -24821,7 +24827,7 @@
         <v>3</v>
       </c>
       <c r="H838" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="839" spans="1:9" x14ac:dyDescent="0.3">
@@ -24873,10 +24879,10 @@
         <v>3</v>
       </c>
       <c r="H840" t="s">
+        <v>603</v>
+      </c>
+      <c r="I840" t="s">
         <v>602</v>
-      </c>
-      <c r="I840" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="841" spans="1:9" x14ac:dyDescent="0.3">
@@ -24928,7 +24934,7 @@
         <v>3</v>
       </c>
       <c r="H842" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="843" spans="1:9" x14ac:dyDescent="0.3">
@@ -24954,7 +24960,7 @@
         <v>3</v>
       </c>
       <c r="H843" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="844" spans="1:9" x14ac:dyDescent="0.3">
@@ -24980,7 +24986,7 @@
         <v>11</v>
       </c>
       <c r="H844" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="845" spans="1:9" x14ac:dyDescent="0.3">
@@ -25110,10 +25116,10 @@
         <v>11</v>
       </c>
       <c r="H849" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="I849" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="850" spans="1:9" x14ac:dyDescent="0.3">
@@ -25165,7 +25171,7 @@
         <v>11</v>
       </c>
       <c r="H851" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="852" spans="1:9" x14ac:dyDescent="0.3">
@@ -25191,10 +25197,10 @@
         <v>11</v>
       </c>
       <c r="H852" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="I852" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="853" spans="1:9" x14ac:dyDescent="0.3">
@@ -25220,10 +25226,10 @@
         <v>3</v>
       </c>
       <c r="H853" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="I853" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="854" spans="1:9" x14ac:dyDescent="0.3">
@@ -25252,7 +25258,7 @@
         <v>5</v>
       </c>
       <c r="I854" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="855" spans="1:9" x14ac:dyDescent="0.3">
@@ -25278,7 +25284,7 @@
         <v>3</v>
       </c>
       <c r="H855" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="856" spans="1:9" x14ac:dyDescent="0.3">
@@ -25304,7 +25310,7 @@
         <v>3</v>
       </c>
       <c r="H856" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="857" spans="1:9" x14ac:dyDescent="0.3">
@@ -25359,7 +25365,7 @@
         <v>470</v>
       </c>
       <c r="I858" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="859" spans="1:9" x14ac:dyDescent="0.3">
@@ -25385,10 +25391,10 @@
         <v>11</v>
       </c>
       <c r="H859" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="I859" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="860" spans="1:9" x14ac:dyDescent="0.3">
@@ -25414,7 +25420,7 @@
         <v>3</v>
       </c>
       <c r="H860" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="861" spans="1:9" x14ac:dyDescent="0.3">
@@ -25440,10 +25446,10 @@
         <v>3</v>
       </c>
       <c r="H861" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="I861" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="862" spans="1:9" x14ac:dyDescent="0.3">
@@ -25469,7 +25475,7 @@
         <v>3</v>
       </c>
       <c r="H862" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="863" spans="1:9" x14ac:dyDescent="0.3">
@@ -25495,10 +25501,10 @@
         <v>11</v>
       </c>
       <c r="H863" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="I863" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="864" spans="1:9" x14ac:dyDescent="0.3">
@@ -25576,7 +25582,7 @@
         <v>3</v>
       </c>
       <c r="H866" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="867" spans="1:9" x14ac:dyDescent="0.3">
@@ -25628,7 +25634,7 @@
         <v>11</v>
       </c>
       <c r="H868" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="869" spans="1:9" x14ac:dyDescent="0.3">
@@ -25654,7 +25660,7 @@
         <v>11</v>
       </c>
       <c r="H869" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="870" spans="1:9" x14ac:dyDescent="0.3">
@@ -25680,7 +25686,7 @@
         <v>3</v>
       </c>
       <c r="H870" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="871" spans="1:9" x14ac:dyDescent="0.3">
@@ -25784,7 +25790,7 @@
         <v>11</v>
       </c>
       <c r="H874" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="875" spans="1:9" x14ac:dyDescent="0.3">
@@ -25810,7 +25816,7 @@
         <v>3</v>
       </c>
       <c r="H875" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="876" spans="1:9" x14ac:dyDescent="0.3">
@@ -25836,7 +25842,7 @@
         <v>3</v>
       </c>
       <c r="H876" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="877" spans="1:9" x14ac:dyDescent="0.3">
@@ -25862,10 +25868,10 @@
         <v>11</v>
       </c>
       <c r="H877" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="I877" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="878" spans="1:9" x14ac:dyDescent="0.3">
@@ -25891,7 +25897,7 @@
         <v>3</v>
       </c>
       <c r="H878" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="879" spans="1:9" x14ac:dyDescent="0.3">
@@ -25917,10 +25923,10 @@
         <v>3</v>
       </c>
       <c r="H879" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="I879" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="880" spans="1:9" x14ac:dyDescent="0.3">
@@ -25998,7 +26004,7 @@
         <v>3</v>
       </c>
       <c r="H882" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="883" spans="1:9" x14ac:dyDescent="0.3">
@@ -26024,7 +26030,7 @@
         <v>11</v>
       </c>
       <c r="H883" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="884" spans="1:9" x14ac:dyDescent="0.3">
@@ -26050,7 +26056,7 @@
         <v>3</v>
       </c>
       <c r="H884" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="885" spans="1:9" x14ac:dyDescent="0.3">
@@ -26180,10 +26186,10 @@
         <v>11</v>
       </c>
       <c r="H889" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="I889" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="890" spans="1:9" x14ac:dyDescent="0.3">
@@ -26209,10 +26215,10 @@
         <v>11</v>
       </c>
       <c r="H890" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="I890" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="891" spans="1:9" x14ac:dyDescent="0.3">
@@ -26264,7 +26270,7 @@
         <v>3</v>
       </c>
       <c r="H892" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="893" spans="1:9" x14ac:dyDescent="0.3">
@@ -26290,10 +26296,10 @@
         <v>11</v>
       </c>
       <c r="H893" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I893" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="894" spans="1:9" x14ac:dyDescent="0.3">
@@ -26319,7 +26325,7 @@
         <v>11</v>
       </c>
       <c r="H894" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="895" spans="1:9" x14ac:dyDescent="0.3">
@@ -26371,10 +26377,10 @@
         <v>5</v>
       </c>
       <c r="H896" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="I896" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="897" spans="1:9" x14ac:dyDescent="0.3">
@@ -26400,7 +26406,7 @@
         <v>5</v>
       </c>
       <c r="H897" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="898" spans="1:9" x14ac:dyDescent="0.3">
@@ -26426,7 +26432,7 @@
         <v>5</v>
       </c>
       <c r="H898" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="899" spans="1:9" x14ac:dyDescent="0.3">
@@ -26452,7 +26458,7 @@
         <v>5</v>
       </c>
       <c r="H899" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="900" spans="1:9" x14ac:dyDescent="0.3">
@@ -26478,7 +26484,7 @@
         <v>3</v>
       </c>
       <c r="H900" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="901" spans="1:9" x14ac:dyDescent="0.3">
@@ -26530,7 +26536,7 @@
         <v>3</v>
       </c>
       <c r="H902" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="903" spans="1:9" x14ac:dyDescent="0.3">
@@ -26608,10 +26614,10 @@
         <v>3</v>
       </c>
       <c r="H905" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="I905" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="906" spans="1:9" x14ac:dyDescent="0.3">
@@ -26663,7 +26669,7 @@
         <v>5</v>
       </c>
       <c r="H907" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="908" spans="1:9" x14ac:dyDescent="0.3">
@@ -26689,7 +26695,7 @@
         <v>3</v>
       </c>
       <c r="H908" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="909" spans="1:9" x14ac:dyDescent="0.3">
@@ -26741,7 +26747,7 @@
         <v>3</v>
       </c>
       <c r="H910" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="911" spans="1:9" x14ac:dyDescent="0.3">
@@ -26767,7 +26773,7 @@
         <v>11</v>
       </c>
       <c r="H911" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="912" spans="1:9" x14ac:dyDescent="0.3">
@@ -26819,7 +26825,7 @@
         <v>11</v>
       </c>
       <c r="H913" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="914" spans="1:9" x14ac:dyDescent="0.3">
@@ -26845,7 +26851,7 @@
         <v>3</v>
       </c>
       <c r="H914" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="915" spans="1:9" x14ac:dyDescent="0.3">
@@ -26871,7 +26877,7 @@
         <v>3</v>
       </c>
       <c r="H915" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="916" spans="1:9" x14ac:dyDescent="0.3">
@@ -26897,7 +26903,7 @@
         <v>3</v>
       </c>
       <c r="H916" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="917" spans="1:9" x14ac:dyDescent="0.3">
@@ -26923,7 +26929,7 @@
         <v>3</v>
       </c>
       <c r="H917" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="918" spans="1:9" x14ac:dyDescent="0.3">
@@ -26949,7 +26955,7 @@
         <v>3</v>
       </c>
       <c r="H918" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="919" spans="1:9" x14ac:dyDescent="0.3">
@@ -26975,10 +26981,10 @@
         <v>11</v>
       </c>
       <c r="H919" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="I919" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="920" spans="1:9" x14ac:dyDescent="0.3">
@@ -27030,7 +27036,7 @@
         <v>3</v>
       </c>
       <c r="H921" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="922" spans="1:9" x14ac:dyDescent="0.3">
@@ -27056,10 +27062,10 @@
         <v>11</v>
       </c>
       <c r="H922" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="I922" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="923" spans="1:9" x14ac:dyDescent="0.3">
@@ -27241,7 +27247,7 @@
         <v>5</v>
       </c>
       <c r="H929" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="930" spans="1:9" x14ac:dyDescent="0.3">
@@ -27371,7 +27377,7 @@
         <v>11</v>
       </c>
       <c r="H934" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="935" spans="1:9" x14ac:dyDescent="0.3">
@@ -27397,7 +27403,7 @@
         <v>5</v>
       </c>
       <c r="H935" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="936" spans="1:9" x14ac:dyDescent="0.3">
@@ -27501,7 +27507,7 @@
         <v>11</v>
       </c>
       <c r="H939" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="940" spans="1:9" x14ac:dyDescent="0.3">
@@ -27527,10 +27533,10 @@
         <v>11</v>
       </c>
       <c r="H940" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="I940" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="941" spans="1:9" x14ac:dyDescent="0.3">
@@ -27556,7 +27562,7 @@
         <v>3</v>
       </c>
       <c r="H941" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="942" spans="1:9" x14ac:dyDescent="0.3">
@@ -27634,7 +27640,7 @@
         <v>11</v>
       </c>
       <c r="H944" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="945" spans="1:9" x14ac:dyDescent="0.3">
@@ -27660,7 +27666,7 @@
         <v>5</v>
       </c>
       <c r="H945" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="946" spans="1:9" x14ac:dyDescent="0.3">
@@ -27712,10 +27718,10 @@
         <v>11</v>
       </c>
       <c r="H947" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="I947" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="948" spans="1:9" x14ac:dyDescent="0.3">
@@ -27741,7 +27747,7 @@
         <v>11</v>
       </c>
       <c r="H948" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="949" spans="1:9" x14ac:dyDescent="0.3">
@@ -27767,7 +27773,7 @@
         <v>5</v>
       </c>
       <c r="H949" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="950" spans="1:9" x14ac:dyDescent="0.3">
@@ -27793,7 +27799,7 @@
         <v>5</v>
       </c>
       <c r="H950" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="951" spans="1:9" x14ac:dyDescent="0.3">
@@ -27819,7 +27825,7 @@
         <v>5</v>
       </c>
       <c r="H951" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="952" spans="1:9" x14ac:dyDescent="0.3">
@@ -27949,7 +27955,7 @@
         <v>5</v>
       </c>
       <c r="H956" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="957" spans="1:9" x14ac:dyDescent="0.3">
@@ -28001,7 +28007,7 @@
         <v>5</v>
       </c>
       <c r="H958" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="959" spans="1:9" x14ac:dyDescent="0.3">
@@ -28105,10 +28111,10 @@
         <v>5</v>
       </c>
       <c r="H962" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="I962" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="963" spans="1:9" x14ac:dyDescent="0.3">
@@ -28350,7 +28356,7 @@
     </row>
     <row r="972" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A972" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B972" t="s">
         <v>1</v>
@@ -28605,10 +28611,10 @@
         <v>11</v>
       </c>
       <c r="H981" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="I981" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="982" spans="1:9" x14ac:dyDescent="0.3">
@@ -28660,10 +28666,10 @@
         <v>3</v>
       </c>
       <c r="H983" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="I983" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="984" spans="1:9" x14ac:dyDescent="0.3">
@@ -28715,7 +28721,7 @@
         <v>3</v>
       </c>
       <c r="H985" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="986" spans="1:9" x14ac:dyDescent="0.3">
@@ -28793,10 +28799,10 @@
         <v>11</v>
       </c>
       <c r="H988" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="I988" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="989" spans="1:9" x14ac:dyDescent="0.3">
@@ -28822,10 +28828,10 @@
         <v>11</v>
       </c>
       <c r="H989" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="I989" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="990" spans="1:9" x14ac:dyDescent="0.3">
@@ -28851,7 +28857,7 @@
         <v>11</v>
       </c>
       <c r="H990" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="991" spans="1:9" x14ac:dyDescent="0.3">
@@ -28880,7 +28886,7 @@
         <v>5</v>
       </c>
       <c r="I991" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="992" spans="1:9" x14ac:dyDescent="0.3">
@@ -28932,7 +28938,7 @@
         <v>5</v>
       </c>
       <c r="H993" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="994" spans="1:9" x14ac:dyDescent="0.3">
@@ -29036,7 +29042,7 @@
         <v>3</v>
       </c>
       <c r="H997" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="998" spans="1:9" x14ac:dyDescent="0.3">
@@ -29062,7 +29068,7 @@
         <v>3</v>
       </c>
       <c r="H998" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="999" spans="1:9" x14ac:dyDescent="0.3">
@@ -29140,7 +29146,7 @@
         <v>11</v>
       </c>
       <c r="H1001" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="1002" spans="1:9" x14ac:dyDescent="0.3">
@@ -29169,7 +29175,7 @@
         <v>5</v>
       </c>
       <c r="I1002" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="1003" spans="1:9" x14ac:dyDescent="0.3">
@@ -29247,10 +29253,10 @@
         <v>11</v>
       </c>
       <c r="H1005" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="I1005" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="1006" spans="1:9" x14ac:dyDescent="0.3">
@@ -29354,7 +29360,7 @@
         <v>3</v>
       </c>
       <c r="H1009" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="I1009" t="s">
         <v>464</v>
@@ -29487,7 +29493,7 @@
         <v>11</v>
       </c>
       <c r="H1014" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="1015" spans="1:9" x14ac:dyDescent="0.3">
@@ -30215,7 +30221,7 @@
         <v>11</v>
       </c>
       <c r="H1042" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="1043" spans="1:8" x14ac:dyDescent="0.3">
@@ -30397,7 +30403,7 @@
         <v>3</v>
       </c>
       <c r="H1049" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="1050" spans="1:8" x14ac:dyDescent="0.3">
@@ -30475,7 +30481,7 @@
         <v>11</v>
       </c>
       <c r="H1052" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="1053" spans="1:8" x14ac:dyDescent="0.3">
@@ -30631,10 +30637,10 @@
         <v>11</v>
       </c>
       <c r="H1058" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="I1058" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="1059" spans="1:9" x14ac:dyDescent="0.3">
@@ -30764,7 +30770,7 @@
         <v>3</v>
       </c>
       <c r="H1063" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="1064" spans="1:9" x14ac:dyDescent="0.3">
@@ -30842,7 +30848,7 @@
         <v>11</v>
       </c>
       <c r="H1066" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="1067" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Found Taurine IS for Arg neg lol
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C240168C-B4CA-41E8-B650-2A10640E88ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7AA839-16B9-4628-B517-5057826E27A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5655" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5654" uniqueCount="738">
   <si>
     <t>Amm</t>
   </si>
@@ -2235,10 +2235,10 @@
     <t>FT2537</t>
   </si>
   <si>
-    <t>Not present???</t>
-  </si>
-  <si>
     <t>FT0189</t>
+  </si>
+  <si>
+    <t>FT1083</t>
   </si>
 </sst>
 </file>
@@ -2564,8 +2564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1093"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A686" workbookViewId="0">
-      <selection activeCell="H700" sqref="H700"/>
+    <sheetView tabSelected="1" topLeftCell="A1077" workbookViewId="0">
+      <selection activeCell="I1093" sqref="I1093"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21224,7 +21224,7 @@
         <v>5</v>
       </c>
       <c r="H700" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="701" spans="1:9" x14ac:dyDescent="0.3">
@@ -31423,7 +31423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1089" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1089" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1089" t="s">
         <v>246</v>
       </c>
@@ -31449,7 +31449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1090" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1090" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1090" t="s">
         <v>246</v>
       </c>
@@ -31475,7 +31475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1091" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1091" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1091" t="s">
         <v>246</v>
       </c>
@@ -31501,7 +31501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1092" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1092" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1092" t="s">
         <v>246</v>
       </c>
@@ -31527,7 +31527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1093" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1093" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1093" t="s">
         <v>246</v>
       </c>
@@ -31550,10 +31550,7 @@
         <v>5</v>
       </c>
       <c r="H1093" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1093" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some annotations apparently?
</commit_message>
<xml_diff>
--- a/untargeted/manual_annotations.xlsx
+++ b/untargeted/manual_annotations.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PARAGON\untargeted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7AA839-16B9-4628-B517-5057826E27A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5975DB2-E5DC-4FE8-94BC-13189741C4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1093</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5654" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5654" uniqueCount="740">
   <si>
     <t>Amm</t>
   </si>
@@ -873,9 +876,6 @@
     <t>Maybe could be rescued? Complicated, not at correct RT</t>
   </si>
   <si>
-    <t>Could be rescued, peak @10.8</t>
-  </si>
-  <si>
     <t>FT1240</t>
   </si>
   <si>
@@ -2239,6 +2239,15 @@
   </si>
   <si>
     <t>FT1083</t>
+  </si>
+  <si>
+    <t>FT1237</t>
+  </si>
+  <si>
+    <t>Saved, peak @10.8</t>
+  </si>
+  <si>
+    <t>FT1569</t>
   </si>
 </sst>
 </file>
@@ -2564,8 +2573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1093"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1077" workbookViewId="0">
-      <selection activeCell="I1093" sqref="I1093"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3579,10 +3588,10 @@
         <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>5</v>
+        <v>737</v>
       </c>
       <c r="I36" t="s">
-        <v>282</v>
+        <v>738</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -3608,7 +3617,7 @@
         <v>3</v>
       </c>
       <c r="H37" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -3634,7 +3643,7 @@
         <v>3</v>
       </c>
       <c r="H38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -3660,10 +3669,10 @@
         <v>3</v>
       </c>
       <c r="H39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I39" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -3689,7 +3698,7 @@
         <v>11</v>
       </c>
       <c r="H40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -3715,7 +3724,7 @@
         <v>3</v>
       </c>
       <c r="H41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I41" t="s">
         <v>277</v>
@@ -3744,7 +3753,7 @@
         <v>3</v>
       </c>
       <c r="H42" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -3770,7 +3779,7 @@
         <v>3</v>
       </c>
       <c r="H43" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -3796,7 +3805,7 @@
         <v>11</v>
       </c>
       <c r="H44" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -3851,7 +3860,7 @@
         <v>11</v>
       </c>
       <c r="H46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -3877,7 +3886,7 @@
         <v>3</v>
       </c>
       <c r="H47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
@@ -3906,7 +3915,7 @@
         <v>5</v>
       </c>
       <c r="I48" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -3932,10 +3941,10 @@
         <v>11</v>
       </c>
       <c r="H49" t="s">
+        <v>293</v>
+      </c>
+      <c r="I49" t="s">
         <v>294</v>
-      </c>
-      <c r="I49" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -3961,7 +3970,7 @@
         <v>11</v>
       </c>
       <c r="H50" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -3987,7 +3996,7 @@
         <v>3</v>
       </c>
       <c r="H51" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -4013,10 +4022,10 @@
         <v>11</v>
       </c>
       <c r="H52" t="s">
+        <v>297</v>
+      </c>
+      <c r="I52" t="s">
         <v>298</v>
-      </c>
-      <c r="I52" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -4100,7 +4109,7 @@
         <v>11</v>
       </c>
       <c r="H55" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -4126,7 +4135,7 @@
         <v>3</v>
       </c>
       <c r="H56" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -4152,7 +4161,7 @@
         <v>3</v>
       </c>
       <c r="H57" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -4178,10 +4187,10 @@
         <v>11</v>
       </c>
       <c r="H58" t="s">
+        <v>302</v>
+      </c>
+      <c r="I58" t="s">
         <v>303</v>
-      </c>
-      <c r="I58" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -4207,7 +4216,7 @@
         <v>3</v>
       </c>
       <c r="H59" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
@@ -4320,10 +4329,10 @@
         <v>3</v>
       </c>
       <c r="H63" t="s">
+        <v>305</v>
+      </c>
+      <c r="I63" t="s">
         <v>306</v>
-      </c>
-      <c r="I63" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -4349,7 +4358,7 @@
         <v>11</v>
       </c>
       <c r="H64" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -4375,7 +4384,7 @@
         <v>3</v>
       </c>
       <c r="H65" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -4430,7 +4439,7 @@
         <v>5</v>
       </c>
       <c r="H67" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -4514,7 +4523,7 @@
         <v>11</v>
       </c>
       <c r="H70" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
@@ -4540,7 +4549,7 @@
         <v>11</v>
       </c>
       <c r="H71" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
@@ -4595,7 +4604,7 @@
         <v>3</v>
       </c>
       <c r="H73" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -4621,7 +4630,7 @@
         <v>11</v>
       </c>
       <c r="H74" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -4647,7 +4656,7 @@
         <v>11</v>
       </c>
       <c r="H75" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -4673,10 +4682,10 @@
         <v>5</v>
       </c>
       <c r="H76" t="s">
+        <v>313</v>
+      </c>
+      <c r="I76" t="s">
         <v>314</v>
-      </c>
-      <c r="I76" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
@@ -4702,10 +4711,10 @@
         <v>5</v>
       </c>
       <c r="H77" t="s">
+        <v>313</v>
+      </c>
+      <c r="I77" t="s">
         <v>314</v>
-      </c>
-      <c r="I77" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
@@ -4731,10 +4740,10 @@
         <v>5</v>
       </c>
       <c r="H78" t="s">
+        <v>313</v>
+      </c>
+      <c r="I78" t="s">
         <v>314</v>
-      </c>
-      <c r="I78" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -4760,7 +4769,7 @@
         <v>5</v>
       </c>
       <c r="H79" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
@@ -4786,7 +4795,7 @@
         <v>5</v>
       </c>
       <c r="H80" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -4812,7 +4821,7 @@
         <v>3</v>
       </c>
       <c r="H81" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -4867,10 +4876,10 @@
         <v>3</v>
       </c>
       <c r="H83" t="s">
+        <v>318</v>
+      </c>
+      <c r="I83" t="s">
         <v>319</v>
-      </c>
-      <c r="I83" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
@@ -4899,7 +4908,7 @@
         <v>5</v>
       </c>
       <c r="I84" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
@@ -4957,7 +4966,7 @@
         <v>5</v>
       </c>
       <c r="I86" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
@@ -5012,7 +5021,7 @@
         <v>5</v>
       </c>
       <c r="H88" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
@@ -5038,7 +5047,7 @@
         <v>3</v>
       </c>
       <c r="H89" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
@@ -5093,7 +5102,7 @@
         <v>3</v>
       </c>
       <c r="H91" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
@@ -5119,7 +5128,7 @@
         <v>11</v>
       </c>
       <c r="H92" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
@@ -5174,7 +5183,7 @@
         <v>11</v>
       </c>
       <c r="H94" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
@@ -5229,7 +5238,7 @@
         <v>3</v>
       </c>
       <c r="H96" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -5255,7 +5264,7 @@
         <v>3</v>
       </c>
       <c r="H97" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
@@ -5281,7 +5290,7 @@
         <v>3</v>
       </c>
       <c r="H98" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
@@ -5307,10 +5316,10 @@
         <v>3</v>
       </c>
       <c r="H99" t="s">
+        <v>328</v>
+      </c>
+      <c r="I99" t="s">
         <v>329</v>
-      </c>
-      <c r="I99" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
@@ -5336,7 +5345,7 @@
         <v>11</v>
       </c>
       <c r="H100" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
@@ -5391,7 +5400,7 @@
         <v>3</v>
       </c>
       <c r="H102" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
@@ -5417,7 +5426,7 @@
         <v>11</v>
       </c>
       <c r="H103" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
@@ -5617,7 +5626,7 @@
         <v>5</v>
       </c>
       <c r="H110" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
@@ -5759,7 +5768,7 @@
         <v>11</v>
       </c>
       <c r="H115" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
@@ -5785,7 +5794,7 @@
         <v>5</v>
       </c>
       <c r="H116" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
@@ -5840,7 +5849,7 @@
         <v>5</v>
       </c>
       <c r="H118" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
@@ -5895,7 +5904,7 @@
         <v>11</v>
       </c>
       <c r="H120" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
@@ -5950,7 +5959,7 @@
         <v>3</v>
       </c>
       <c r="H122" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
@@ -6034,7 +6043,7 @@
         <v>11</v>
       </c>
       <c r="H125" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
@@ -6060,7 +6069,7 @@
         <v>5</v>
       </c>
       <c r="H126" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
@@ -6115,7 +6124,7 @@
         <v>11</v>
       </c>
       <c r="H128" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
@@ -6141,7 +6150,7 @@
         <v>11</v>
       </c>
       <c r="H129" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
@@ -6170,7 +6179,7 @@
         <v>5</v>
       </c>
       <c r="I130" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
@@ -6199,7 +6208,7 @@
         <v>5</v>
       </c>
       <c r="I131" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
@@ -6225,7 +6234,7 @@
         <v>5</v>
       </c>
       <c r="H132" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
@@ -6355,10 +6364,10 @@
         <v>5</v>
       </c>
       <c r="H137" t="s">
+        <v>339</v>
+      </c>
+      <c r="I137" t="s">
         <v>340</v>
-      </c>
-      <c r="I137" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
@@ -6410,7 +6419,7 @@
         <v>5</v>
       </c>
       <c r="H139" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
@@ -6514,10 +6523,10 @@
         <v>5</v>
       </c>
       <c r="H143" t="s">
+        <v>342</v>
+      </c>
+      <c r="I143" t="s">
         <v>343</v>
-      </c>
-      <c r="I143" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
@@ -6736,7 +6745,7 @@
         <v>1</v>
       </c>
       <c r="C152" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D152">
         <v>130.0471</v>
@@ -6751,7 +6760,7 @@
         <v>5</v>
       </c>
       <c r="H152" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
@@ -6762,7 +6771,7 @@
         <v>1</v>
       </c>
       <c r="C153" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D153">
         <v>174.13650000000001</v>
@@ -6777,7 +6786,7 @@
         <v>5</v>
       </c>
       <c r="H153" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
@@ -6803,10 +6812,10 @@
         <v>5</v>
       </c>
       <c r="H154" t="s">
+        <v>354</v>
+      </c>
+      <c r="I154" t="s">
         <v>355</v>
-      </c>
-      <c r="I154" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
@@ -6832,7 +6841,7 @@
         <v>5</v>
       </c>
       <c r="H155" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
@@ -6910,7 +6919,7 @@
         <v>5</v>
       </c>
       <c r="I158" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
@@ -7066,7 +7075,7 @@
         <v>3</v>
       </c>
       <c r="I164" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
@@ -7118,7 +7127,7 @@
         <v>3</v>
       </c>
       <c r="H166" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
@@ -7196,7 +7205,7 @@
         <v>11</v>
       </c>
       <c r="H169" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
@@ -7222,7 +7231,7 @@
         <v>11</v>
       </c>
       <c r="H170" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
@@ -7248,7 +7257,7 @@
         <v>11</v>
       </c>
       <c r="H171" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
@@ -7274,7 +7283,7 @@
         <v>3</v>
       </c>
       <c r="I172" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
@@ -7326,7 +7335,7 @@
         <v>5</v>
       </c>
       <c r="H174" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
@@ -7430,7 +7439,7 @@
         <v>3</v>
       </c>
       <c r="H178" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
@@ -7456,7 +7465,7 @@
         <v>3</v>
       </c>
       <c r="H179" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.3">
@@ -7482,7 +7491,7 @@
         <v>3</v>
       </c>
       <c r="H180" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.3">
@@ -7511,7 +7520,7 @@
         <v>5</v>
       </c>
       <c r="I181" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
@@ -7537,7 +7546,7 @@
         <v>11</v>
       </c>
       <c r="H182" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
@@ -7563,7 +7572,7 @@
         <v>3</v>
       </c>
       <c r="H183" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
@@ -7693,7 +7702,7 @@
         <v>11</v>
       </c>
       <c r="H188" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
@@ -7745,7 +7754,7 @@
         <v>3</v>
       </c>
       <c r="H190" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
@@ -7875,7 +7884,7 @@
         <v>11</v>
       </c>
       <c r="H195" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.3">
@@ -7956,7 +7965,7 @@
         <v>5</v>
       </c>
       <c r="I198" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
@@ -8011,7 +8020,7 @@
         <v>5</v>
       </c>
       <c r="I200" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.3">
@@ -8323,10 +8332,10 @@
         <v>11</v>
       </c>
       <c r="H212" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I212" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.3">
@@ -8456,10 +8465,10 @@
         <v>5</v>
       </c>
       <c r="H217" t="s">
+        <v>373</v>
+      </c>
+      <c r="I217" t="s">
         <v>374</v>
-      </c>
-      <c r="I217" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.3">
@@ -8797,10 +8806,10 @@
         <v>3</v>
       </c>
       <c r="H230" t="s">
+        <v>375</v>
+      </c>
+      <c r="I230" t="s">
         <v>376</v>
-      </c>
-      <c r="I230" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
@@ -8829,7 +8838,7 @@
         <v>5</v>
       </c>
       <c r="I231" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
@@ -9167,7 +9176,7 @@
         <v>3</v>
       </c>
       <c r="H244" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.3">
@@ -9932,7 +9941,7 @@
         <v>155</v>
       </c>
       <c r="C274" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D274">
         <v>128.0325</v>
@@ -9947,7 +9956,7 @@
         <v>5</v>
       </c>
       <c r="H274" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.3">
@@ -10025,10 +10034,10 @@
         <v>3</v>
       </c>
       <c r="H277" t="s">
+        <v>379</v>
+      </c>
+      <c r="I277" t="s">
         <v>380</v>
-      </c>
-      <c r="I277" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.3">
@@ -10080,10 +10089,10 @@
         <v>3</v>
       </c>
       <c r="H279" t="s">
+        <v>381</v>
+      </c>
+      <c r="I279" t="s">
         <v>382</v>
-      </c>
-      <c r="I279" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.3">
@@ -10109,7 +10118,7 @@
         <v>3</v>
       </c>
       <c r="H280" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.3">
@@ -10135,7 +10144,7 @@
         <v>11</v>
       </c>
       <c r="H281" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.3">
@@ -10161,7 +10170,7 @@
         <v>3</v>
       </c>
       <c r="H282" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.3">
@@ -10187,7 +10196,7 @@
         <v>11</v>
       </c>
       <c r="H283" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.3">
@@ -10268,7 +10277,7 @@
         <v>5</v>
       </c>
       <c r="I286" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.3">
@@ -10294,10 +10303,10 @@
         <v>3</v>
       </c>
       <c r="H287" t="s">
+        <v>388</v>
+      </c>
+      <c r="I287" t="s">
         <v>389</v>
-      </c>
-      <c r="I287" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.3">
@@ -10349,7 +10358,7 @@
         <v>11</v>
       </c>
       <c r="H289" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.3">
@@ -10375,10 +10384,10 @@
         <v>3</v>
       </c>
       <c r="H290" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I290" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.3">
@@ -10430,7 +10439,7 @@
         <v>3</v>
       </c>
       <c r="H292" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.3">
@@ -10456,10 +10465,10 @@
         <v>3</v>
       </c>
       <c r="H293" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I293" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">
@@ -10485,7 +10494,7 @@
         <v>3</v>
       </c>
       <c r="H294" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.3">
@@ -10537,10 +10546,10 @@
         <v>3</v>
       </c>
       <c r="H296" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I296" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.3">
@@ -10566,10 +10575,10 @@
         <v>3</v>
       </c>
       <c r="H297" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I297" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.3">
@@ -10595,7 +10604,7 @@
         <v>11</v>
       </c>
       <c r="H298" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.3">
@@ -10676,7 +10685,7 @@
         <v>5</v>
       </c>
       <c r="I301" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.3">
@@ -10728,10 +10737,10 @@
         <v>11</v>
       </c>
       <c r="H303" t="s">
+        <v>398</v>
+      </c>
+      <c r="I303" t="s">
         <v>399</v>
-      </c>
-      <c r="I303" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.3">
@@ -10783,7 +10792,7 @@
         <v>11</v>
       </c>
       <c r="H305" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.3">
@@ -10864,7 +10873,7 @@
         <v>5</v>
       </c>
       <c r="I308" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.3">
@@ -10890,7 +10899,7 @@
         <v>3</v>
       </c>
       <c r="H309" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.3">
@@ -10916,7 +10925,7 @@
         <v>3</v>
       </c>
       <c r="H310" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.3">
@@ -10942,10 +10951,10 @@
         <v>3</v>
       </c>
       <c r="H311" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I311" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.3">
@@ -10971,10 +10980,10 @@
         <v>3</v>
       </c>
       <c r="H312" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I312" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.3">
@@ -11000,7 +11009,7 @@
         <v>11</v>
       </c>
       <c r="H313" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="314" spans="1:9" x14ac:dyDescent="0.3">
@@ -11026,10 +11035,10 @@
         <v>3</v>
       </c>
       <c r="H314" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I314" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.3">
@@ -11055,10 +11064,10 @@
         <v>3</v>
       </c>
       <c r="H315" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I315" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="316" spans="1:9" x14ac:dyDescent="0.3">
@@ -11084,10 +11093,10 @@
         <v>3</v>
       </c>
       <c r="H316" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I316" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="317" spans="1:9" x14ac:dyDescent="0.3">
@@ -11113,7 +11122,7 @@
         <v>11</v>
       </c>
       <c r="H317" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="318" spans="1:9" x14ac:dyDescent="0.3">
@@ -11165,7 +11174,7 @@
         <v>11</v>
       </c>
       <c r="H319" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="320" spans="1:9" x14ac:dyDescent="0.3">
@@ -11191,7 +11200,7 @@
         <v>3</v>
       </c>
       <c r="H320" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.3">
@@ -11220,7 +11229,7 @@
         <v>5</v>
       </c>
       <c r="I321" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="322" spans="1:9" x14ac:dyDescent="0.3">
@@ -11246,7 +11255,7 @@
         <v>11</v>
       </c>
       <c r="H322" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.3">
@@ -11272,7 +11281,7 @@
         <v>11</v>
       </c>
       <c r="H323" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="324" spans="1:9" x14ac:dyDescent="0.3">
@@ -11298,7 +11307,7 @@
         <v>3</v>
       </c>
       <c r="H324" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="325" spans="1:9" x14ac:dyDescent="0.3">
@@ -11324,10 +11333,10 @@
         <v>11</v>
       </c>
       <c r="H325" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I325" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.3">
@@ -11405,7 +11414,7 @@
         <v>11</v>
       </c>
       <c r="H328" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.3">
@@ -11431,7 +11440,7 @@
         <v>3</v>
       </c>
       <c r="H329" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.3">
@@ -11457,7 +11466,7 @@
         <v>3</v>
       </c>
       <c r="H330" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.3">
@@ -11486,7 +11495,7 @@
         <v>5</v>
       </c>
       <c r="I331" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.3">
@@ -11512,7 +11521,7 @@
         <v>3</v>
       </c>
       <c r="H332" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.3">
@@ -11538,10 +11547,10 @@
         <v>3</v>
       </c>
       <c r="H333" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I333" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.3">
@@ -11622,10 +11631,10 @@
         <v>3</v>
       </c>
       <c r="H336" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I336" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="337" spans="1:9" x14ac:dyDescent="0.3">
@@ -11651,7 +11660,7 @@
         <v>11</v>
       </c>
       <c r="H337" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.3">
@@ -11677,10 +11686,10 @@
         <v>3</v>
       </c>
       <c r="H338" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I338" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.3">
@@ -11735,7 +11744,7 @@
         <v>5</v>
       </c>
       <c r="I340" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.3">
@@ -11761,7 +11770,7 @@
         <v>5</v>
       </c>
       <c r="H341" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="342" spans="1:9" x14ac:dyDescent="0.3">
@@ -11813,7 +11822,7 @@
         <v>11</v>
       </c>
       <c r="H343" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.3">
@@ -11891,7 +11900,7 @@
         <v>3</v>
       </c>
       <c r="H346" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.3">
@@ -11917,7 +11926,7 @@
         <v>11</v>
       </c>
       <c r="H347" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.3">
@@ -11943,7 +11952,7 @@
         <v>11</v>
       </c>
       <c r="H348" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="349" spans="1:9" x14ac:dyDescent="0.3">
@@ -11969,10 +11978,10 @@
         <v>5</v>
       </c>
       <c r="H349" t="s">
+        <v>428</v>
+      </c>
+      <c r="I349" t="s">
         <v>429</v>
-      </c>
-      <c r="I349" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.3">
@@ -12050,10 +12059,10 @@
         <v>5</v>
       </c>
       <c r="H352" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I352" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="353" spans="1:9" x14ac:dyDescent="0.3">
@@ -12079,7 +12088,7 @@
         <v>5</v>
       </c>
       <c r="H353" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="354" spans="1:9" x14ac:dyDescent="0.3">
@@ -12105,7 +12114,7 @@
         <v>3</v>
       </c>
       <c r="H354" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="355" spans="1:9" x14ac:dyDescent="0.3">
@@ -12157,10 +12166,10 @@
         <v>3</v>
       </c>
       <c r="H356" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I356" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="357" spans="1:9" x14ac:dyDescent="0.3">
@@ -12241,7 +12250,7 @@
         <v>5</v>
       </c>
       <c r="I359" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.3">
@@ -12293,7 +12302,7 @@
         <v>5</v>
       </c>
       <c r="H361" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.3">
@@ -12319,7 +12328,7 @@
         <v>3</v>
       </c>
       <c r="H362" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.3">
@@ -12371,7 +12380,7 @@
         <v>3</v>
       </c>
       <c r="H364" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.3">
@@ -12397,7 +12406,7 @@
         <v>11</v>
       </c>
       <c r="H365" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.3">
@@ -12449,7 +12458,7 @@
         <v>11</v>
       </c>
       <c r="H367" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="368" spans="1:9" x14ac:dyDescent="0.3">
@@ -12478,7 +12487,7 @@
         <v>5</v>
       </c>
       <c r="I368" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="369" spans="1:9" x14ac:dyDescent="0.3">
@@ -12504,10 +12513,10 @@
         <v>3</v>
       </c>
       <c r="H369" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I369" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="370" spans="1:9" x14ac:dyDescent="0.3">
@@ -12533,7 +12542,7 @@
         <v>3</v>
       </c>
       <c r="H370" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="371" spans="1:9" x14ac:dyDescent="0.3">
@@ -12559,7 +12568,7 @@
         <v>3</v>
       </c>
       <c r="H371" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="372" spans="1:9" x14ac:dyDescent="0.3">
@@ -12585,10 +12594,10 @@
         <v>3</v>
       </c>
       <c r="H372" t="s">
+        <v>442</v>
+      </c>
+      <c r="I372" t="s">
         <v>443</v>
-      </c>
-      <c r="I372" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="373" spans="1:9" x14ac:dyDescent="0.3">
@@ -12614,10 +12623,10 @@
         <v>11</v>
       </c>
       <c r="H373" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I373" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="374" spans="1:9" x14ac:dyDescent="0.3">
@@ -12646,7 +12655,7 @@
         <v>5</v>
       </c>
       <c r="I374" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="375" spans="1:9" x14ac:dyDescent="0.3">
@@ -12672,7 +12681,7 @@
         <v>3</v>
       </c>
       <c r="H375" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="376" spans="1:9" x14ac:dyDescent="0.3">
@@ -12880,7 +12889,7 @@
         <v>5</v>
       </c>
       <c r="H383" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="384" spans="1:9" x14ac:dyDescent="0.3">
@@ -13010,7 +13019,7 @@
         <v>11</v>
       </c>
       <c r="H388" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="389" spans="1:9" x14ac:dyDescent="0.3">
@@ -13036,7 +13045,7 @@
         <v>5</v>
       </c>
       <c r="H389" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="390" spans="1:9" x14ac:dyDescent="0.3">
@@ -13088,7 +13097,7 @@
         <v>5</v>
       </c>
       <c r="H391" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="392" spans="1:9" x14ac:dyDescent="0.3">
@@ -13114,7 +13123,7 @@
         <v>3</v>
       </c>
       <c r="H392" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="393" spans="1:9" x14ac:dyDescent="0.3">
@@ -13140,7 +13149,7 @@
         <v>11</v>
       </c>
       <c r="H393" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="394" spans="1:9" x14ac:dyDescent="0.3">
@@ -13166,10 +13175,10 @@
         <v>11</v>
       </c>
       <c r="H394" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I394" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="395" spans="1:9" x14ac:dyDescent="0.3">
@@ -13195,7 +13204,7 @@
         <v>3</v>
       </c>
       <c r="H395" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="396" spans="1:9" x14ac:dyDescent="0.3">
@@ -13273,7 +13282,7 @@
         <v>11</v>
       </c>
       <c r="H398" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="399" spans="1:9" x14ac:dyDescent="0.3">
@@ -13299,7 +13308,7 @@
         <v>5</v>
       </c>
       <c r="H399" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="400" spans="1:9" x14ac:dyDescent="0.3">
@@ -13351,7 +13360,7 @@
         <v>11</v>
       </c>
       <c r="H401" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="402" spans="1:9" x14ac:dyDescent="0.3">
@@ -13377,7 +13386,7 @@
         <v>11</v>
       </c>
       <c r="H402" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="403" spans="1:9" x14ac:dyDescent="0.3">
@@ -13403,7 +13412,7 @@
         <v>5</v>
       </c>
       <c r="H403" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="404" spans="1:9" x14ac:dyDescent="0.3">
@@ -13432,7 +13441,7 @@
         <v>5</v>
       </c>
       <c r="I404" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="405" spans="1:9" x14ac:dyDescent="0.3">
@@ -13458,7 +13467,7 @@
         <v>5</v>
       </c>
       <c r="H405" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="406" spans="1:9" x14ac:dyDescent="0.3">
@@ -13588,7 +13597,7 @@
         <v>5</v>
       </c>
       <c r="H410" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="411" spans="1:9" x14ac:dyDescent="0.3">
@@ -13640,7 +13649,7 @@
         <v>5</v>
       </c>
       <c r="H412" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="413" spans="1:9" x14ac:dyDescent="0.3">
@@ -13666,10 +13675,10 @@
         <v>5</v>
       </c>
       <c r="H413" t="s">
+        <v>459</v>
+      </c>
+      <c r="I413" t="s">
         <v>460</v>
-      </c>
-      <c r="I413" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="414" spans="1:9" x14ac:dyDescent="0.3">
@@ -13747,7 +13756,7 @@
         <v>5</v>
       </c>
       <c r="H416" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="417" spans="1:9" x14ac:dyDescent="0.3">
@@ -13966,7 +13975,7 @@
         <v>1</v>
       </c>
       <c r="C425" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D425">
         <v>130.0471</v>
@@ -13984,7 +13993,7 @@
         <v>5</v>
       </c>
       <c r="I425" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="426" spans="1:9" x14ac:dyDescent="0.3">
@@ -13995,7 +14004,7 @@
         <v>1</v>
       </c>
       <c r="C426" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D426">
         <v>174.13650000000001</v>
@@ -14013,7 +14022,7 @@
         <v>5</v>
       </c>
       <c r="I426" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="427" spans="1:9" x14ac:dyDescent="0.3">
@@ -14039,10 +14048,10 @@
         <v>5</v>
       </c>
       <c r="H427" t="s">
+        <v>462</v>
+      </c>
+      <c r="I427" t="s">
         <v>463</v>
-      </c>
-      <c r="I427" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="428" spans="1:9" x14ac:dyDescent="0.3">
@@ -14068,7 +14077,7 @@
         <v>5</v>
       </c>
       <c r="H428" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="429" spans="1:9" x14ac:dyDescent="0.3">
@@ -14149,7 +14158,7 @@
         <v>5</v>
       </c>
       <c r="I431" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="432" spans="1:9" x14ac:dyDescent="0.3">
@@ -14253,7 +14262,7 @@
         <v>11</v>
       </c>
       <c r="H435" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="436" spans="1:9" x14ac:dyDescent="0.3">
@@ -14305,7 +14314,7 @@
         <v>3</v>
       </c>
       <c r="H437" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="438" spans="1:9" x14ac:dyDescent="0.3">
@@ -14357,7 +14366,7 @@
         <v>3</v>
       </c>
       <c r="H439" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="440" spans="1:9" x14ac:dyDescent="0.3">
@@ -14435,10 +14444,10 @@
         <v>11</v>
       </c>
       <c r="H442" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I442" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="443" spans="1:9" x14ac:dyDescent="0.3">
@@ -14464,10 +14473,10 @@
         <v>11</v>
       </c>
       <c r="H443" t="s">
+        <v>469</v>
+      </c>
+      <c r="I443" t="s">
         <v>470</v>
-      </c>
-      <c r="I443" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="444" spans="1:9" x14ac:dyDescent="0.3">
@@ -14493,7 +14502,7 @@
         <v>11</v>
       </c>
       <c r="H444" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="445" spans="1:9" x14ac:dyDescent="0.3">
@@ -14522,7 +14531,7 @@
         <v>5</v>
       </c>
       <c r="I445" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="446" spans="1:9" x14ac:dyDescent="0.3">
@@ -14574,7 +14583,7 @@
         <v>5</v>
       </c>
       <c r="I447" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="448" spans="1:9" x14ac:dyDescent="0.3">
@@ -14678,7 +14687,7 @@
         <v>3</v>
       </c>
       <c r="H451" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="452" spans="1:9" x14ac:dyDescent="0.3">
@@ -14704,7 +14713,7 @@
         <v>3</v>
       </c>
       <c r="H452" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="453" spans="1:9" x14ac:dyDescent="0.3">
@@ -14730,7 +14739,7 @@
         <v>3</v>
       </c>
       <c r="H453" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="454" spans="1:9" x14ac:dyDescent="0.3">
@@ -14759,7 +14768,7 @@
         <v>5</v>
       </c>
       <c r="I454" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="455" spans="1:9" x14ac:dyDescent="0.3">
@@ -14785,7 +14794,7 @@
         <v>11</v>
       </c>
       <c r="H455" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="456" spans="1:9" x14ac:dyDescent="0.3">
@@ -14814,7 +14823,7 @@
         <v>5</v>
       </c>
       <c r="I456" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="457" spans="1:9" x14ac:dyDescent="0.3">
@@ -15126,7 +15135,7 @@
         <v>11</v>
       </c>
       <c r="H468" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="469" spans="1:9" x14ac:dyDescent="0.3">
@@ -15204,10 +15213,10 @@
         <v>11</v>
       </c>
       <c r="H471" t="s">
+        <v>478</v>
+      </c>
+      <c r="I471" t="s">
         <v>479</v>
-      </c>
-      <c r="I471" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="472" spans="1:9" x14ac:dyDescent="0.3">
@@ -15259,10 +15268,10 @@
         <v>11</v>
       </c>
       <c r="H473" t="s">
+        <v>480</v>
+      </c>
+      <c r="I473" t="s">
         <v>481</v>
-      </c>
-      <c r="I473" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="474" spans="1:9" x14ac:dyDescent="0.3">
@@ -15574,7 +15583,7 @@
         <v>11</v>
       </c>
       <c r="H485" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="486" spans="1:9" x14ac:dyDescent="0.3">
@@ -15600,7 +15609,7 @@
         <v>11</v>
       </c>
       <c r="H486" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="487" spans="1:9" x14ac:dyDescent="0.3">
@@ -15704,7 +15713,7 @@
         <v>5</v>
       </c>
       <c r="H490" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="491" spans="1:9" x14ac:dyDescent="0.3">
@@ -15834,10 +15843,10 @@
         <v>3</v>
       </c>
       <c r="H495" t="s">
+        <v>485</v>
+      </c>
+      <c r="I495" t="s">
         <v>486</v>
-      </c>
-      <c r="I495" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="496" spans="1:9" x14ac:dyDescent="0.3">
@@ -16253,7 +16262,7 @@
         <v>5</v>
       </c>
       <c r="H511" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="512" spans="1:9" x14ac:dyDescent="0.3">
@@ -16282,7 +16291,7 @@
         <v>5</v>
       </c>
       <c r="I512" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="513" spans="1:8" x14ac:dyDescent="0.3">
@@ -16412,7 +16421,7 @@
         <v>3</v>
       </c>
       <c r="H517" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="518" spans="1:8" x14ac:dyDescent="0.3">
@@ -16490,7 +16499,7 @@
         <v>11</v>
       </c>
       <c r="H520" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="521" spans="1:8" x14ac:dyDescent="0.3">
@@ -17177,7 +17186,7 @@
         <v>155</v>
       </c>
       <c r="C547" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D547">
         <v>128.0325</v>
@@ -17195,7 +17204,7 @@
         <v>5</v>
       </c>
       <c r="I547" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="548" spans="1:9" x14ac:dyDescent="0.3">
@@ -17273,10 +17282,10 @@
         <v>3</v>
       </c>
       <c r="H550" t="s">
+        <v>624</v>
+      </c>
+      <c r="I550" t="s">
         <v>625</v>
-      </c>
-      <c r="I550" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="551" spans="1:9" x14ac:dyDescent="0.3">
@@ -17328,10 +17337,10 @@
         <v>3</v>
       </c>
       <c r="H552" t="s">
+        <v>626</v>
+      </c>
+      <c r="I552" t="s">
         <v>627</v>
-      </c>
-      <c r="I552" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="553" spans="1:9" x14ac:dyDescent="0.3">
@@ -17357,7 +17366,7 @@
         <v>3</v>
       </c>
       <c r="H553" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="554" spans="1:9" x14ac:dyDescent="0.3">
@@ -17383,7 +17392,7 @@
         <v>11</v>
       </c>
       <c r="H554" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="555" spans="1:9" x14ac:dyDescent="0.3">
@@ -17409,7 +17418,7 @@
         <v>3</v>
       </c>
       <c r="H555" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="556" spans="1:9" x14ac:dyDescent="0.3">
@@ -17435,7 +17444,7 @@
         <v>11</v>
       </c>
       <c r="H556" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="557" spans="1:9" x14ac:dyDescent="0.3">
@@ -17516,7 +17525,7 @@
         <v>5</v>
       </c>
       <c r="I559" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="560" spans="1:9" x14ac:dyDescent="0.3">
@@ -17542,7 +17551,7 @@
         <v>3</v>
       </c>
       <c r="H560" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="561" spans="1:9" x14ac:dyDescent="0.3">
@@ -17594,7 +17603,7 @@
         <v>11</v>
       </c>
       <c r="H562" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="563" spans="1:9" x14ac:dyDescent="0.3">
@@ -17620,7 +17629,7 @@
         <v>3</v>
       </c>
       <c r="H563" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="564" spans="1:9" x14ac:dyDescent="0.3">
@@ -17672,7 +17681,7 @@
         <v>3</v>
       </c>
       <c r="H565" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="566" spans="1:9" x14ac:dyDescent="0.3">
@@ -17724,7 +17733,7 @@
         <v>3</v>
       </c>
       <c r="H567" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="568" spans="1:9" x14ac:dyDescent="0.3">
@@ -17776,10 +17785,10 @@
         <v>3</v>
       </c>
       <c r="H569" t="s">
+        <v>638</v>
+      </c>
+      <c r="I569" t="s">
         <v>639</v>
-      </c>
-      <c r="I569" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="570" spans="1:9" x14ac:dyDescent="0.3">
@@ -17805,7 +17814,7 @@
         <v>3</v>
       </c>
       <c r="H570" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="571" spans="1:9" x14ac:dyDescent="0.3">
@@ -17831,7 +17840,7 @@
         <v>11</v>
       </c>
       <c r="H571" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="572" spans="1:9" x14ac:dyDescent="0.3">
@@ -17909,7 +17918,7 @@
         <v>11</v>
       </c>
       <c r="H574" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="575" spans="1:9" x14ac:dyDescent="0.3">
@@ -17961,10 +17970,10 @@
         <v>11</v>
       </c>
       <c r="H576" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="I576" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="577" spans="1:9" x14ac:dyDescent="0.3">
@@ -17990,7 +17999,7 @@
         <v>11</v>
       </c>
       <c r="H577" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.3">
@@ -18016,7 +18025,7 @@
         <v>11</v>
       </c>
       <c r="H578" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.3">
@@ -18042,7 +18051,7 @@
         <v>11</v>
       </c>
       <c r="H579" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="580" spans="1:9" x14ac:dyDescent="0.3">
@@ -18068,10 +18077,10 @@
         <v>3</v>
       </c>
       <c r="H580" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I580" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="581" spans="1:9" x14ac:dyDescent="0.3">
@@ -18123,7 +18132,7 @@
         <v>3</v>
       </c>
       <c r="H582" t="s">
-        <v>5</v>
+        <v>739</v>
       </c>
     </row>
     <row r="583" spans="1:9" x14ac:dyDescent="0.3">
@@ -18149,7 +18158,7 @@
         <v>3</v>
       </c>
       <c r="H583" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="584" spans="1:9" x14ac:dyDescent="0.3">
@@ -18175,10 +18184,10 @@
         <v>3</v>
       </c>
       <c r="H584" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="I584" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="585" spans="1:9" x14ac:dyDescent="0.3">
@@ -18204,10 +18213,10 @@
         <v>3</v>
       </c>
       <c r="H585" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="I585" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="586" spans="1:9" x14ac:dyDescent="0.3">
@@ -18233,7 +18242,7 @@
         <v>11</v>
       </c>
       <c r="H586" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="587" spans="1:9" x14ac:dyDescent="0.3">
@@ -18259,10 +18268,10 @@
         <v>3</v>
       </c>
       <c r="H587" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I587" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="588" spans="1:9" x14ac:dyDescent="0.3">
@@ -18288,10 +18297,10 @@
         <v>3</v>
       </c>
       <c r="H588" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="I588" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="589" spans="1:9" x14ac:dyDescent="0.3">
@@ -18317,7 +18326,7 @@
         <v>3</v>
       </c>
       <c r="H589" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="590" spans="1:9" x14ac:dyDescent="0.3">
@@ -18343,7 +18352,7 @@
         <v>11</v>
       </c>
       <c r="H590" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="591" spans="1:9" x14ac:dyDescent="0.3">
@@ -18395,7 +18404,7 @@
         <v>11</v>
       </c>
       <c r="H592" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="593" spans="1:8" x14ac:dyDescent="0.3">
@@ -18421,7 +18430,7 @@
         <v>3</v>
       </c>
       <c r="H593" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="594" spans="1:8" x14ac:dyDescent="0.3">
@@ -18473,7 +18482,7 @@
         <v>11</v>
       </c>
       <c r="H595" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="596" spans="1:8" x14ac:dyDescent="0.3">
@@ -18499,7 +18508,7 @@
         <v>11</v>
       </c>
       <c r="H596" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="597" spans="1:8" x14ac:dyDescent="0.3">
@@ -18525,7 +18534,7 @@
         <v>3</v>
       </c>
       <c r="H597" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="598" spans="1:8" x14ac:dyDescent="0.3">
@@ -18551,7 +18560,7 @@
         <v>11</v>
       </c>
       <c r="H598" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="599" spans="1:8" x14ac:dyDescent="0.3">
@@ -18629,7 +18638,7 @@
         <v>11</v>
       </c>
       <c r="H601" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="602" spans="1:8" x14ac:dyDescent="0.3">
@@ -18655,7 +18664,7 @@
         <v>3</v>
       </c>
       <c r="H602" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="603" spans="1:8" x14ac:dyDescent="0.3">
@@ -18681,7 +18690,7 @@
         <v>3</v>
       </c>
       <c r="H603" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="604" spans="1:8" x14ac:dyDescent="0.3">
@@ -18707,7 +18716,7 @@
         <v>11</v>
       </c>
       <c r="H604" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="605" spans="1:8" x14ac:dyDescent="0.3">
@@ -18733,7 +18742,7 @@
         <v>3</v>
       </c>
       <c r="H605" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="606" spans="1:8" x14ac:dyDescent="0.3">
@@ -18759,7 +18768,7 @@
         <v>3</v>
       </c>
       <c r="H606" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="607" spans="1:8" x14ac:dyDescent="0.3">
@@ -18837,7 +18846,7 @@
         <v>3</v>
       </c>
       <c r="H609" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="610" spans="1:9" x14ac:dyDescent="0.3">
@@ -18863,7 +18872,7 @@
         <v>11</v>
       </c>
       <c r="H610" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="611" spans="1:9" x14ac:dyDescent="0.3">
@@ -18889,7 +18898,7 @@
         <v>3</v>
       </c>
       <c r="H611" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="612" spans="1:9" x14ac:dyDescent="0.3">
@@ -19019,7 +19028,7 @@
         <v>11</v>
       </c>
       <c r="H616" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="617" spans="1:9" x14ac:dyDescent="0.3">
@@ -19045,7 +19054,7 @@
         <v>11</v>
       </c>
       <c r="H617" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="618" spans="1:9" x14ac:dyDescent="0.3">
@@ -19097,7 +19106,7 @@
         <v>3</v>
       </c>
       <c r="H619" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="620" spans="1:9" x14ac:dyDescent="0.3">
@@ -19123,10 +19132,10 @@
         <v>11</v>
       </c>
       <c r="H620" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I620" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="621" spans="1:9" x14ac:dyDescent="0.3">
@@ -19152,7 +19161,7 @@
         <v>11</v>
       </c>
       <c r="H621" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="622" spans="1:9" x14ac:dyDescent="0.3">
@@ -19204,10 +19213,10 @@
         <v>5</v>
       </c>
       <c r="H623" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I623" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="624" spans="1:9" x14ac:dyDescent="0.3">
@@ -19259,7 +19268,7 @@
         <v>5</v>
       </c>
       <c r="H625" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="626" spans="1:9" x14ac:dyDescent="0.3">
@@ -19285,7 +19294,7 @@
         <v>5</v>
       </c>
       <c r="H626" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="627" spans="1:9" x14ac:dyDescent="0.3">
@@ -19311,7 +19320,7 @@
         <v>3</v>
       </c>
       <c r="H627" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="628" spans="1:9" x14ac:dyDescent="0.3">
@@ -19363,7 +19372,7 @@
         <v>3</v>
       </c>
       <c r="H629" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="630" spans="1:9" x14ac:dyDescent="0.3">
@@ -19392,7 +19401,7 @@
         <v>5</v>
       </c>
       <c r="I630" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="631" spans="1:9" x14ac:dyDescent="0.3">
@@ -19444,7 +19453,7 @@
         <v>3</v>
       </c>
       <c r="H632" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="633" spans="1:9" x14ac:dyDescent="0.3">
@@ -19496,7 +19505,7 @@
         <v>5</v>
       </c>
       <c r="H634" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="635" spans="1:9" x14ac:dyDescent="0.3">
@@ -19522,7 +19531,7 @@
         <v>3</v>
       </c>
       <c r="H635" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="636" spans="1:9" x14ac:dyDescent="0.3">
@@ -19574,7 +19583,7 @@
         <v>3</v>
       </c>
       <c r="H637" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="638" spans="1:9" x14ac:dyDescent="0.3">
@@ -19600,7 +19609,7 @@
         <v>11</v>
       </c>
       <c r="H638" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="639" spans="1:9" x14ac:dyDescent="0.3">
@@ -19652,7 +19661,7 @@
         <v>11</v>
       </c>
       <c r="H640" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="641" spans="1:9" x14ac:dyDescent="0.3">
@@ -19704,7 +19713,7 @@
         <v>3</v>
       </c>
       <c r="H642" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="643" spans="1:9" x14ac:dyDescent="0.3">
@@ -19730,10 +19739,10 @@
         <v>3</v>
       </c>
       <c r="H643" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="I643" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="644" spans="1:9" x14ac:dyDescent="0.3">
@@ -19759,7 +19768,7 @@
         <v>3</v>
       </c>
       <c r="H644" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="645" spans="1:9" x14ac:dyDescent="0.3">
@@ -19785,7 +19794,7 @@
         <v>3</v>
       </c>
       <c r="H645" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="646" spans="1:9" x14ac:dyDescent="0.3">
@@ -19863,7 +19872,7 @@
         <v>3</v>
       </c>
       <c r="H648" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="649" spans="1:9" x14ac:dyDescent="0.3">
@@ -20071,7 +20080,7 @@
         <v>5</v>
       </c>
       <c r="H656" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="657" spans="1:9" x14ac:dyDescent="0.3">
@@ -20097,7 +20106,7 @@
         <v>3</v>
       </c>
       <c r="H657" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="658" spans="1:9" x14ac:dyDescent="0.3">
@@ -20201,7 +20210,7 @@
         <v>11</v>
       </c>
       <c r="H661" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="662" spans="1:9" x14ac:dyDescent="0.3">
@@ -20227,7 +20236,7 @@
         <v>5</v>
       </c>
       <c r="H662" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="663" spans="1:9" x14ac:dyDescent="0.3">
@@ -20253,7 +20262,7 @@
         <v>5</v>
       </c>
       <c r="H663" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="664" spans="1:9" x14ac:dyDescent="0.3">
@@ -20308,7 +20317,7 @@
         <v>5</v>
       </c>
       <c r="I665" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="666" spans="1:9" x14ac:dyDescent="0.3">
@@ -20334,7 +20343,7 @@
         <v>11</v>
       </c>
       <c r="H666" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="667" spans="1:9" x14ac:dyDescent="0.3">
@@ -20360,7 +20369,7 @@
         <v>11</v>
       </c>
       <c r="H667" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="668" spans="1:9" x14ac:dyDescent="0.3">
@@ -20386,7 +20395,7 @@
         <v>3</v>
       </c>
       <c r="H668" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="669" spans="1:9" x14ac:dyDescent="0.3">
@@ -20464,7 +20473,7 @@
         <v>11</v>
       </c>
       <c r="H671" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="672" spans="1:9" x14ac:dyDescent="0.3">
@@ -20490,7 +20499,7 @@
         <v>5</v>
       </c>
       <c r="H672" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="673" spans="1:8" x14ac:dyDescent="0.3">
@@ -20542,7 +20551,7 @@
         <v>11</v>
       </c>
       <c r="H674" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="675" spans="1:8" x14ac:dyDescent="0.3">
@@ -20568,7 +20577,7 @@
         <v>11</v>
       </c>
       <c r="H675" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="676" spans="1:8" x14ac:dyDescent="0.3">
@@ -20594,7 +20603,7 @@
         <v>5</v>
       </c>
       <c r="H676" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="677" spans="1:8" x14ac:dyDescent="0.3">
@@ -20620,7 +20629,7 @@
         <v>5</v>
       </c>
       <c r="H677" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="678" spans="1:8" x14ac:dyDescent="0.3">
@@ -20646,7 +20655,7 @@
         <v>5</v>
       </c>
       <c r="H678" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="679" spans="1:8" x14ac:dyDescent="0.3">
@@ -20776,7 +20785,7 @@
         <v>5</v>
       </c>
       <c r="H683" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="684" spans="1:8" x14ac:dyDescent="0.3">
@@ -20828,7 +20837,7 @@
         <v>5</v>
       </c>
       <c r="H685" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="686" spans="1:8" x14ac:dyDescent="0.3">
@@ -20932,10 +20941,10 @@
         <v>5</v>
       </c>
       <c r="H689" t="s">
+        <v>701</v>
+      </c>
+      <c r="I689" t="s">
         <v>702</v>
-      </c>
-      <c r="I689" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="690" spans="1:9" x14ac:dyDescent="0.3">
@@ -21154,7 +21163,7 @@
         <v>1</v>
       </c>
       <c r="C698" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D698">
         <v>130.0471</v>
@@ -21169,7 +21178,7 @@
         <v>5</v>
       </c>
       <c r="H698" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="699" spans="1:9" x14ac:dyDescent="0.3">
@@ -21180,7 +21189,7 @@
         <v>1</v>
       </c>
       <c r="C699" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D699">
         <v>174.13650000000001</v>
@@ -21195,10 +21204,10 @@
         <v>5</v>
       </c>
       <c r="H699" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="I699" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="700" spans="1:9" x14ac:dyDescent="0.3">
@@ -21224,7 +21233,7 @@
         <v>5</v>
       </c>
       <c r="H700" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="701" spans="1:9" x14ac:dyDescent="0.3">
@@ -21250,7 +21259,7 @@
         <v>5</v>
       </c>
       <c r="H701" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="702" spans="1:9" x14ac:dyDescent="0.3">
@@ -21432,10 +21441,10 @@
         <v>11</v>
       </c>
       <c r="H708" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="I708" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="709" spans="1:9" x14ac:dyDescent="0.3">
@@ -21490,7 +21499,7 @@
         <v>5</v>
       </c>
       <c r="I710" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="711" spans="1:9" x14ac:dyDescent="0.3">
@@ -21542,7 +21551,7 @@
         <v>3</v>
       </c>
       <c r="H712" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="713" spans="1:9" x14ac:dyDescent="0.3">
@@ -21620,7 +21629,7 @@
         <v>11</v>
       </c>
       <c r="H715" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="716" spans="1:9" x14ac:dyDescent="0.3">
@@ -21646,10 +21655,10 @@
         <v>11</v>
       </c>
       <c r="H716" t="s">
+        <v>706</v>
+      </c>
+      <c r="I716" t="s">
         <v>707</v>
-      </c>
-      <c r="I716" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="717" spans="1:9" x14ac:dyDescent="0.3">
@@ -21675,7 +21684,7 @@
         <v>11</v>
       </c>
       <c r="H717" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="718" spans="1:9" x14ac:dyDescent="0.3">
@@ -21701,7 +21710,7 @@
         <v>3</v>
       </c>
       <c r="H718" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="719" spans="1:9" x14ac:dyDescent="0.3">
@@ -21857,7 +21866,7 @@
         <v>3</v>
       </c>
       <c r="H724" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="725" spans="1:8" x14ac:dyDescent="0.3">
@@ -21883,7 +21892,7 @@
         <v>3</v>
       </c>
       <c r="H725" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="726" spans="1:8" x14ac:dyDescent="0.3">
@@ -21909,7 +21918,7 @@
         <v>3</v>
       </c>
       <c r="H726" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="727" spans="1:8" x14ac:dyDescent="0.3">
@@ -21961,7 +21970,7 @@
         <v>11</v>
       </c>
       <c r="H728" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="729" spans="1:8" x14ac:dyDescent="0.3">
@@ -21987,7 +21996,7 @@
         <v>3</v>
       </c>
       <c r="H729" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="730" spans="1:8" x14ac:dyDescent="0.3">
@@ -22169,7 +22178,7 @@
         <v>3</v>
       </c>
       <c r="H736" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="737" spans="1:8" x14ac:dyDescent="0.3">
@@ -22299,7 +22308,7 @@
         <v>11</v>
       </c>
       <c r="H741" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="742" spans="1:8" x14ac:dyDescent="0.3">
@@ -22741,7 +22750,7 @@
         <v>11</v>
       </c>
       <c r="H758" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="759" spans="1:8" x14ac:dyDescent="0.3">
@@ -22871,7 +22880,7 @@
         <v>5</v>
       </c>
       <c r="H763" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="764" spans="1:8" x14ac:dyDescent="0.3">
@@ -23209,7 +23218,7 @@
         <v>3</v>
       </c>
       <c r="H776" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="777" spans="1:9" x14ac:dyDescent="0.3">
@@ -23235,7 +23244,7 @@
         <v>11</v>
       </c>
       <c r="H777" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="778" spans="1:9" x14ac:dyDescent="0.3">
@@ -23287,7 +23296,7 @@
         <v>11</v>
       </c>
       <c r="H779" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="780" spans="1:9" x14ac:dyDescent="0.3">
@@ -23394,7 +23403,7 @@
         <v>5</v>
       </c>
       <c r="I783" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="784" spans="1:9" x14ac:dyDescent="0.3">
@@ -23420,7 +23429,7 @@
         <v>5</v>
       </c>
       <c r="H784" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="785" spans="1:8" x14ac:dyDescent="0.3">
@@ -23576,7 +23585,7 @@
         <v>3</v>
       </c>
       <c r="H790" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="791" spans="1:8" x14ac:dyDescent="0.3">
@@ -23654,7 +23663,7 @@
         <v>11</v>
       </c>
       <c r="H793" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="794" spans="1:8" x14ac:dyDescent="0.3">
@@ -24341,7 +24350,7 @@
         <v>155</v>
       </c>
       <c r="C820" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D820">
         <v>128.0325</v>
@@ -24356,7 +24365,7 @@
         <v>5</v>
       </c>
       <c r="H820" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="821" spans="1:8" x14ac:dyDescent="0.3">
@@ -24434,7 +24443,7 @@
         <v>3</v>
       </c>
       <c r="H823" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="824" spans="1:8" x14ac:dyDescent="0.3">
@@ -24486,7 +24495,7 @@
         <v>3</v>
       </c>
       <c r="H825" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="826" spans="1:8" x14ac:dyDescent="0.3">
@@ -24512,7 +24521,7 @@
         <v>3</v>
       </c>
       <c r="H826" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="827" spans="1:8" x14ac:dyDescent="0.3">
@@ -24564,7 +24573,7 @@
         <v>3</v>
       </c>
       <c r="H828" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="829" spans="1:8" x14ac:dyDescent="0.3">
@@ -24590,7 +24599,7 @@
         <v>11</v>
       </c>
       <c r="H829" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="830" spans="1:8" x14ac:dyDescent="0.3">
@@ -24694,7 +24703,7 @@
         <v>3</v>
       </c>
       <c r="H833" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="834" spans="1:9" x14ac:dyDescent="0.3">
@@ -24746,10 +24755,10 @@
         <v>11</v>
       </c>
       <c r="H835" t="s">
+        <v>600</v>
+      </c>
+      <c r="I835" t="s">
         <v>601</v>
-      </c>
-      <c r="I835" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="836" spans="1:9" x14ac:dyDescent="0.3">
@@ -24775,7 +24784,7 @@
         <v>3</v>
       </c>
       <c r="H836" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="837" spans="1:9" x14ac:dyDescent="0.3">
@@ -24827,7 +24836,7 @@
         <v>3</v>
       </c>
       <c r="H838" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="839" spans="1:9" x14ac:dyDescent="0.3">
@@ -24879,10 +24888,10 @@
         <v>3</v>
       </c>
       <c r="H840" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I840" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="841" spans="1:9" x14ac:dyDescent="0.3">
@@ -24934,7 +24943,7 @@
         <v>3</v>
       </c>
       <c r="H842" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="843" spans="1:9" x14ac:dyDescent="0.3">
@@ -24960,7 +24969,7 @@
         <v>3</v>
       </c>
       <c r="H843" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="844" spans="1:9" x14ac:dyDescent="0.3">
@@ -24986,7 +24995,7 @@
         <v>11</v>
       </c>
       <c r="H844" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="845" spans="1:9" x14ac:dyDescent="0.3">
@@ -25116,10 +25125,10 @@
         <v>11</v>
       </c>
       <c r="H849" t="s">
+        <v>603</v>
+      </c>
+      <c r="I849" t="s">
         <v>604</v>
-      </c>
-      <c r="I849" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="850" spans="1:9" x14ac:dyDescent="0.3">
@@ -25171,7 +25180,7 @@
         <v>11</v>
       </c>
       <c r="H851" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="852" spans="1:9" x14ac:dyDescent="0.3">
@@ -25197,10 +25206,10 @@
         <v>11</v>
       </c>
       <c r="H852" t="s">
+        <v>521</v>
+      </c>
+      <c r="I852" t="s">
         <v>522</v>
-      </c>
-      <c r="I852" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="853" spans="1:9" x14ac:dyDescent="0.3">
@@ -25226,10 +25235,10 @@
         <v>3</v>
       </c>
       <c r="H853" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I853" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="854" spans="1:9" x14ac:dyDescent="0.3">
@@ -25258,7 +25267,7 @@
         <v>5</v>
       </c>
       <c r="I854" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="855" spans="1:9" x14ac:dyDescent="0.3">
@@ -25284,7 +25293,7 @@
         <v>3</v>
       </c>
       <c r="H855" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="856" spans="1:9" x14ac:dyDescent="0.3">
@@ -25310,7 +25319,7 @@
         <v>3</v>
       </c>
       <c r="H856" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="857" spans="1:9" x14ac:dyDescent="0.3">
@@ -25362,10 +25371,10 @@
         <v>3</v>
       </c>
       <c r="H858" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I858" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="859" spans="1:9" x14ac:dyDescent="0.3">
@@ -25391,10 +25400,10 @@
         <v>11</v>
       </c>
       <c r="H859" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I859" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="860" spans="1:9" x14ac:dyDescent="0.3">
@@ -25420,7 +25429,7 @@
         <v>3</v>
       </c>
       <c r="H860" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="861" spans="1:9" x14ac:dyDescent="0.3">
@@ -25446,10 +25455,10 @@
         <v>3</v>
       </c>
       <c r="H861" t="s">
+        <v>608</v>
+      </c>
+      <c r="I861" t="s">
         <v>609</v>
-      </c>
-      <c r="I861" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="862" spans="1:9" x14ac:dyDescent="0.3">
@@ -25475,7 +25484,7 @@
         <v>3</v>
       </c>
       <c r="H862" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="863" spans="1:9" x14ac:dyDescent="0.3">
@@ -25501,10 +25510,10 @@
         <v>11</v>
       </c>
       <c r="H863" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I863" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="864" spans="1:9" x14ac:dyDescent="0.3">
@@ -25556,7 +25565,7 @@
         <v>11</v>
       </c>
       <c r="H865" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="866" spans="1:9" x14ac:dyDescent="0.3">
@@ -25582,7 +25591,7 @@
         <v>3</v>
       </c>
       <c r="H866" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="867" spans="1:9" x14ac:dyDescent="0.3">
@@ -25634,7 +25643,7 @@
         <v>11</v>
       </c>
       <c r="H868" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="869" spans="1:9" x14ac:dyDescent="0.3">
@@ -25660,7 +25669,7 @@
         <v>11</v>
       </c>
       <c r="H869" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="870" spans="1:9" x14ac:dyDescent="0.3">
@@ -25686,7 +25695,7 @@
         <v>3</v>
       </c>
       <c r="H870" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="871" spans="1:9" x14ac:dyDescent="0.3">
@@ -25790,7 +25799,7 @@
         <v>11</v>
       </c>
       <c r="H874" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="875" spans="1:9" x14ac:dyDescent="0.3">
@@ -25816,7 +25825,7 @@
         <v>3</v>
       </c>
       <c r="H875" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="876" spans="1:9" x14ac:dyDescent="0.3">
@@ -25842,7 +25851,7 @@
         <v>3</v>
       </c>
       <c r="H876" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="877" spans="1:9" x14ac:dyDescent="0.3">
@@ -25868,10 +25877,10 @@
         <v>11</v>
       </c>
       <c r="H877" t="s">
+        <v>535</v>
+      </c>
+      <c r="I877" t="s">
         <v>536</v>
-      </c>
-      <c r="I877" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="878" spans="1:9" x14ac:dyDescent="0.3">
@@ -25897,7 +25906,7 @@
         <v>3</v>
       </c>
       <c r="H878" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="879" spans="1:9" x14ac:dyDescent="0.3">
@@ -25923,10 +25932,10 @@
         <v>3</v>
       </c>
       <c r="H879" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I879" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="880" spans="1:9" x14ac:dyDescent="0.3">
@@ -26004,7 +26013,7 @@
         <v>3</v>
       </c>
       <c r="H882" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="883" spans="1:9" x14ac:dyDescent="0.3">
@@ -26030,7 +26039,7 @@
         <v>11</v>
       </c>
       <c r="H883" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="884" spans="1:9" x14ac:dyDescent="0.3">
@@ -26056,7 +26065,7 @@
         <v>3</v>
       </c>
       <c r="H884" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="885" spans="1:9" x14ac:dyDescent="0.3">
@@ -26186,10 +26195,10 @@
         <v>11</v>
       </c>
       <c r="H889" t="s">
+        <v>540</v>
+      </c>
+      <c r="I889" t="s">
         <v>541</v>
-      </c>
-      <c r="I889" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="890" spans="1:9" x14ac:dyDescent="0.3">
@@ -26215,10 +26224,10 @@
         <v>11</v>
       </c>
       <c r="H890" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I890" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="891" spans="1:9" x14ac:dyDescent="0.3">
@@ -26270,7 +26279,7 @@
         <v>3</v>
       </c>
       <c r="H892" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="893" spans="1:9" x14ac:dyDescent="0.3">
@@ -26296,10 +26305,10 @@
         <v>11</v>
       </c>
       <c r="H893" t="s">
+        <v>544</v>
+      </c>
+      <c r="I893" t="s">
         <v>545</v>
-      </c>
-      <c r="I893" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="894" spans="1:9" x14ac:dyDescent="0.3">
@@ -26325,7 +26334,7 @@
         <v>11</v>
       </c>
       <c r="H894" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="895" spans="1:9" x14ac:dyDescent="0.3">
@@ -26377,10 +26386,10 @@
         <v>5</v>
       </c>
       <c r="H896" t="s">
+        <v>547</v>
+      </c>
+      <c r="I896" t="s">
         <v>548</v>
-      </c>
-      <c r="I896" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="897" spans="1:9" x14ac:dyDescent="0.3">
@@ -26406,7 +26415,7 @@
         <v>5</v>
       </c>
       <c r="H897" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="898" spans="1:9" x14ac:dyDescent="0.3">
@@ -26432,7 +26441,7 @@
         <v>5</v>
       </c>
       <c r="H898" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="899" spans="1:9" x14ac:dyDescent="0.3">
@@ -26458,7 +26467,7 @@
         <v>5</v>
       </c>
       <c r="H899" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="900" spans="1:9" x14ac:dyDescent="0.3">
@@ -26484,7 +26493,7 @@
         <v>3</v>
       </c>
       <c r="H900" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="901" spans="1:9" x14ac:dyDescent="0.3">
@@ -26536,7 +26545,7 @@
         <v>3</v>
       </c>
       <c r="H902" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="903" spans="1:9" x14ac:dyDescent="0.3">
@@ -26614,10 +26623,10 @@
         <v>3</v>
       </c>
       <c r="H905" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I905" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="906" spans="1:9" x14ac:dyDescent="0.3">
@@ -26669,7 +26678,7 @@
         <v>5</v>
       </c>
       <c r="H907" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="908" spans="1:9" x14ac:dyDescent="0.3">
@@ -26695,7 +26704,7 @@
         <v>3</v>
       </c>
       <c r="H908" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="909" spans="1:9" x14ac:dyDescent="0.3">
@@ -26747,7 +26756,7 @@
         <v>3</v>
       </c>
       <c r="H910" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="911" spans="1:9" x14ac:dyDescent="0.3">
@@ -26773,7 +26782,7 @@
         <v>11</v>
       </c>
       <c r="H911" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="912" spans="1:9" x14ac:dyDescent="0.3">
@@ -26825,7 +26834,7 @@
         <v>11</v>
       </c>
       <c r="H913" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="914" spans="1:9" x14ac:dyDescent="0.3">
@@ -26851,7 +26860,7 @@
         <v>3</v>
       </c>
       <c r="H914" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="915" spans="1:9" x14ac:dyDescent="0.3">
@@ -26877,7 +26886,7 @@
         <v>3</v>
       </c>
       <c r="H915" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="916" spans="1:9" x14ac:dyDescent="0.3">
@@ -26903,7 +26912,7 @@
         <v>3</v>
       </c>
       <c r="H916" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="917" spans="1:9" x14ac:dyDescent="0.3">
@@ -26929,7 +26938,7 @@
         <v>3</v>
       </c>
       <c r="H917" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="918" spans="1:9" x14ac:dyDescent="0.3">
@@ -26955,7 +26964,7 @@
         <v>3</v>
       </c>
       <c r="H918" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="919" spans="1:9" x14ac:dyDescent="0.3">
@@ -26981,10 +26990,10 @@
         <v>11</v>
       </c>
       <c r="H919" t="s">
+        <v>615</v>
+      </c>
+      <c r="I919" t="s">
         <v>616</v>
-      </c>
-      <c r="I919" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="920" spans="1:9" x14ac:dyDescent="0.3">
@@ -27036,7 +27045,7 @@
         <v>3</v>
       </c>
       <c r="H921" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="922" spans="1:9" x14ac:dyDescent="0.3">
@@ -27062,10 +27071,10 @@
         <v>11</v>
       </c>
       <c r="H922" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I922" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="923" spans="1:9" x14ac:dyDescent="0.3">
@@ -27247,7 +27256,7 @@
         <v>5</v>
       </c>
       <c r="H929" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="930" spans="1:9" x14ac:dyDescent="0.3">
@@ -27377,7 +27386,7 @@
         <v>11</v>
       </c>
       <c r="H934" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="935" spans="1:9" x14ac:dyDescent="0.3">
@@ -27403,7 +27412,7 @@
         <v>5</v>
       </c>
       <c r="H935" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="936" spans="1:9" x14ac:dyDescent="0.3">
@@ -27507,7 +27516,7 @@
         <v>11</v>
       </c>
       <c r="H939" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="940" spans="1:9" x14ac:dyDescent="0.3">
@@ -27533,10 +27542,10 @@
         <v>11</v>
       </c>
       <c r="H940" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="I940" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="941" spans="1:9" x14ac:dyDescent="0.3">
@@ -27562,7 +27571,7 @@
         <v>3</v>
       </c>
       <c r="H941" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="942" spans="1:9" x14ac:dyDescent="0.3">
@@ -27640,7 +27649,7 @@
         <v>11</v>
       </c>
       <c r="H944" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="945" spans="1:9" x14ac:dyDescent="0.3">
@@ -27666,7 +27675,7 @@
         <v>5</v>
       </c>
       <c r="H945" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="946" spans="1:9" x14ac:dyDescent="0.3">
@@ -27718,10 +27727,10 @@
         <v>11</v>
       </c>
       <c r="H947" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I947" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="948" spans="1:9" x14ac:dyDescent="0.3">
@@ -27747,7 +27756,7 @@
         <v>11</v>
       </c>
       <c r="H948" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="949" spans="1:9" x14ac:dyDescent="0.3">
@@ -27773,7 +27782,7 @@
         <v>5</v>
       </c>
       <c r="H949" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="950" spans="1:9" x14ac:dyDescent="0.3">
@@ -27799,7 +27808,7 @@
         <v>5</v>
       </c>
       <c r="H950" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="951" spans="1:9" x14ac:dyDescent="0.3">
@@ -27825,7 +27834,7 @@
         <v>5</v>
       </c>
       <c r="H951" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="952" spans="1:9" x14ac:dyDescent="0.3">
@@ -27955,7 +27964,7 @@
         <v>5</v>
       </c>
       <c r="H956" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="957" spans="1:9" x14ac:dyDescent="0.3">
@@ -28007,7 +28016,7 @@
         <v>5</v>
       </c>
       <c r="H958" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="959" spans="1:9" x14ac:dyDescent="0.3">
@@ -28111,10 +28120,10 @@
         <v>5</v>
       </c>
       <c r="H962" t="s">
+        <v>578</v>
+      </c>
+      <c r="I962" t="s">
         <v>579</v>
-      </c>
-      <c r="I962" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="963" spans="1:9" x14ac:dyDescent="0.3">
@@ -28333,7 +28342,7 @@
         <v>1</v>
       </c>
       <c r="C971" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D971">
         <v>130.0471</v>
@@ -28348,10 +28357,10 @@
         <v>5</v>
       </c>
       <c r="H971" t="s">
+        <v>732</v>
+      </c>
+      <c r="I971" t="s">
         <v>733</v>
-      </c>
-      <c r="I971" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="972" spans="1:9" x14ac:dyDescent="0.3">
@@ -28362,7 +28371,7 @@
         <v>1</v>
       </c>
       <c r="C972" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D972">
         <v>174.13650000000001</v>
@@ -28377,7 +28386,7 @@
         <v>5</v>
       </c>
       <c r="H972" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="973" spans="1:9" x14ac:dyDescent="0.3">
@@ -28611,10 +28620,10 @@
         <v>11</v>
       </c>
       <c r="H981" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I981" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="982" spans="1:9" x14ac:dyDescent="0.3">
@@ -28666,10 +28675,10 @@
         <v>3</v>
       </c>
       <c r="H983" t="s">
+        <v>580</v>
+      </c>
+      <c r="I983" t="s">
         <v>581</v>
-      </c>
-      <c r="I983" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="984" spans="1:9" x14ac:dyDescent="0.3">
@@ -28721,7 +28730,7 @@
         <v>3</v>
       </c>
       <c r="H985" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="986" spans="1:9" x14ac:dyDescent="0.3">
@@ -28799,10 +28808,10 @@
         <v>11</v>
       </c>
       <c r="H988" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I988" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="989" spans="1:9" x14ac:dyDescent="0.3">
@@ -28828,10 +28837,10 @@
         <v>11</v>
       </c>
       <c r="H989" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I989" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="990" spans="1:9" x14ac:dyDescent="0.3">
@@ -28857,7 +28866,7 @@
         <v>11</v>
       </c>
       <c r="H990" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="991" spans="1:9" x14ac:dyDescent="0.3">
@@ -28886,7 +28895,7 @@
         <v>5</v>
       </c>
       <c r="I991" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="992" spans="1:9" x14ac:dyDescent="0.3">
@@ -28938,7 +28947,7 @@
         <v>5</v>
       </c>
       <c r="H993" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="994" spans="1:9" x14ac:dyDescent="0.3">
@@ -29042,7 +29051,7 @@
         <v>3</v>
       </c>
       <c r="H997" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="998" spans="1:9" x14ac:dyDescent="0.3">
@@ -29068,7 +29077,7 @@
         <v>3</v>
       </c>
       <c r="H998" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="999" spans="1:9" x14ac:dyDescent="0.3">
@@ -29094,7 +29103,7 @@
         <v>3</v>
       </c>
       <c r="H999" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="1000" spans="1:9" x14ac:dyDescent="0.3">
@@ -29146,7 +29155,7 @@
         <v>11</v>
       </c>
       <c r="H1001" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="1002" spans="1:9" x14ac:dyDescent="0.3">
@@ -29175,7 +29184,7 @@
         <v>5</v>
       </c>
       <c r="I1002" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="1003" spans="1:9" x14ac:dyDescent="0.3">
@@ -29253,10 +29262,10 @@
         <v>11</v>
       </c>
       <c r="H1005" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I1005" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="1006" spans="1:9" x14ac:dyDescent="0.3">
@@ -29360,10 +29369,10 @@
         <v>3</v>
       </c>
       <c r="H1009" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I1009" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="1010" spans="1:9" x14ac:dyDescent="0.3">
@@ -29493,7 +29502,7 @@
         <v>11</v>
       </c>
       <c r="H1014" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="1015" spans="1:9" x14ac:dyDescent="0.3">
@@ -29935,7 +29944,7 @@
         <v>11</v>
       </c>
       <c r="H1031" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="1032" spans="1:8" x14ac:dyDescent="0.3">
@@ -30065,7 +30074,7 @@
         <v>5</v>
       </c>
       <c r="H1036" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="1037" spans="1:8" x14ac:dyDescent="0.3">
@@ -30221,7 +30230,7 @@
         <v>11</v>
       </c>
       <c r="H1042" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="1043" spans="1:8" x14ac:dyDescent="0.3">
@@ -30403,7 +30412,7 @@
         <v>3</v>
       </c>
       <c r="H1049" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="1050" spans="1:8" x14ac:dyDescent="0.3">
@@ -30481,7 +30490,7 @@
         <v>11</v>
       </c>
       <c r="H1052" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="1053" spans="1:8" x14ac:dyDescent="0.3">
@@ -30611,7 +30620,7 @@
         <v>5</v>
       </c>
       <c r="H1057" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="1058" spans="1:9" x14ac:dyDescent="0.3">
@@ -30637,10 +30646,10 @@
         <v>11</v>
       </c>
       <c r="H1058" t="s">
+        <v>596</v>
+      </c>
+      <c r="I1058" t="s">
         <v>597</v>
-      </c>
-      <c r="I1058" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="1059" spans="1:9" x14ac:dyDescent="0.3">
@@ -30770,7 +30779,7 @@
         <v>3</v>
       </c>
       <c r="H1063" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="1064" spans="1:9" x14ac:dyDescent="0.3">
@@ -30848,7 +30857,7 @@
         <v>11</v>
       </c>
       <c r="H1066" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="1067" spans="1:9" x14ac:dyDescent="0.3">
@@ -31535,7 +31544,7 @@
         <v>155</v>
       </c>
       <c r="C1093" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D1093">
         <v>128.0325</v>
@@ -31550,7 +31559,7 @@
         <v>5</v>
       </c>
       <c r="H1093" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
   </sheetData>

</xml_diff>